<commit_message>
update version num in xml files
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="705">
   <si>
     <t>Variable Name</t>
   </si>
@@ -38,7 +38,7 @@
     <t>PANORAMA_TYPE</t>
   </si>
   <si>
-    <t>static</t>
+    <t>cloud</t>
   </si>
   <si>
     <t>Panorama management IP type - static or cloud (for dhcp)</t>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>MGMT_TYPE</t>
+  </si>
+  <si>
+    <t>dhcp-client</t>
   </si>
   <si>
     <t>firewall management IP type (static or dhcp-client)</t>
@@ -3222,197 +3225,197 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -3430,32 +3433,32 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -3508,12 +3511,12 @@
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -3530,82 +3533,82 @@
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:1">
@@ -3616,57 +3619,57 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:1">
@@ -3689,27 +3692,27 @@
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:1">
@@ -3720,192 +3723,192 @@
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="95" spans="1:1">
@@ -3922,557 +3925,557 @@
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="208" spans="1:1">
@@ -4489,62 +4492,62 @@
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="222" spans="1:1">
@@ -4561,62 +4564,62 @@
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="236" spans="1:1">
@@ -4633,62 +4636,62 @@
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="250" spans="1:1">
@@ -4705,42 +4708,42 @@
     </row>
     <row r="252" spans="1:1">
       <c r="A252" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="260" spans="1:1">
@@ -4757,1427 +4760,1427 @@
     </row>
     <row r="262" spans="1:1">
       <c r="A262" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="391" spans="1:1">
       <c r="A391" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="421" spans="1:1">
       <c r="A421" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="529" spans="1:1">
       <c r="A529" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="547" spans="1:1">
@@ -6206,222 +6209,222 @@
     </row>
     <row r="551" spans="1:1">
       <c r="A551" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="595" spans="1:1">
@@ -6444,17 +6447,17 @@
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="601" spans="1:1">
@@ -6465,72 +6468,72 @@
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="615" spans="1:1">
       <c r="A615" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="616" spans="1:1">
@@ -6559,12 +6562,12 @@
     </row>
     <row r="620" spans="1:1">
       <c r="A620" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="621" spans="1:1">
       <c r="A621" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="622" spans="1:1">
@@ -6575,12 +6578,12 @@
     </row>
     <row r="623" spans="1:1">
       <c r="A623" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="624" spans="1:1">
       <c r="A624" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="625" spans="1:1">
@@ -6609,12 +6612,12 @@
     </row>
     <row r="629" spans="1:1">
       <c r="A629" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="630" spans="1:1">
       <c r="A630" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="631" spans="1:1">
@@ -6643,7 +6646,7 @@
     </row>
     <row r="635" spans="1:1">
       <c r="A635" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="636" spans="1:1">
@@ -7140,262 +7143,262 @@
     </row>
     <row r="718" spans="1:1">
       <c r="A718" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="719" spans="1:1">
       <c r="A719" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="720" spans="1:1">
       <c r="A720" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="721" spans="1:1">
       <c r="A721" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="766" spans="1:1">
       <c r="A766" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="767" spans="1:1">
       <c r="A767" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="768" spans="1:1">
       <c r="A768" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="769" spans="1:1">
       <c r="A769" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first push for 9.0
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="703">
   <si>
     <t>Variable Name</t>
   </si>
@@ -47,7 +47,7 @@
     <t>PANORAMA_IP</t>
   </si>
   <si>
-    <t>192.168.55.7</t>
+    <t>192.168.55.6</t>
   </si>
   <si>
     <t>Panorama IP</t>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>IP address for scheduled config exports</t>
+  </si>
+  <si>
+    <t>TEMPLATE</t>
+  </si>
+  <si>
+    <t>sample_template</t>
+  </si>
+  <si>
+    <t>Template name for Panorama</t>
   </si>
   <si>
     <t>STACK</t>
@@ -2455,7 +2464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2657,18 +2666,18 @@
         <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
         <v>55</v>
@@ -2766,11 +2775,22 @@
       <c r="A28" t="s">
         <v>80</v>
       </c>
-      <c r="B28" t="b">
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" t="b">
         <v>1</v>
       </c>
-      <c r="C28" t="s">
-        <v>81</v>
+      <c r="C29" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2788,27 +2808,27 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -2837,118 +2857,118 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <f>SUBSTITUTE("set deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B19)</f>
+        <f>SUBSTITUTE("set deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <f>SUBSTITUTE("set deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B20)</f>
+        <f>SUBSTITUTE("set deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
-        <f>SUBSTITUTE("set deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
+        <f>SUBSTITUTE("set deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
-        <f>SUBSTITUTE("set deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
+        <f>SUBSTITUTE("set deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} password", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} password", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
-        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:1">
@@ -2959,3689 +2979,3689 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B24)</f>
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B26)</f>
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56">
-        <f>SUBSTITUTE("set panorama log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B27)</f>
+        <f>SUBSTITUTE("set panorama log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95">
-        <f>SUBSTITUTE("set shared address Sinkhole-IPv4 ip-netmask {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set shared address Sinkhole-IPv4 ip-netmask {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96">
-        <f>SUBSTITUTE("set shared address Sinkhole-IPv6 ip-netmask {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared address Sinkhole-IPv6 ip-netmask {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208">
-        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209">
-        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="252" spans="1:1">
       <c r="A252" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260">
-        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261">
-        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
     </row>
     <row r="391" spans="1:1">
       <c r="A391" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
     </row>
     <row r="421" spans="1:1">
       <c r="A421" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
     </row>
     <row r="529" spans="1:1">
       <c r="A529" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B19)</f>
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="548" spans="1:1">
       <c r="A548">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B20)</f>
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="549" spans="1:1">
       <c r="A549">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="550" spans="1:1">
       <c r="A550">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="551" spans="1:1">
       <c r="A551" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B24)</f>
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B26)</f>
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B27)</f>
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
         <v>0</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
     </row>
     <row r="615" spans="1:1">
       <c r="A615" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="617" spans="1:1">
       <c r="A617">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="618" spans="1:1">
       <c r="A618">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B10), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B11), "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="620" spans="1:1">
       <c r="A620" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
     </row>
     <row r="621" spans="1:1">
       <c r="A621">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="622" spans="1:1">
       <c r="A622">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="623" spans="1:1">
       <c r="A623">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="624" spans="1:1">
       <c r="A624">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
     </row>
     <row r="627" spans="1:1">
       <c r="A627">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="628" spans="1:1">
       <c r="A628">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B12), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B13), "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="629" spans="1:1">
       <c r="A629">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B13), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B14), "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="630" spans="1:1">
       <c r="A630">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B14), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B15), "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="632" spans="1:1">
       <c r="A632">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="633" spans="1:1">
       <c r="A633">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="634" spans="1:1">
       <c r="A634">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="635" spans="1:1">
       <c r="A635">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="636" spans="1:1">
       <c r="A636">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="637" spans="1:1">
       <c r="A637">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="638" spans="1:1">
       <c r="A638">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="641" spans="1:1">
       <c r="A641">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="642" spans="1:1">
       <c r="A642">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="643" spans="1:1">
       <c r="A643">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="647" spans="1:1">
       <c r="A647">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="648" spans="1:1">
       <c r="A648">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="649" spans="1:1">
       <c r="A649">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="654" spans="1:1">
       <c r="A654">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="659" spans="1:1">
       <c r="A659">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="664" spans="1:1">
       <c r="A664">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="665" spans="1:1">
       <c r="A665">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="670" spans="1:1">
       <c r="A670">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="672" spans="1:1">
       <c r="A672">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="673" spans="1:1">
       <c r="A673">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="675" spans="1:1">
       <c r="A675">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="676" spans="1:1">
       <c r="A676">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="677" spans="1:1">
       <c r="A677">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="678" spans="1:1">
       <c r="A678">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="679" spans="1:1">
       <c r="A679">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="680" spans="1:1">
       <c r="A680">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="681" spans="1:1">
       <c r="A681">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="682" spans="1:1">
       <c r="A682">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="683" spans="1:1">
       <c r="A683">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="684" spans="1:1">
       <c r="A684">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="685" spans="1:1">
       <c r="A685">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="686" spans="1:1">
       <c r="A686">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="687" spans="1:1">
       <c r="A687">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="688" spans="1:1">
       <c r="A688">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="689" spans="1:1">
       <c r="A689">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="690" spans="1:1">
       <c r="A690">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="691" spans="1:1">
       <c r="A691">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="692" spans="1:1">
       <c r="A692">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="693" spans="1:1">
       <c r="A693">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="694" spans="1:1">
       <c r="A694">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="695" spans="1:1">
       <c r="A695">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="696" spans="1:1">
       <c r="A696">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="697" spans="1:1">
       <c r="A697">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="698" spans="1:1">
       <c r="A698">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="699" spans="1:1">
       <c r="A699">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="700" spans="1:1">
       <c r="A700">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="701" spans="1:1">
       <c r="A701">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="702" spans="1:1">
       <c r="A702">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="703" spans="1:1">
       <c r="A703">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="704" spans="1:1">
       <c r="A704">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="705" spans="1:1">
       <c r="A705">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="706" spans="1:1">
       <c r="A706">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="707" spans="1:1">
       <c r="A707">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="708" spans="1:1">
       <c r="A708">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="709" spans="1:1">
       <c r="A709">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="710" spans="1:1">
       <c r="A710">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="711" spans="1:1">
       <c r="A711">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="712" spans="1:1">
       <c r="A712">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="713" spans="1:1">
       <c r="A713">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" email-profile Sample_Email_Profile", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" email-profile Sample_Email_Profile", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="715" spans="1:1">
       <c r="A715" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
     </row>
     <row r="716" spans="1:1">
       <c r="A716" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
     </row>
     <row r="717" spans="1:1">
       <c r="A717" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
     </row>
     <row r="718" spans="1:1">
       <c r="A718" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
     </row>
     <row r="719" spans="1:1">
       <c r="A719" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
     </row>
     <row r="720" spans="1:1">
       <c r="A720" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
     </row>
     <row r="721" spans="1:1">
       <c r="A721" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated configs with max csv log value
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="704">
   <si>
     <t>Variable Name</t>
   </si>
@@ -38,7 +38,7 @@
     <t>PANORAMA_TYPE</t>
   </si>
   <si>
-    <t>cloud</t>
+    <t>static</t>
   </si>
   <si>
     <t>Panorama management IP type - static or cloud (for dhcp)</t>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>ADMINISTRATOR_PASSWORD</t>
+  </si>
+  <si>
+    <t>paloalto</t>
   </si>
   <si>
     <t>admin password</t>
@@ -2677,120 +2680,120 @@
         <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2808,27 +2811,27 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -2881,7 +2884,7 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -2898,77 +2901,77 @@
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:1">
@@ -2979,52 +2982,52 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:1">
@@ -3047,27 +3050,27 @@
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:1">
@@ -3078,177 +3081,177 @@
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="95" spans="1:1">
@@ -3265,542 +3268,542 @@
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="208" spans="1:1">
@@ -3817,62 +3820,62 @@
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="222" spans="1:1">
@@ -3889,62 +3892,62 @@
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="236" spans="1:1">
@@ -3961,62 +3964,62 @@
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="250" spans="1:1">
@@ -4033,42 +4036,42 @@
     </row>
     <row r="252" spans="1:1">
       <c r="A252" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="260" spans="1:1">
@@ -4085,1412 +4088,1412 @@
     </row>
     <row r="262" spans="1:1">
       <c r="A262" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="391" spans="1:1">
       <c r="A391" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="421" spans="1:1">
       <c r="A421" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="529" spans="1:1">
       <c r="A529" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="547" spans="1:1">
@@ -5519,222 +5522,222 @@
     </row>
     <row r="551" spans="1:1">
       <c r="A551" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="595" spans="1:1">
@@ -5757,17 +5760,17 @@
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="601" spans="1:1">
@@ -5778,67 +5781,67 @@
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="615" spans="1:1">
       <c r="A615" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="616" spans="1:1">
@@ -5861,7 +5864,7 @@
     </row>
     <row r="620" spans="1:1">
       <c r="A620" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="621" spans="1:1">
@@ -5890,7 +5893,7 @@
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="627" spans="1:1">
@@ -6411,257 +6414,257 @@
     </row>
     <row r="715" spans="1:1">
       <c r="A715" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="716" spans="1:1">
       <c r="A716" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="717" spans="1:1">
       <c r="A717" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="718" spans="1:1">
       <c r="A718" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="719" spans="1:1">
       <c r="A719" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="720" spans="1:1">
       <c r="A720" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="721" spans="1:1">
       <c r="A721" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added vm50 downsize instructions and max csv export rows
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="705">
   <si>
     <t>Variable Name</t>
   </si>
@@ -47,7 +47,7 @@
     <t>PANORAMA_IP</t>
   </si>
   <si>
-    <t>192.168.55.7</t>
+    <t>192.168.55.8</t>
   </si>
   <si>
     <t>Panorama IP</t>
@@ -80,6 +80,15 @@
     <t>IP address for scheduled config exports</t>
   </si>
   <si>
+    <t>TEMPLATE</t>
+  </si>
+  <si>
+    <t>sample_template</t>
+  </si>
+  <si>
+    <t>Template name for Panorama</t>
+  </si>
+  <si>
     <t>STACK</t>
   </si>
   <si>
@@ -350,6 +359,9 @@
     <t>set deviceconfig setting management share-unused-objects-with-devices no</t>
   </si>
   <si>
+    <t>set deviceconfig setting management max-rows-in-csv-export 1048576</t>
+  </si>
+  <si>
     <t># Panorama log settings</t>
   </si>
   <si>
@@ -1800,6 +1812,9 @@
   </si>
   <si>
     <t>set template iron-skillet config deviceconfig setting management enable-log-high-dp-load yes</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig setting management max-rows-in-csv-export 1048576</t>
   </si>
   <si>
     <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit pe size-limit 10</t>
@@ -2455,7 +2470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2657,18 +2672,18 @@
         <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
         <v>55</v>
@@ -2766,11 +2781,22 @@
       <c r="A28" t="s">
         <v>80</v>
       </c>
-      <c r="B28" t="b">
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" t="b">
         <v>1</v>
       </c>
-      <c r="C28" t="s">
-        <v>81</v>
+      <c r="C29" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2780,7 +2806,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A765"/>
+  <dimension ref="A2:A767"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2788,27 +2814,27 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -2837,118 +2863,118 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <f>SUBSTITUTE("set deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B19)</f>
+        <f>SUBSTITUTE("set deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <f>SUBSTITUTE("set deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B20)</f>
+        <f>SUBSTITUTE("set deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
-        <f>SUBSTITUTE("set deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
+        <f>SUBSTITUTE("set deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
-        <f>SUBSTITUTE("set deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
+        <f>SUBSTITUTE("set deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} password", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} password", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
-        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:1">
@@ -2959,3689 +2985,3699 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
-        <v>111</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B24)</f>
-        <v>0</v>
+      <c r="A48" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B26)</f>
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" t="s">
-        <v>113</v>
+      <c r="A51">
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56">
-        <f>SUBSTITUTE("set panorama log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B27)</f>
-        <v>0</v>
+      <c r="A56" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" t="s">
-        <v>118</v>
+      <c r="A57">
+        <f>SUBSTITUTE("set panorama log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" t="s">
-        <v>148</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95">
-        <f>SUBSTITUTE("set shared address Sinkhole-IPv4 ip-netmask {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A95" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96">
-        <f>SUBSTITUTE("set shared address Sinkhole-IPv6 ip-netmask {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared address Sinkhole-IPv4 ip-netmask {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" t="s">
-        <v>153</v>
+      <c r="A97">
+        <f>SUBSTITUTE("set shared address Sinkhole-IPv6 ip-netmask {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1">
-      <c r="A104" t="s">
-        <v>159</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1">
-      <c r="A127" t="s">
-        <v>181</v>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1">
-      <c r="A146" t="s">
-        <v>199</v>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="208" spans="1:1">
-      <c r="A208">
-        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A208" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209">
-        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="210" spans="1:1">
-      <c r="A210" t="s">
-        <v>261</v>
+      <c r="A210">
+        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="222" spans="1:1">
-      <c r="A222">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A222" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:1">
-      <c r="A224" t="s">
-        <v>273</v>
+      <c r="A224">
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="236" spans="1:1">
-      <c r="A236">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A236" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="238" spans="1:1">
-      <c r="A238" t="s">
-        <v>285</v>
+      <c r="A238">
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="250" spans="1:1">
-      <c r="A250">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A250" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="252" spans="1:1">
-      <c r="A252" t="s">
-        <v>297</v>
+      <c r="A252">
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="260" spans="1:1">
-      <c r="A260">
-        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A260" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261">
-        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="262" spans="1:1">
-      <c r="A262" t="s">
-        <v>305</v>
+      <c r="A262">
+        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="391" spans="1:1">
-      <c r="A391" t="s">
-        <v>433</v>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1">
+      <c r="A390" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="421" spans="1:1">
-      <c r="A421" t="s">
-        <v>462</v>
+        <v>464</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1">
+      <c r="A420" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="529" spans="1:1">
-      <c r="A529" t="s">
-        <v>569</v>
+        <v>571</v>
+      </c>
+    </row>
+    <row r="528" spans="1:1">
+      <c r="A528" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
     </row>
     <row r="547" spans="1:1">
-      <c r="A547">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B19)</f>
-        <v>0</v>
+      <c r="A547" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="548" spans="1:1">
       <c r="A548">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B20)</f>
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="549" spans="1:1">
       <c r="A549">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="550" spans="1:1">
       <c r="A550">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="551" spans="1:1">
-      <c r="A551" t="s">
-        <v>587</v>
+      <c r="A551">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B17)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
     </row>
     <row r="595" spans="1:1">
-      <c r="A595">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B24)</f>
-        <v>0</v>
+      <c r="A595" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="596" spans="1:1">
-      <c r="A596">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B25)</f>
-        <v>0</v>
+      <c r="A596" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B26)</f>
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="598" spans="1:1">
-      <c r="A598" t="s">
-        <v>631</v>
+      <c r="A598">
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="599" spans="1:1">
-      <c r="A599" t="s">
-        <v>632</v>
+      <c r="A599">
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
     </row>
     <row r="601" spans="1:1">
-      <c r="A601">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B27)</f>
-        <v>0</v>
+      <c r="A601" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
     </row>
     <row r="603" spans="1:1">
-      <c r="A603" t="s">
-        <v>635</v>
+      <c r="A603">
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>644</v>
+        <v>647</v>
+      </c>
+    </row>
+    <row r="613" spans="1:1">
+      <c r="A613" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="615" spans="1:1">
-      <c r="A615" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
     </row>
     <row r="616" spans="1:1">
-      <c r="A616">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A616" t="s">
+        <v>650</v>
       </c>
     </row>
     <row r="617" spans="1:1">
-      <c r="A617">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A617" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="618" spans="1:1">
       <c r="A618">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B10), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="619" spans="1:1">
+      <c r="A619">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="620" spans="1:1">
-      <c r="A620" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="621" spans="1:1">
-      <c r="A621">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B8)</f>
+      <c r="A620">
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B11), "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="622" spans="1:1">
-      <c r="A622">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A622" t="s">
+        <v>652</v>
       </c>
     </row>
     <row r="623" spans="1:1">
       <c r="A623">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="624" spans="1:1">
       <c r="A624">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="625" spans="1:1">
+      <c r="A625">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="626" spans="1:1">
-      <c r="A626" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="627" spans="1:1">
-      <c r="A627">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B8)</f>
+      <c r="A626">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="628" spans="1:1">
-      <c r="A628">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B12), "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A628" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="629" spans="1:1">
       <c r="A629">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B13), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="630" spans="1:1">
       <c r="A630">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B14), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B13), "{{ STACK }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="631" spans="1:1">
+      <c r="A631">
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B14), "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="632" spans="1:1">
       <c r="A632">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="633" spans="1:1">
-      <c r="A633">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B15), "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="634" spans="1:1">
       <c r="A634">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="635" spans="1:1">
       <c r="A635">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="636" spans="1:1">
       <c r="A636">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="637" spans="1:1">
       <c r="A637">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="638" spans="1:1">
       <c r="A638">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="641" spans="1:1">
       <c r="A641">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="642" spans="1:1">
       <c r="A642">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="643" spans="1:1">
       <c r="A643">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="647" spans="1:1">
       <c r="A647">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="648" spans="1:1">
       <c r="A648">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="649" spans="1:1">
       <c r="A649">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="654" spans="1:1">
       <c r="A654">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="659" spans="1:1">
       <c r="A659">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="664" spans="1:1">
       <c r="A664">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="665" spans="1:1">
       <c r="A665">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="670" spans="1:1">
       <c r="A670">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="672" spans="1:1">
       <c r="A672">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="673" spans="1:1">
       <c r="A673">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="675" spans="1:1">
       <c r="A675">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="676" spans="1:1">
       <c r="A676">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="677" spans="1:1">
       <c r="A677">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="678" spans="1:1">
       <c r="A678">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="679" spans="1:1">
       <c r="A679">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="680" spans="1:1">
       <c r="A680">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="681" spans="1:1">
       <c r="A681">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="682" spans="1:1">
       <c r="A682">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="683" spans="1:1">
       <c r="A683">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="684" spans="1:1">
       <c r="A684">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="685" spans="1:1">
       <c r="A685">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="686" spans="1:1">
       <c r="A686">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="687" spans="1:1">
       <c r="A687">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="688" spans="1:1">
       <c r="A688">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="689" spans="1:1">
       <c r="A689">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="690" spans="1:1">
       <c r="A690">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="691" spans="1:1">
       <c r="A691">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="692" spans="1:1">
       <c r="A692">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="693" spans="1:1">
       <c r="A693">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="694" spans="1:1">
       <c r="A694">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="695" spans="1:1">
       <c r="A695">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="696" spans="1:1">
       <c r="A696">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="697" spans="1:1">
       <c r="A697">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="698" spans="1:1">
       <c r="A698">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="699" spans="1:1">
       <c r="A699">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="700" spans="1:1">
       <c r="A700">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="701" spans="1:1">
       <c r="A701">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="702" spans="1:1">
       <c r="A702">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="703" spans="1:1">
       <c r="A703">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="704" spans="1:1">
       <c r="A704">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="705" spans="1:1">
       <c r="A705">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="706" spans="1:1">
       <c r="A706">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="707" spans="1:1">
       <c r="A707">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="708" spans="1:1">
       <c r="A708">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="709" spans="1:1">
       <c r="A709">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="710" spans="1:1">
       <c r="A710">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="711" spans="1:1">
       <c r="A711">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="712" spans="1:1">
       <c r="A712">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="713" spans="1:1">
       <c r="A713">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" email-profile Sample_Email_Profile", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="714" spans="1:1">
+      <c r="A714">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="715" spans="1:1">
-      <c r="A715" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="716" spans="1:1">
-      <c r="A716" t="s">
-        <v>650</v>
+      <c r="A715">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" email-profile Sample_Email_Profile", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="717" spans="1:1">
       <c r="A717" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
     </row>
     <row r="718" spans="1:1">
       <c r="A718" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
     </row>
     <row r="719" spans="1:1">
       <c r="A719" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
     </row>
     <row r="720" spans="1:1">
       <c r="A720" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
     </row>
     <row r="721" spans="1:1">
       <c r="A721" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765" t="s">
-        <v>699</v>
+        <v>702</v>
+      </c>
+    </row>
+    <row r="766" spans="1:1">
+      <c r="A766" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="767" spans="1:1">
+      <c r="A767" t="s">
+        <v>704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to vm50 docs and adding max csv export
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="706">
   <si>
     <t>Variable Name</t>
   </si>
@@ -359,6 +359,9 @@
     <t>set deviceconfig setting management share-unused-objects-with-devices no</t>
   </si>
   <si>
+    <t>set deviceconfig setting management max-rows-in-csv-export 1048576</t>
+  </si>
+  <si>
     <t># Panorama log settings</t>
   </si>
   <si>
@@ -1809,6 +1812,9 @@
   </si>
   <si>
     <t>set template iron-skillet config deviceconfig setting management enable-log-high-dp-load yes</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig setting management max-rows-in-csv-export 1048576</t>
   </si>
   <si>
     <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit pe size-limit 10</t>
@@ -2803,7 +2809,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A769"/>
+  <dimension ref="A2:A771"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3020,8 +3026,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
         <v>114</v>
       </c>
     </row>
@@ -3031,26 +3037,26 @@
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
-        <v>0</v>
+      <c r="A48" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50">
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51">
         <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:1">
@@ -3074,14 +3080,14 @@
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56">
+      <c r="A56" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57">
         <f>SUBSTITUTE("set panorama log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:1">
@@ -3224,13 +3230,13 @@
         <v>149</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
-      <c r="A88" t="s">
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
-      <c r="A90" t="s">
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
         <v>151</v>
       </c>
     </row>
@@ -3255,20 +3261,20 @@
       </c>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95">
-        <f>SUBSTITUTE("set shared address Sinkhole-IPv4 ip-netmask {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
+      <c r="A95" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96">
+        <f>SUBSTITUTE("set shared address Sinkhole-IPv4 ip-netmask {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97">
         <f>SUBSTITUTE("set shared address Sinkhole-IPv6 ip-netmask {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1">
-      <c r="A97" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="98" spans="1:1">
@@ -3296,8 +3302,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
-      <c r="A104" t="s">
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
         <v>162</v>
       </c>
     </row>
@@ -3406,8 +3412,8 @@
         <v>183</v>
       </c>
     </row>
-    <row r="127" spans="1:1">
-      <c r="A127" t="s">
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
         <v>184</v>
       </c>
     </row>
@@ -3496,8 +3502,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="146" spans="1:1">
-      <c r="A146" t="s">
+    <row r="145" spans="1:1">
+      <c r="A145" t="s">
         <v>202</v>
       </c>
     </row>
@@ -3807,20 +3813,20 @@
       </c>
     </row>
     <row r="208" spans="1:1">
-      <c r="A208">
-        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
+      <c r="A208" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209">
+        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210">
         <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="210" spans="1:1">
-      <c r="A210" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="211" spans="1:1">
@@ -3879,20 +3885,20 @@
       </c>
     </row>
     <row r="222" spans="1:1">
-      <c r="A222">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
+      <c r="A222" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223">
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224">
         <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="224" spans="1:1">
-      <c r="A224" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="225" spans="1:1">
@@ -3951,20 +3957,20 @@
       </c>
     </row>
     <row r="236" spans="1:1">
-      <c r="A236">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
+      <c r="A236" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237">
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238">
         <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="238" spans="1:1">
-      <c r="A238" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="239" spans="1:1">
@@ -4023,20 +4029,20 @@
       </c>
     </row>
     <row r="250" spans="1:1">
-      <c r="A250">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
+      <c r="A250" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251">
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1">
+      <c r="A252">
         <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="252" spans="1:1">
-      <c r="A252" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="253" spans="1:1">
@@ -4075,20 +4081,20 @@
       </c>
     </row>
     <row r="260" spans="1:1">
-      <c r="A260">
-        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
+      <c r="A260" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261">
+        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1">
+      <c r="A262">
         <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="262" spans="1:1">
-      <c r="A262" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="263" spans="1:1">
@@ -4726,8 +4732,8 @@
         <v>435</v>
       </c>
     </row>
-    <row r="391" spans="1:1">
-      <c r="A391" t="s">
+    <row r="390" spans="1:1">
+      <c r="A390" t="s">
         <v>436</v>
       </c>
     </row>
@@ -4871,8 +4877,8 @@
         <v>464</v>
       </c>
     </row>
-    <row r="421" spans="1:1">
-      <c r="A421" t="s">
+    <row r="420" spans="1:1">
+      <c r="A420" t="s">
         <v>465</v>
       </c>
     </row>
@@ -5406,8 +5412,8 @@
         <v>571</v>
       </c>
     </row>
-    <row r="529" spans="1:1">
-      <c r="A529" t="s">
+    <row r="528" spans="1:1">
+      <c r="A528" t="s">
         <v>572</v>
       </c>
     </row>
@@ -5497,32 +5503,32 @@
       </c>
     </row>
     <row r="547" spans="1:1">
-      <c r="A547">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A547" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="548" spans="1:1">
       <c r="A548">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="549" spans="1:1">
       <c r="A549">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B16)</f>
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="550" spans="1:1">
       <c r="A550">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="551" spans="1:1">
+      <c r="A551">
         <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B17)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="551" spans="1:1">
-      <c r="A551" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="552" spans="1:1">
@@ -5741,31 +5747,31 @@
       </c>
     </row>
     <row r="595" spans="1:1">
-      <c r="A595">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
-        <v>0</v>
+      <c r="A595" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="596" spans="1:1">
-      <c r="A596">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
-        <v>0</v>
+      <c r="A596" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597">
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="598" spans="1:1">
+      <c r="A598">
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="599" spans="1:1">
+      <c r="A599">
         <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="598" spans="1:1">
-      <c r="A598" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="599" spans="1:1">
-      <c r="A599" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="600" spans="1:1">
@@ -5774,19 +5780,19 @@
       </c>
     </row>
     <row r="601" spans="1:1">
-      <c r="A601">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
-        <v>0</v>
+      <c r="A601" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="603" spans="1:1">
-      <c r="A603" t="s">
-        <v>638</v>
+      <c r="A603">
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="604" spans="1:1">
@@ -5834,609 +5840,609 @@
         <v>647</v>
       </c>
     </row>
+    <row r="613" spans="1:1">
+      <c r="A613" t="s">
+        <v>648</v>
+      </c>
+    </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="615" spans="1:1">
-      <c r="A615" t="s">
         <v>649</v>
       </c>
     </row>
     <row r="616" spans="1:1">
-      <c r="A616">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A616" t="s">
+        <v>650</v>
       </c>
     </row>
     <row r="617" spans="1:1">
-      <c r="A617">
-        <f>SUBSTITUTE("set template {{ TEMPLATE }} settings default-vsys vsys1", "{{ TEMPLATE }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A617" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="618" spans="1:1">
       <c r="A618">
-        <f>SUBSTITUTE("set template {{ TEMPLATE }} config vsys vsys1", "{{ TEMPLATE }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="619" spans="1:1">
       <c r="A619">
+        <f>SUBSTITUTE("set template {{ TEMPLATE }} settings default-vsys vsys1", "{{ TEMPLATE }}", 'values'!B8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="620" spans="1:1">
+      <c r="A620">
+        <f>SUBSTITUTE("set template {{ TEMPLATE }} config vsys vsys1", "{{ TEMPLATE }}", 'values'!B8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="621" spans="1:1">
+      <c r="A621">
         <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} templates {{ TEMPLATE }}", "{{ STACK }}", 'values'!B9), "{{ TEMPLATE }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="621" spans="1:1">
-      <c r="A621" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="622" spans="1:1">
-      <c r="A622">
+    <row r="623" spans="1:1">
+      <c r="A623" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="624" spans="1:1">
+      <c r="A624">
         <f>SUBSTITUTE(SUBSTITUTE("set template {{ TEMPLATE }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B11), "{{ TEMPLATE }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="624" spans="1:1">
-      <c r="A624" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="625" spans="1:1">
-      <c r="A625">
-        <f>SUBSTITUTE("set template {{ TEMPLATE }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ TEMPLATE }}", 'values'!B8)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="626" spans="1:1">
-      <c r="A626">
-        <f>SUBSTITUTE("set template {{ TEMPLATE }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ TEMPLATE }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A626" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="627" spans="1:1">
       <c r="A627">
-        <f>SUBSTITUTE("set template {{ TEMPLATE }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ TEMPLATE }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template {{ TEMPLATE }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ TEMPLATE }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="628" spans="1:1">
       <c r="A628">
+        <f>SUBSTITUTE("set template {{ TEMPLATE }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ TEMPLATE }}", 'values'!B8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="629" spans="1:1">
+      <c r="A629">
+        <f>SUBSTITUTE("set template {{ TEMPLATE }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ TEMPLATE }}", 'values'!B8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="630" spans="1:1">
+      <c r="A630">
         <f>SUBSTITUTE("set template {{ TEMPLATE }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ TEMPLATE }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="630" spans="1:1">
-      <c r="A630" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="631" spans="1:1">
-      <c r="A631">
-        <f>SUBSTITUTE("set template {{ TEMPLATE }} config devices localhost.localdomain deviceconfig system type static", "{{ TEMPLATE }}", 'values'!B8)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="632" spans="1:1">
-      <c r="A632">
-        <f>SUBSTITUTE(SUBSTITUTE("set template {{ TEMPLATE }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B13), "{{ TEMPLATE }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A632" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="633" spans="1:1">
       <c r="A633">
-        <f>SUBSTITUTE(SUBSTITUTE("set template {{ TEMPLATE }}} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B14), "{{ TEMPLATE }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template {{ TEMPLATE }} config devices localhost.localdomain deviceconfig system type static", "{{ TEMPLATE }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="634" spans="1:1">
       <c r="A634">
-        <f>SUBSTITUTE(SUBSTITUTE("set template {{ TEMPLATE }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B15), "{{ TEMPLATE }}", 'values'!B8)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template {{ TEMPLATE }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B13), "{{ TEMPLATE }}", 'values'!B8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="635" spans="1:1">
+      <c r="A635">
+        <f>SUBSTITUTE(SUBSTITUTE("set template {{ TEMPLATE }}} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B14), "{{ TEMPLATE }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="636" spans="1:1">
       <c r="A636">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="637" spans="1:1">
-      <c r="A637">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template {{ TEMPLATE }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B15), "{{ TEMPLATE }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="638" spans="1:1">
       <c r="A638">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="641" spans="1:1">
       <c r="A641">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="642" spans="1:1">
       <c r="A642">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="643" spans="1:1">
       <c r="A643">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="647" spans="1:1">
       <c r="A647">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="648" spans="1:1">
       <c r="A648">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="649" spans="1:1">
       <c r="A649">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="654" spans="1:1">
       <c r="A654">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="659" spans="1:1">
       <c r="A659">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="664" spans="1:1">
       <c r="A664">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="665" spans="1:1">
       <c r="A665">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="670" spans="1:1">
       <c r="A670">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="672" spans="1:1">
       <c r="A672">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="673" spans="1:1">
       <c r="A673">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="675" spans="1:1">
       <c r="A675">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="676" spans="1:1">
       <c r="A676">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="677" spans="1:1">
       <c r="A677">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="678" spans="1:1">
       <c r="A678">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="679" spans="1:1">
       <c r="A679">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="680" spans="1:1">
       <c r="A680">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="681" spans="1:1">
       <c r="A681">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="682" spans="1:1">
       <c r="A682">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="683" spans="1:1">
       <c r="A683">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="684" spans="1:1">
       <c r="A684">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="685" spans="1:1">
       <c r="A685">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="686" spans="1:1">
       <c r="A686">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="687" spans="1:1">
       <c r="A687">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="688" spans="1:1">
       <c r="A688">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="689" spans="1:1">
       <c r="A689">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="690" spans="1:1">
       <c r="A690">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="691" spans="1:1">
       <c r="A691">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="692" spans="1:1">
       <c r="A692">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="693" spans="1:1">
       <c r="A693">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="694" spans="1:1">
       <c r="A694">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="695" spans="1:1">
       <c r="A695">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="696" spans="1:1">
       <c r="A696">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="697" spans="1:1">
       <c r="A697">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="698" spans="1:1">
       <c r="A698">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="699" spans="1:1">
       <c r="A699">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="700" spans="1:1">
       <c r="A700">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="701" spans="1:1">
       <c r="A701">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="702" spans="1:1">
       <c r="A702">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="703" spans="1:1">
       <c r="A703">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="704" spans="1:1">
       <c r="A704">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="705" spans="1:1">
       <c r="A705">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="706" spans="1:1">
       <c r="A706">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="707" spans="1:1">
       <c r="A707">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="708" spans="1:1">
       <c r="A708">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="709" spans="1:1">
       <c r="A709">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="710" spans="1:1">
       <c r="A710">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="711" spans="1:1">
       <c r="A711">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="712" spans="1:1">
       <c r="A712">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="713" spans="1:1">
       <c r="A713">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="714" spans="1:1">
       <c r="A714">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="715" spans="1:1">
       <c r="A715">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="716" spans="1:1">
       <c r="A716">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="717" spans="1:1">
       <c r="A717">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="718" spans="1:1">
+      <c r="A718">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="719" spans="1:1">
+      <c r="A719">
         <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" email-profile Sample_Email_Profile", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="719" spans="1:1">
-      <c r="A719" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="720" spans="1:1">
-      <c r="A720" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="721" spans="1:1">
@@ -6682,6 +6688,16 @@
     <row r="769" spans="1:1">
       <c r="A769" t="s">
         <v>703</v>
+      </c>
+    </row>
+    <row r="770" spans="1:1">
+      <c r="A770" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="771" spans="1:1">
+      <c r="A771" t="s">
+        <v>705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update tag version and changes in template guide docs
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="704">
   <si>
     <t>Variable Name</t>
   </si>
@@ -38,7 +38,7 @@
     <t>PANORAMA_TYPE</t>
   </si>
   <si>
-    <t>cloud</t>
+    <t>static</t>
   </si>
   <si>
     <t>Panorama management IP type - static or cloud (for dhcp)</t>
@@ -119,9 +119,6 @@
     <t>MGMT_TYPE</t>
   </si>
   <si>
-    <t>dhcp-client</t>
-  </si>
-  <si>
     <t>firewall management IP type (static or dhcp-client)</t>
   </si>
   <si>
@@ -485,7 +482,7 @@
     <t>set shared tag Internal comments ""Internal to Internal""</t>
   </si>
   <si>
-    <t>set shared tag iron-skillet-version comments ""version 1.0.4: version of this iron-skillet template file""</t>
+    <t>set shared tag iron-skillet-version comments ""version 1.0.5: version of this iron-skillet template file""</t>
   </si>
   <si>
     <t>set shared external-list ""Team Cymru Bogons IPv4"" type ip recurring hourly</t>
@@ -2606,197 +2603,197 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>46</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
         <v>54</v>
-      </c>
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
         <v>56</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>57</v>
-      </c>
-      <c r="C20" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
         <v>59</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>60</v>
-      </c>
-      <c r="C21" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
         <v>62</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>63</v>
-      </c>
-      <c r="C22" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
         <v>65</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>66</v>
-      </c>
-      <c r="C23" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
         <v>68</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>69</v>
-      </c>
-      <c r="C24" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" t="s">
         <v>71</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>72</v>
-      </c>
-      <c r="C25" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
         <v>74</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>75</v>
-      </c>
-      <c r="C26" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
         <v>77</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>78</v>
-      </c>
-      <c r="C27" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
         <v>80</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>81</v>
-      </c>
-      <c r="C28" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2814,27 +2811,27 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -2887,7 +2884,7 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -2904,77 +2901,77 @@
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:1">
@@ -2985,57 +2982,57 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:1">
@@ -3058,27 +3055,27 @@
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:1">
@@ -3089,177 +3086,177 @@
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="96" spans="1:1">
@@ -3276,542 +3273,542 @@
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="209" spans="1:1">
@@ -3828,62 +3825,62 @@
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="223" spans="1:1">
@@ -3900,62 +3897,62 @@
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="237" spans="1:1">
@@ -3972,62 +3969,62 @@
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="251" spans="1:1">
@@ -4044,42 +4041,42 @@
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="261" spans="1:1">
@@ -4096,1412 +4093,1412 @@
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="548" spans="1:1">
@@ -5530,227 +5527,227 @@
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="597" spans="1:1">
@@ -5773,17 +5770,17 @@
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="603" spans="1:1">
@@ -5794,67 +5791,67 @@
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="617" spans="1:1">
       <c r="A617" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="618" spans="1:1">
@@ -5877,7 +5874,7 @@
     </row>
     <row r="622" spans="1:1">
       <c r="A622" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="623" spans="1:1">
@@ -5906,7 +5903,7 @@
     </row>
     <row r="628" spans="1:1">
       <c r="A628" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="629" spans="1:1">
@@ -6427,257 +6424,257 @@
     </row>
     <row r="717" spans="1:1">
       <c r="A717" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="718" spans="1:1">
       <c r="A718" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="719" spans="1:1">
       <c r="A719" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="720" spans="1:1">
       <c r="A720" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="721" spans="1:1">
       <c r="A721" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="766" spans="1:1">
       <c r="A766" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="767" spans="1:1">
       <c r="A767" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added max csv export to template guides
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="705">
   <si>
     <t>Variable Name</t>
   </si>
@@ -38,7 +38,7 @@
     <t>PANORAMA_TYPE</t>
   </si>
   <si>
-    <t>cloud</t>
+    <t>static</t>
   </si>
   <si>
     <t>Panorama management IP type - static or cloud (for dhcp)</t>
@@ -119,9 +119,6 @@
     <t>MGMT_TYPE</t>
   </si>
   <si>
-    <t>dhcp-client</t>
-  </si>
-  <si>
     <t>firewall management IP type (static or dhcp-client)</t>
   </si>
   <si>
@@ -485,7 +482,7 @@
     <t>set shared tag Internal comments ""Internal to Internal""</t>
   </si>
   <si>
-    <t>set shared tag iron-skillet-version comments ""version 1.0.4: version of this iron-skillet template file""</t>
+    <t>set shared tag iron-skillet-version comments ""version 1.0.5: version of this iron-skillet template file""</t>
   </si>
   <si>
     <t>set shared external-list ""Team Cymru Bogons IPv4"" type ip recurring hourly</t>
@@ -2609,197 +2606,197 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>46</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
         <v>54</v>
-      </c>
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
         <v>56</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>57</v>
-      </c>
-      <c r="C20" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
         <v>59</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>60</v>
-      </c>
-      <c r="C21" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
         <v>62</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>63</v>
-      </c>
-      <c r="C22" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
         <v>65</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>66</v>
-      </c>
-      <c r="C23" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
         <v>68</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>69</v>
-      </c>
-      <c r="C24" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" t="s">
         <v>71</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>72</v>
-      </c>
-      <c r="C25" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
         <v>74</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>75</v>
-      </c>
-      <c r="C26" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
         <v>77</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>78</v>
-      </c>
-      <c r="C27" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
         <v>80</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>81</v>
-      </c>
-      <c r="C28" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2817,27 +2814,27 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -2890,7 +2887,7 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -2907,77 +2904,77 @@
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:1">
@@ -2988,57 +2985,57 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:1">
@@ -3061,27 +3058,27 @@
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:1">
@@ -3092,177 +3089,177 @@
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="96" spans="1:1">
@@ -3279,542 +3276,542 @@
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="209" spans="1:1">
@@ -3831,62 +3828,62 @@
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="223" spans="1:1">
@@ -3903,62 +3900,62 @@
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="237" spans="1:1">
@@ -3975,62 +3972,62 @@
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="251" spans="1:1">
@@ -4047,42 +4044,42 @@
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="261" spans="1:1">
@@ -4099,1412 +4096,1412 @@
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="548" spans="1:1">
@@ -5533,227 +5530,227 @@
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="597" spans="1:1">
@@ -5776,17 +5773,17 @@
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="603" spans="1:1">
@@ -5797,67 +5794,67 @@
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="617" spans="1:1">
       <c r="A617" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="618" spans="1:1">
@@ -5886,7 +5883,7 @@
     </row>
     <row r="623" spans="1:1">
       <c r="A623" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="624" spans="1:1">
@@ -5897,7 +5894,7 @@
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="627" spans="1:1">
@@ -5926,7 +5923,7 @@
     </row>
     <row r="632" spans="1:1">
       <c r="A632" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="633" spans="1:1">
@@ -6447,257 +6444,257 @@
     </row>
     <row r="721" spans="1:1">
       <c r="A721" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="766" spans="1:1">
       <c r="A766" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="767" spans="1:1">
       <c r="A767" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="768" spans="1:1">
       <c r="A768" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="769" spans="1:1">
       <c r="A769" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="770" spans="1:1">
       <c r="A770" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="771" spans="1:1">
       <c r="A771" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edits to panorama set commands
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="724">
   <si>
     <t>Variable Name</t>
   </si>
@@ -278,7 +278,7 @@
     <t>include the predefined Palo Alto Networks external lists security rules</t>
   </si>
   <si>
-    <t># set command configuration for Panorama version 8.1</t>
+    <t># set command configuration for Panorama version 9.0</t>
   </si>
   <si>
     <t># commands are expected to be load in order</t>
@@ -296,9 +296,45 @@
     <t># remove admin/admin default and add user defined super user</t>
   </si>
   <si>
+    <t># recommended to delete the admin user with another superuser username</t>
+  </si>
+  <si>
     <t>delete mgt-config users admin</t>
   </si>
   <si>
+    <t># add password complexity profile - will not effect existing passwords</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity enabled yes</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity minimum-length 12</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity minimum-uppercase-letters 1</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity minimum-lowercase-letters 1</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity minimum-numeric-letters 1</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity minimum-special-characters 1</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity block-username-inclusion yes</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity password-history-count 24</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity new-password-differs-by-characters 3</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity password-change expiration-period 90</t>
+  </si>
+  <si>
     <t># additional base Panorama system configuration</t>
   </si>
   <si>
@@ -368,6 +404,18 @@
     <t>set deviceconfig setting management max-rows-in-csv-export 1048576</t>
   </si>
   <si>
+    <t>set deviceconfig setting management admin-lockout failed-attempts 5</t>
+  </si>
+  <si>
+    <t>set deviceconfig setting management admin-lockout lockout-time 30</t>
+  </si>
+  <si>
+    <t>set deviceconfig setting management idle-timeout 10</t>
+  </si>
+  <si>
+    <t>set deviceconfig setting management auto-acquire-commit-lock yes</t>
+  </si>
+  <si>
     <t># Panorama log settings</t>
   </si>
   <si>
@@ -491,25 +539,7 @@
     <t>set shared tag Internal comments ""Internal to Internal""</t>
   </si>
   <si>
-    <t>set shared tag iron-skillet-version comments ""version 0.0.1 for 9.0: version of this IronSkillet template file""</t>
-  </si>
-  <si>
-    <t>set shared external-list ""Team Cymru Bogons IPv4"" type ip recurring hourly</t>
-  </si>
-  <si>
-    <t>set shared external-list ""Team Cymru Bogons IPv4"" type ip url http://www.team-cymru.org/Services/Bogons/fullbogons-ipv4.txt</t>
-  </si>
-  <si>
-    <t>set shared external-list ""Team Cymru Bogons IPv4"" type ip description ""IPv4 addresses that should not be routed across the Internet. Either reserved IP address space or unassigned and may be used for malicious purposes. More information: http://www.team-cymru.com/bogon-reference.html""</t>
-  </si>
-  <si>
-    <t>set shared external-list ""Team Cymru Bogons IPv6"" type ip recurring hourly</t>
-  </si>
-  <si>
-    <t>set shared external-list ""Team Cymru Bogons IPv6"" type ip url http://www.team-cymru.org/Services/Bogons/fullbogons-ipv6.txt</t>
-  </si>
-  <si>
-    <t>set shared external-list ""Team Cymru Bogons IPv6"" type ip description ""IPv6 addresses that should not be routed across the Internet. Either reserved IP address space or unassigned and may be used for malicious purposes. More information: http://www.team-cymru.com/bogon-reference.html""</t>
+    <t>set shared tag iron-skillet-version comments ""version 0.0.2 for 9.0: version of this IronSkillet template file""</t>
   </si>
   <si>
     <t># shared log settings</t>
@@ -1553,7 +1583,7 @@
     <t>set shared pre-rulebase security rules ""Outbound Block Rule"" source any</t>
   </si>
   <si>
-    <t>set shared pre-rulebase security rules ""Outbound Block Rule"" destination [ panw-highrisk-ip-list panw-known-ip-list ]</t>
+    <t>set shared pre-rulebase security rules ""Outbound Block Rule"" destination [ panw-highrisk-ip-list panw-known-ip-list panw-bulletproof-ip-list ]</t>
   </si>
   <si>
     <t>set shared pre-rulebase security rules ""Outbound Block Rule"" source-user any</t>
@@ -1592,7 +1622,7 @@
     <t>set shared pre-rulebase security rules ""Inbound Block Rule"" from any</t>
   </si>
   <si>
-    <t>set shared pre-rulebase security rules ""Inbound Block Rule"" source [ panw-highrisk-ip-list panw-known-ip-list ]</t>
+    <t>set shared pre-rulebase security rules ""Inbound Block Rule"" source [ panw-highrisk-ip-list panw-known-ip-list panw-bulletproof-ip-list ]</t>
   </si>
   <si>
     <t>set shared pre-rulebase security rules ""Inbound Block Rule"" destination any</t>
@@ -1664,96 +1694,6 @@
     <t>set shared pre-rulebase security rules ""DNS Sinkhole Block"" tag Outbound</t>
   </si>
   <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" description ""Block outbound sessions with a destination address matching a known bogon address that should not be transitting the firewall. Add known exceptions to the rule before activating.""</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" target negate no</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" to any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" from any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" source any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" destination [ ""Team Cymru Bogons IPv4"" ""Team Cymru Bogons IPv6"" ]</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" source-user any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" category any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" application any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" service any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" hip-profiles any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" action deny</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" log-setting default</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" tag Outbound</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" disabled yes</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" description ""Block inbound sessions with a source address matching a known bogon address that should not be transitting the firewall. Add known exceptions to the rule before activating.""</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" target negate no</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" to any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" from any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" source [ ""Team Cymru Bogons IPv4"" ""Team Cymru Bogons IPv6"" ]</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" destination any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" source-user any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" category any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" application any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" service any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" hip-profiles any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" action deny</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" log-setting default</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" tag Inbound</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" disabled yes</t>
-  </si>
-  <si>
     <t>set shared pre-rulebase decryption rules ""NO-Decrypt URL Categories"" target negate no</t>
   </si>
   <si>
@@ -1802,6 +1742,36 @@
     <t>set template iron-skillet config vsys vsys1</t>
   </si>
   <si>
+    <t>set template iron-skillet config mgt-config password-complexity enabled yes</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity minimum-length 12</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity minimum-uppercase-letters 1</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity minimum-lowercase-letters 1</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity minimum-numeric-letters 1</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity minimum-special-characters 1</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity block-username-inclusion yes</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity password-history-count 24</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity new-password-differs-by-characters 3</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity password-change expiration-period 90</t>
+  </si>
+  <si>
     <t>set template iron-skillet config deviceconfig system update-schedule statistics-service application-reports yes</t>
   </si>
   <si>
@@ -1844,6 +1814,18 @@
     <t>set template iron-skillet config deviceconfig system update-schedule wildfire recurring every-min action download-and-install</t>
   </si>
   <si>
+    <t>set template iron-skillet config deviceconfig system update-schedule global-protect-datafile recurring hourly at 40</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig system update-schedule global-protect-datafile recurring hourly action download-and-install</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig system update-schedule global-protect-clientless-vpn recurring hourly at 50</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig system update-schedule global-protect-clientless-vpn recurring hourly action download-and-install</t>
+  </si>
+  <si>
     <t>set template iron-skillet config deviceconfig system snmp-setting access-setting version v3</t>
   </si>
   <si>
@@ -1875,6 +1857,18 @@
   </si>
   <si>
     <t>set template iron-skillet config deviceconfig setting management max-rows-in-csv-export 1048576</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig setting management admin-lockout failed-attempts 5</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig setting management admin-lockout lockout-time 30</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig setting management idle-timeout 10</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig setting management auto-acquire-commit-lock yes</t>
   </si>
   <si>
     <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit pe size-limit 10</t>
@@ -2880,7 +2874,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A787"/>
+  <dimension ref="A2:A788"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2981,8 +2975,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3041,20 +3035,14 @@
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>106</v>
-      </c>
-    </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36">
-        <f>SUBSTITUTE("set deviceconfig system config-bundle-export-schedule Recommended_Config_Export protocol scp hostname {{ CONFIG_EXPORT_IP }}", "{{ CONFIG_EXPORT_IP }}", 'values'!B7)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:1">
@@ -3098,128 +3086,128 @@
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45">
-        <f>SUBSTITUTE("set deviceconfig setting management api key lifetime {{ API_KEY_LIFETIME }}", "{{ API_KEY_LIFETIME }}", 'values'!B29)</f>
-        <v>0</v>
+      <c r="A45" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>116</v>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>118</v>
+      <c r="A49">
+        <f>SUBSTITUTE("set deviceconfig system config-bundle-export-schedule Recommended_Config_Export protocol scp hostname {{ CONFIG_EXPORT_IP }}", "{{ CONFIG_EXPORT_IP }}", 'values'!B7)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
-        <v>0</v>
+      <c r="A50" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
-        <v>0</v>
+      <c r="A51" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
-        <v>0</v>
+      <c r="A52" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58">
-        <f>SUBSTITUTE("set panorama log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
+        <f>SUBSTITUTE("set deviceconfig setting management api key lifetime {{ API_KEY_LIFETIME }}", "{{ API_KEY_LIFETIME }}", 'values'!B29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" t="s">
-        <v>132</v>
+      <c r="A67">
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" t="s">
-        <v>133</v>
+      <c r="A68">
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" t="s">
-        <v>134</v>
+      <c r="A69">
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:1">
@@ -3248,249 +3236,255 @@
       </c>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" t="s">
-        <v>140</v>
+      <c r="A75">
+        <f>SUBSTITUTE("set panorama log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
         <v>152</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>153</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97">
-        <f>SUBSTITUTE("set shared address Sinkhole-IPv4 ip-netmask {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
+      <c r="A97" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98">
-        <f>SUBSTITUTE("set shared address Sinkhole-IPv6 ip-netmask {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A98" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1">
-      <c r="A106" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1">
-      <c r="A108" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="114" spans="1:1">
-      <c r="A114" t="s">
-        <v>173</v>
+      <c r="A114">
+        <f>SUBSTITUTE("set shared address Sinkhole-IPv4 ip-netmask {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:1">
-      <c r="A115" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1">
-      <c r="A116" t="s">
-        <v>175</v>
+      <c r="A115">
+        <f>SUBSTITUTE("set shared address Sinkhole-IPv6 ip-netmask {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
         <v>186</v>
       </c>
     </row>
@@ -3544,43 +3538,43 @@
         <v>196</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
-      <c r="A139" t="s">
-        <v>197</v>
-      </c>
-    </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" t="s">
         <v>204</v>
       </c>
     </row>
@@ -3634,1268 +3628,1268 @@
         <v>214</v>
       </c>
     </row>
-    <row r="158" spans="1:1">
-      <c r="A158" t="s">
-        <v>215</v>
-      </c>
-    </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="220" spans="1:1">
-      <c r="A220">
-        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="221" spans="1:1">
-      <c r="A221">
-        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A221" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="231" spans="1:1">
-      <c r="A231" t="s">
-        <v>286</v>
+      <c r="A231">
+        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="232" spans="1:1">
-      <c r="A232" t="s">
-        <v>287</v>
+      <c r="A232">
+        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="236" spans="1:1">
-      <c r="A236">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="237" spans="1:1">
-      <c r="A237">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A237" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="247" spans="1:1">
-      <c r="A247" t="s">
-        <v>300</v>
+      <c r="A247">
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="248" spans="1:1">
-      <c r="A248" t="s">
-        <v>301</v>
+      <c r="A248">
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1">
+      <c r="A252" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="252" spans="1:1">
-      <c r="A252">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="253" spans="1:1">
-      <c r="A253">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A253" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="263" spans="1:1">
-      <c r="A263" t="s">
-        <v>314</v>
+      <c r="A263">
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="264" spans="1:1">
-      <c r="A264" t="s">
-        <v>315</v>
+      <c r="A264">
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1">
+      <c r="A268" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="268" spans="1:1">
-      <c r="A268">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="269" spans="1:1">
-      <c r="A269">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A269" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279">
-        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280">
-        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="290" spans="1:1">
-      <c r="A290" t="s">
-        <v>337</v>
+      <c r="A290">
+        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="291" spans="1:1">
-      <c r="A291" t="s">
-        <v>338</v>
+      <c r="A291">
+        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="391" spans="1:1">
       <c r="A391" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1">
+      <c r="A409" t="s">
         <v>455</v>
       </c>
     </row>
@@ -4949,98 +4943,98 @@
         <v>465</v>
       </c>
     </row>
-    <row r="420" spans="1:1">
-      <c r="A420" t="s">
-        <v>466</v>
-      </c>
-    </row>
     <row r="421" spans="1:1">
       <c r="A421" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1">
+      <c r="A439" t="s">
         <v>484</v>
       </c>
     </row>
@@ -5094,1765 +5088,1767 @@
         <v>494</v>
       </c>
     </row>
-    <row r="450" spans="1:1">
-      <c r="A450" t="s">
-        <v>495</v>
-      </c>
-    </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="528" spans="1:1">
-      <c r="A528" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="529" spans="1:1">
       <c r="A529" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="532" spans="1:1">
-      <c r="A532" t="s">
-        <v>577</v>
+      <c r="A532">
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="533" spans="1:1">
-      <c r="A533" t="s">
-        <v>578</v>
+      <c r="A533">
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>591</v>
+        <v>587</v>
+      </c>
+    </row>
+    <row r="547" spans="1:1">
+      <c r="A547" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="548" spans="1:1">
       <c r="A548" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="549" spans="1:1">
       <c r="A549" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="550" spans="1:1">
       <c r="A550" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="551" spans="1:1">
       <c r="A551" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="563" spans="1:1">
-      <c r="A563" t="s">
-        <v>607</v>
+      <c r="A563">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="564" spans="1:1">
-      <c r="A564" t="s">
-        <v>608</v>
+      <c r="A564">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="565" spans="1:1">
-      <c r="A565" t="s">
-        <v>609</v>
+      <c r="A565">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B16)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B20)</f>
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="567" spans="1:1">
-      <c r="A567">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A567" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="568" spans="1:1">
-      <c r="A568">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B16)</f>
-        <v>0</v>
+      <c r="A568" t="s">
+        <v>605</v>
       </c>
     </row>
     <row r="569" spans="1:1">
-      <c r="A569">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B17)</f>
-        <v>0</v>
+      <c r="A569" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
     </row>
     <row r="615" spans="1:1">
       <c r="A615" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="617" spans="1:1">
-      <c r="A617">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
-        <v>0</v>
+      <c r="A617" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="618" spans="1:1">
       <c r="A618">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="619" spans="1:1">
       <c r="A619">
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="620" spans="1:1">
+      <c r="A620">
         <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="620" spans="1:1">
-      <c r="A620" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="621" spans="1:1">
       <c r="A621" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
     </row>
     <row r="622" spans="1:1">
       <c r="A622" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
     </row>
     <row r="623" spans="1:1">
-      <c r="A623">
+      <c r="A623" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="624" spans="1:1">
+      <c r="A624">
         <f>SUBSTITUTE("set template iron-skillet config shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="624" spans="1:1">
-      <c r="A624" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="625" spans="1:1">
       <c r="A625" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
     </row>
     <row r="627" spans="1:1">
       <c r="A627" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
     </row>
     <row r="628" spans="1:1">
       <c r="A628" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
     </row>
     <row r="629" spans="1:1">
       <c r="A629" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="630" spans="1:1">
       <c r="A630" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="631" spans="1:1">
       <c r="A631" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="632" spans="1:1">
       <c r="A632" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
     </row>
     <row r="633" spans="1:1">
       <c r="A633" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
     </row>
     <row r="634" spans="1:1">
       <c r="A634" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="636" spans="1:1">
-      <c r="A636" t="s">
-        <v>671</v>
+        <v>667</v>
+      </c>
+    </row>
+    <row r="635" spans="1:1">
+      <c r="A635" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="637" spans="1:1">
       <c r="A637" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
     </row>
     <row r="638" spans="1:1">
-      <c r="A638">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A638" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="641" spans="1:1">
+      <c r="A641">
         <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B11), "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="642" spans="1:1">
-      <c r="A642" t="s">
-        <v>673</v>
-      </c>
-    </row>
     <row r="643" spans="1:1">
-      <c r="A643">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A643" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="647" spans="1:1">
+      <c r="A647">
         <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="648" spans="1:1">
-      <c r="A648" t="s">
-        <v>674</v>
-      </c>
-    </row>
     <row r="649" spans="1:1">
-      <c r="A649">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A649" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B13), "{{ STACK }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B14), "{{ STACK }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B13), "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652">
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B14), "{{ STACK }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="653" spans="1:1">
+      <c r="A653">
         <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B15), "{{ STACK }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="654" spans="1:1">
-      <c r="A654">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="659" spans="1:1">
       <c r="A659">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="664" spans="1:1">
       <c r="A664">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="665" spans="1:1">
       <c r="A665">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="670" spans="1:1">
       <c r="A670">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="672" spans="1:1">
       <c r="A672">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="673" spans="1:1">
       <c r="A673">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="675" spans="1:1">
       <c r="A675">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="676" spans="1:1">
       <c r="A676">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="677" spans="1:1">
       <c r="A677">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="678" spans="1:1">
       <c r="A678">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="679" spans="1:1">
       <c r="A679">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="680" spans="1:1">
       <c r="A680">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="681" spans="1:1">
       <c r="A681">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="682" spans="1:1">
       <c r="A682">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="683" spans="1:1">
       <c r="A683">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="684" spans="1:1">
       <c r="A684">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="685" spans="1:1">
       <c r="A685">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="686" spans="1:1">
       <c r="A686">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="687" spans="1:1">
       <c r="A687">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="688" spans="1:1">
       <c r="A688">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="689" spans="1:1">
       <c r="A689">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="690" spans="1:1">
       <c r="A690">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="691" spans="1:1">
       <c r="A691">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="692" spans="1:1">
       <c r="A692">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="693" spans="1:1">
       <c r="A693">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="694" spans="1:1">
       <c r="A694">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="695" spans="1:1">
       <c r="A695">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="696" spans="1:1">
       <c r="A696">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="697" spans="1:1">
       <c r="A697">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="698" spans="1:1">
       <c r="A698">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="699" spans="1:1">
       <c r="A699">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="700" spans="1:1">
       <c r="A700">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="701" spans="1:1">
       <c r="A701">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="702" spans="1:1">
       <c r="A702">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="703" spans="1:1">
       <c r="A703">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="704" spans="1:1">
       <c r="A704">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="705" spans="1:1">
       <c r="A705">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="706" spans="1:1">
       <c r="A706">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="707" spans="1:1">
       <c r="A707">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="708" spans="1:1">
       <c r="A708">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="709" spans="1:1">
       <c r="A709">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="710" spans="1:1">
       <c r="A710">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="711" spans="1:1">
       <c r="A711">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="712" spans="1:1">
       <c r="A712">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="713" spans="1:1">
       <c r="A713">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="714" spans="1:1">
       <c r="A714">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="715" spans="1:1">
       <c r="A715">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="716" spans="1:1">
       <c r="A716">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="717" spans="1:1">
       <c r="A717">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="718" spans="1:1">
       <c r="A718">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="719" spans="1:1">
       <c r="A719">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="720" spans="1:1">
       <c r="A720">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="721" spans="1:1">
       <c r="A721">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="736" spans="1:1">
+      <c r="A736">
         <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" email-profile Sample_Email_Profile", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="737" spans="1:1">
-      <c r="A737" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="766" spans="1:1">
       <c r="A766" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="767" spans="1:1">
       <c r="A767" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="768" spans="1:1">
       <c r="A768" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="769" spans="1:1">
       <c r="A769" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="770" spans="1:1">
       <c r="A770" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="771" spans="1:1">
       <c r="A771" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
     </row>
     <row r="772" spans="1:1">
       <c r="A772" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
     </row>
     <row r="773" spans="1:1">
       <c r="A773" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
     </row>
     <row r="774" spans="1:1">
       <c r="A774" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
     <row r="775" spans="1:1">
       <c r="A775" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
     </row>
     <row r="776" spans="1:1">
       <c r="A776" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
     </row>
     <row r="777" spans="1:1">
       <c r="A777" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="778" spans="1:1">
       <c r="A778" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
     </row>
     <row r="779" spans="1:1">
       <c r="A779" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
     </row>
     <row r="780" spans="1:1">
       <c r="A780" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
     </row>
     <row r="781" spans="1:1">
       <c r="A781" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
     </row>
     <row r="782" spans="1:1">
       <c r="A782" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="783" spans="1:1">
       <c r="A783" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="784" spans="1:1">
       <c r="A784" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
     </row>
     <row r="785" spans="1:1">
       <c r="A785" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
     </row>
     <row r="786" spans="1:1">
       <c r="A786" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
     </row>
     <row r="787" spans="1:1">
       <c r="A787" t="s">
-        <v>725</v>
+        <v>722</v>
+      </c>
+    </row>
+    <row r="788" spans="1:1">
+      <c r="A788" t="s">
+        <v>723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
panos snippets meta-cnc file
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="707">
   <si>
     <t>Variable Name</t>
   </si>
@@ -47,7 +47,7 @@
     <t>PANORAMA_IP</t>
   </si>
   <si>
-    <t>192.168.55.8</t>
+    <t>192.168.55.161</t>
   </si>
   <si>
     <t>Panorama IP</t>
@@ -263,10 +263,19 @@
     <t>syslog server ip address</t>
   </si>
   <si>
+    <t>API_KEY_LIFETIME</t>
+  </si>
+  <si>
+    <t>lifetime for the api key in minutes</t>
+  </si>
+  <si>
     <t>INCLUDE_PAN_EDL</t>
   </si>
   <si>
-    <t>include the predefined Palo Alto Networks external lists</t>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>include the predefined Palo Alto Networks external lists security rules</t>
   </si>
   <si>
     <t># set command configuration for Panorama version 8.1</t>
@@ -2467,7 +2476,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2789,11 +2798,22 @@
       <c r="A29" t="s">
         <v>82</v>
       </c>
-      <c r="B29" t="b">
-        <v>1</v>
+      <c r="B29">
+        <v>525600</v>
       </c>
       <c r="C29" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2811,27 +2831,27 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -2884,7 +2904,7 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -2901,77 +2921,77 @@
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:1">
@@ -2982,57 +3002,57 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:1">
@@ -3055,27 +3075,27 @@
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:1">
@@ -3086,177 +3106,177 @@
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="96" spans="1:1">
@@ -3273,542 +3293,542 @@
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="209" spans="1:1">
@@ -3825,62 +3845,62 @@
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="223" spans="1:1">
@@ -3897,62 +3917,62 @@
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="237" spans="1:1">
@@ -3969,62 +3989,62 @@
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="251" spans="1:1">
@@ -4041,42 +4061,42 @@
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="261" spans="1:1">
@@ -4093,1412 +4113,1412 @@
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="548" spans="1:1">
@@ -5527,227 +5547,227 @@
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="597" spans="1:1">
@@ -5770,17 +5790,17 @@
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
     </row>
     <row r="603" spans="1:1">
@@ -5791,67 +5811,67 @@
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
     </row>
     <row r="617" spans="1:1">
       <c r="A617" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
     </row>
     <row r="618" spans="1:1">
@@ -5874,7 +5894,7 @@
     </row>
     <row r="622" spans="1:1">
       <c r="A622" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
     </row>
     <row r="623" spans="1:1">
@@ -5903,7 +5923,7 @@
     </row>
     <row r="628" spans="1:1">
       <c r="A628" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
     </row>
     <row r="629" spans="1:1">
@@ -6424,257 +6444,257 @@
     </row>
     <row r="717" spans="1:1">
       <c r="A717" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
     </row>
     <row r="718" spans="1:1">
       <c r="A718" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
     </row>
     <row r="719" spans="1:1">
       <c r="A719" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
     </row>
     <row r="720" spans="1:1">
       <c r="A720" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
     </row>
     <row r="721" spans="1:1">
       <c r="A721" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
     </row>
     <row r="766" spans="1:1">
       <c r="A766" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
     </row>
     <row r="767" spans="1:1">
       <c r="A767" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rebuild all full configs
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="706">
   <si>
     <t>Variable Name</t>
   </si>
@@ -296,9 +296,45 @@
     <t># remove admin/admin default and add user defined super user</t>
   </si>
   <si>
+    <t># recommended to delete the admin user with another superuser username</t>
+  </si>
+  <si>
     <t>delete mgt-config users admin</t>
   </si>
   <si>
+    <t># add password complexity profile - will not effect existing passwords</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity enabled yes</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity minimum-length 12</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity minimum-uppercase-letters 1</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity minimum-lowercase-letters 1</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity minimum-numeric-letters 1</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity minimum-special-characters 1</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity block-username-inclusion yes</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity password-history-count 24</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity new-password-differs-by-characters 3</t>
+  </si>
+  <si>
+    <t>set mgt-config password-complexity password-change expiration-period 90</t>
+  </si>
+  <si>
     <t># additional base Panorama system configuration</t>
   </si>
   <si>
@@ -344,7 +380,7 @@
     <t>set deviceconfig system config-bundle-export-schedule Recommended_Config_Export protocol scp username testuser</t>
   </si>
   <si>
-    <t>set deviceconfig system config-bundle-export-schedule Recommended_Config_Export protocol scp password</t>
+    <t>set deviceconfig system config-bundle-export-schedule Recommended_Config_Export protocol scp password -AQ==zPJb3ngM1sGjXlfX2+Qk6rbdv1I=ucInIpBmFcnkQK7zF4VO1w==</t>
   </si>
   <si>
     <t>set deviceconfig system config-bundle-export-schedule Recommended_Config_Export start-time 02:00</t>
@@ -368,6 +404,18 @@
     <t>set deviceconfig setting management max-rows-in-csv-export 1048576</t>
   </si>
   <si>
+    <t>set deviceconfig setting management admin-lockout failed-attempts 5</t>
+  </si>
+  <si>
+    <t>set deviceconfig setting management admin-lockout lockout-time 30</t>
+  </si>
+  <si>
+    <t>set deviceconfig setting management idle-timeout 10</t>
+  </si>
+  <si>
+    <t>set deviceconfig setting management auto-acquire-commit-lock yes</t>
+  </si>
+  <si>
     <t># Panorama log settings</t>
   </si>
   <si>
@@ -491,25 +539,7 @@
     <t>set shared tag Internal comments ""Internal to Internal""</t>
   </si>
   <si>
-    <t>set shared tag iron-skillet-version comments ""version 1.0.5: version of this iron-skillet template file""</t>
-  </si>
-  <si>
-    <t>set shared external-list ""Team Cymru Bogons IPv4"" type ip recurring hourly</t>
-  </si>
-  <si>
-    <t>set shared external-list ""Team Cymru Bogons IPv4"" type ip url http://www.team-cymru.org/Services/Bogons/fullbogons-ipv4.txt</t>
-  </si>
-  <si>
-    <t>set shared external-list ""Team Cymru Bogons IPv4"" type ip description ""IPv4 addresses that should not be routed across the Internet. Either reserved IP address space or unassigned and may be used for malicious purposes. More information: http://www.team-cymru.com/bogon-reference.html""</t>
-  </si>
-  <si>
-    <t>set shared external-list ""Team Cymru Bogons IPv6"" type ip recurring hourly</t>
-  </si>
-  <si>
-    <t>set shared external-list ""Team Cymru Bogons IPv6"" type ip url http://www.team-cymru.org/Services/Bogons/fullbogons-ipv6.txt</t>
-  </si>
-  <si>
-    <t>set shared external-list ""Team Cymru Bogons IPv6"" type ip description ""IPv6 addresses that should not be routed across the Internet. Either reserved IP address space or unassigned and may be used for malicious purposes. More information: http://www.team-cymru.com/bogon-reference.html""</t>
+    <t>set shared tag iron-skillet-version comments ""version 1.0.6: version of this iron-skillet template file""</t>
   </si>
   <si>
     <t># shared log settings</t>
@@ -647,10 +677,10 @@
     <t>set shared profiles virus Alert-Only-AV decoder http wildfire-action alert</t>
   </si>
   <si>
-    <t>set shared profiles virus Alert-Only-AV decoder imap action default</t>
-  </si>
-  <si>
-    <t>set shared profiles virus Alert-Only-AV decoder imap wildfire-action default</t>
+    <t>set shared profiles virus Alert-Only-AV decoder imap action alert</t>
+  </si>
+  <si>
+    <t>set shared profiles virus Alert-Only-AV decoder imap wildfire-action alert</t>
   </si>
   <si>
     <t>set shared profiles virus Alert-Only-AV decoder pop3 action alert</t>
@@ -782,13 +812,13 @@
     <t>set shared profiles virus Exception-AV decoder ftp action reset-both</t>
   </si>
   <si>
-    <t>set shared profiles virus Exception-AV decoder ftp wildfire-action default</t>
+    <t>set shared profiles virus Exception-AV decoder ftp wildfire-action reset-both</t>
   </si>
   <si>
     <t>set shared profiles virus Exception-AV decoder http action reset-both</t>
   </si>
   <si>
-    <t>set shared profiles virus Exception-AV decoder http wildfire-action default</t>
+    <t>set shared profiles virus Exception-AV decoder http wildfire-action reset-both</t>
   </si>
   <si>
     <t>set shared profiles virus Exception-AV decoder imap action reset-both</t>
@@ -806,7 +836,7 @@
     <t>set shared profiles virus Exception-AV decoder smb action reset-both</t>
   </si>
   <si>
-    <t>set shared profiles virus Exception-AV decoder smb wildfire-action default</t>
+    <t>set shared profiles virus Exception-AV decoder smb wildfire-action reset-both</t>
   </si>
   <si>
     <t>set shared profiles virus Exception-AV decoder smtp action reset-both</t>
@@ -1250,13 +1280,13 @@
     <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement log-severity medium</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Alert-Only-URL action block</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Alert-Only-URL alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set shared profiles url-filtering Alert-Only-URL alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Exception-URL credential-enforcement mode ip-user</t>
@@ -1265,7 +1295,7 @@
     <t>set shared profiles url-filtering Exception-URL credential-enforcement log-severity high</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Exception-URL credential-enforcement block [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List ]</t>
+    <t>set shared profiles url-filtering Exception-URL credential-enforcement block [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Exception-URL log-http-hdr-user-agent yes</t>
@@ -1613,96 +1643,6 @@
     <t>set shared pre-rulebase security rules ""DNS Sinkhole Block"" tag Outbound</t>
   </si>
   <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" description ""Block outbound sessions with a destination address matching a known bogon address that should not be transitting the firewall. Add known exceptions to the rule before activating.""</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" target negate no</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" to any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" from any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" source any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" destination [ ""Team Cymru Bogons IPv4"" ""Team Cymru Bogons IPv6"" ]</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" source-user any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" category any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" application any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" service any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" hip-profiles any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" action deny</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" log-setting default</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" tag Outbound</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Outbound Bogon Block Rule"" disabled yes</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" description ""Block inbound sessions with a source address matching a known bogon address that should not be transitting the firewall. Add known exceptions to the rule before activating.""</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" target negate no</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" to any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" from any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" source [ ""Team Cymru Bogons IPv4"" ""Team Cymru Bogons IPv6"" ]</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" destination any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" source-user any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" category any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" application any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" service any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" hip-profiles any</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" action deny</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" log-setting default</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" tag Inbound</t>
-  </si>
-  <si>
-    <t>set shared pre-rulebase security rules ""Inbound Bogon Block Rule"" disabled yes</t>
-  </si>
-  <si>
     <t>set shared pre-rulebase decryption rules ""NO-Decrypt URL Categories"" target negate no</t>
   </si>
   <si>
@@ -1751,6 +1691,36 @@
     <t>set template iron-skillet config vsys vsys1</t>
   </si>
   <si>
+    <t>set template iron-skillet config mgt-config password-complexity enabled yes</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity minimum-length 12</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity minimum-uppercase-letters 1</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity minimum-lowercase-letters 1</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity minimum-numeric-letters 1</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity minimum-special-characters 1</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity block-username-inclusion yes</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity password-history-count 24</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity new-password-differs-by-characters 3</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config mgt-config password-complexity password-change expiration-period 90</t>
+  </si>
+  <si>
     <t>set template iron-skillet config deviceconfig system update-schedule statistics-service application-reports yes</t>
   </si>
   <si>
@@ -1793,6 +1763,18 @@
     <t>set template iron-skillet config deviceconfig system update-schedule wildfire recurring every-min action download-and-install</t>
   </si>
   <si>
+    <t>set template iron-skillet config deviceconfig system update-schedule global-protect-datafile recurring hourly at 40</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig system update-schedule global-protect-datafile recurring hourly action download-and-install</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig system update-schedule global-protect-clientless-vpn recurring hourly at 50</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig system update-schedule global-protect-clientless-vpn recurring hourly action download-and-install</t>
+  </si>
+  <si>
     <t>set template iron-skillet config deviceconfig system snmp-setting access-setting version v3</t>
   </si>
   <si>
@@ -1823,6 +1805,18 @@
     <t>set template iron-skillet config deviceconfig setting management max-rows-in-csv-export 1048576</t>
   </si>
   <si>
+    <t>set template iron-skillet config deviceconfig setting management admin-lockout failed-attempts 5</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig setting management admin-lockout lockout-time 30</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig setting management idle-timeout 10</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig setting management auto-acquire-commit-lock yes</t>
+  </si>
+  <si>
     <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit pe size-limit 10</t>
   </si>
   <si>
@@ -1848,6 +1842,9 @@
   </si>
   <si>
     <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit linux size-limit 2</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit script size-limit 2000</t>
   </si>
   <si>
     <t>set template iron-skillet config deviceconfig setting wildfire report-benign-file yes</t>
@@ -2823,7 +2820,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A767"/>
+  <dimension ref="A2:A769"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2924,8 +2921,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2984,20 +2981,14 @@
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>106</v>
-      </c>
-    </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36">
-        <f>SUBSTITUTE("set deviceconfig system config-bundle-export-schedule Recommended_Config_Export protocol scp hostname {{ CONFIG_EXPORT_IP }}", "{{ CONFIG_EXPORT_IP }}", 'values'!B7)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:1">
@@ -3045,118 +3036,118 @@
         <v>116</v>
       </c>
     </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>117</v>
+      </c>
+    </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set deviceconfig system config-bundle-export-schedule Recommended_Config_Export protocol scp hostname {{ CONFIG_EXPORT_IP }}", "{{ CONFIG_EXPORT_IP }}", 'values'!B7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
-        <v>0</v>
+      <c r="A50" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
-        <v>0</v>
+      <c r="A51" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57">
-        <f>SUBSTITUTE("set panorama log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
-        <v>0</v>
+      <c r="A57" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" t="s">
-        <v>132</v>
+      <c r="A66">
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" t="s">
-        <v>133</v>
+      <c r="A67">
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" t="s">
-        <v>134</v>
+      <c r="A68">
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:1">
@@ -3185,249 +3176,255 @@
       </c>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" t="s">
-        <v>140</v>
+      <c r="A74">
+        <f>SUBSTITUTE("set panorama log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
         <v>152</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>153</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96">
-        <f>SUBSTITUTE("set shared address Sinkhole-IPv4 ip-netmask {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
+      <c r="A96" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97">
-        <f>SUBSTITUTE("set shared address Sinkhole-IPv6 ip-netmask {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A97" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1">
-      <c r="A107" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="113" spans="1:1">
-      <c r="A113" t="s">
-        <v>173</v>
+      <c r="A113">
+        <f>SUBSTITUTE("set shared address Sinkhole-IPv4 ip-netmask {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:1">
-      <c r="A114" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1">
-      <c r="A115" t="s">
-        <v>175</v>
+      <c r="A114">
+        <f>SUBSTITUTE("set shared address Sinkhole-IPv6 ip-netmask {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
         <v>186</v>
       </c>
     </row>
@@ -3481,43 +3478,43 @@
         <v>196</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
-      <c r="A138" t="s">
-        <v>197</v>
-      </c>
-    </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="s">
         <v>204</v>
       </c>
     </row>
@@ -3571,1183 +3568,1183 @@
         <v>214</v>
       </c>
     </row>
-    <row r="157" spans="1:1">
-      <c r="A157" t="s">
-        <v>215</v>
-      </c>
-    </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="209" spans="1:1">
-      <c r="A209">
-        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="210" spans="1:1">
-      <c r="A210">
-        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A210" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="220" spans="1:1">
-      <c r="A220" t="s">
-        <v>276</v>
+      <c r="A220">
+        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="221" spans="1:1">
-      <c r="A221" t="s">
-        <v>277</v>
+      <c r="A221">
+        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="223" spans="1:1">
-      <c r="A223">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="224" spans="1:1">
-      <c r="A224">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A224" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="234" spans="1:1">
-      <c r="A234" t="s">
-        <v>288</v>
+      <c r="A234">
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="235" spans="1:1">
-      <c r="A235" t="s">
-        <v>289</v>
+      <c r="A235">
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="237" spans="1:1">
-      <c r="A237">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="238" spans="1:1">
-      <c r="A238">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A238" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="248" spans="1:1">
-      <c r="A248" t="s">
-        <v>300</v>
+      <c r="A248">
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="249" spans="1:1">
-      <c r="A249" t="s">
-        <v>301</v>
+      <c r="A249">
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1">
+      <c r="A251" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="251" spans="1:1">
-      <c r="A251">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="252" spans="1:1">
-      <c r="A252">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A252" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="261" spans="1:1">
-      <c r="A261">
-        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
+      <c r="A261" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262">
-        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="263" spans="1:1">
-      <c r="A263" t="s">
-        <v>311</v>
+      <c r="A263">
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="272" spans="1:1">
-      <c r="A272" t="s">
-        <v>320</v>
+      <c r="A272">
+        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="273" spans="1:1">
-      <c r="A273" t="s">
-        <v>321</v>
+      <c r="A273">
+        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1">
+      <c r="A391" t="s">
         <v>438</v>
       </c>
     </row>
@@ -4801,98 +4798,98 @@
         <v>448</v>
       </c>
     </row>
-    <row r="402" spans="1:1">
-      <c r="A402" t="s">
-        <v>449</v>
-      </c>
-    </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1">
+      <c r="A421" t="s">
         <v>467</v>
       </c>
     </row>
@@ -4946,1755 +4943,1762 @@
         <v>477</v>
       </c>
     </row>
-    <row r="432" spans="1:1">
-      <c r="A432" t="s">
-        <v>478</v>
-      </c>
-    </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="510" spans="1:1">
-      <c r="A510" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="514" spans="1:1">
-      <c r="A514" t="s">
-        <v>560</v>
+      <c r="A514">
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="515" spans="1:1">
-      <c r="A515" t="s">
-        <v>561</v>
+      <c r="A515">
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>574</v>
+        <v>570</v>
+      </c>
+    </row>
+    <row r="529" spans="1:1">
+      <c r="A529" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="545" spans="1:1">
-      <c r="A545" t="s">
-        <v>590</v>
+      <c r="A545">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="546" spans="1:1">
-      <c r="A546" t="s">
-        <v>591</v>
+      <c r="A546">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="547" spans="1:1">
-      <c r="A547" t="s">
-        <v>592</v>
+      <c r="A547">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B16)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="548" spans="1:1">
       <c r="A548">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B20)</f>
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="549" spans="1:1">
-      <c r="A549">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A549" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="550" spans="1:1">
-      <c r="A550">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B16)</f>
-        <v>0</v>
+      <c r="A550" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="551" spans="1:1">
-      <c r="A551">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B17)</f>
-        <v>0</v>
+      <c r="A551" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
     <row r="597" spans="1:1">
-      <c r="A597">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
-        <v>0</v>
+      <c r="A597" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="598" spans="1:1">
-      <c r="A598">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
-        <v>0</v>
+      <c r="A598" t="s">
+        <v>636</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599">
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="600" spans="1:1">
+      <c r="A600">
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="601" spans="1:1">
+      <c r="A601">
         <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="600" spans="1:1">
-      <c r="A600" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="601" spans="1:1">
-      <c r="A601" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="603" spans="1:1">
-      <c r="A603">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
-        <v>0</v>
+      <c r="A603" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="605" spans="1:1">
-      <c r="A605" t="s">
-        <v>642</v>
+      <c r="A605">
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>651</v>
+        <v>648</v>
+      </c>
+    </row>
+    <row r="615" spans="1:1">
+      <c r="A615" t="s">
+        <v>649</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="618" spans="1:1">
+      <c r="A618" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="619" spans="1:1">
+      <c r="A619" t="s">
         <v>652</v>
-      </c>
-    </row>
-    <row r="617" spans="1:1">
-      <c r="A617" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="618" spans="1:1">
-      <c r="A618">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="619" spans="1:1">
-      <c r="A619">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B9)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="620" spans="1:1">
       <c r="A620">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="621" spans="1:1">
+      <c r="A621">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="622" spans="1:1">
+      <c r="A622">
         <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B11), "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="622" spans="1:1">
-      <c r="A622" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="623" spans="1:1">
-      <c r="A623">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="624" spans="1:1">
-      <c r="A624">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A624" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="625" spans="1:1">
       <c r="A625">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="626" spans="1:1">
       <c r="A626">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="627" spans="1:1">
+      <c r="A627">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="628" spans="1:1">
+      <c r="A628">
         <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="628" spans="1:1">
-      <c r="A628" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="629" spans="1:1">
-      <c r="A629">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="630" spans="1:1">
-      <c r="A630">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B13), "{{ STACK }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A630" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="631" spans="1:1">
       <c r="A631">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B14), "{{ STACK }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="632" spans="1:1">
       <c r="A632">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B15), "{{ STACK }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B13), "{{ STACK }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="633" spans="1:1">
+      <c r="A633">
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B14), "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="634" spans="1:1">
       <c r="A634">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="635" spans="1:1">
-      <c r="A635">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B15), "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="636" spans="1:1">
       <c r="A636">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="637" spans="1:1">
       <c r="A637">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="638" spans="1:1">
       <c r="A638">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="641" spans="1:1">
       <c r="A641">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="642" spans="1:1">
       <c r="A642">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="643" spans="1:1">
       <c r="A643">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="647" spans="1:1">
       <c r="A647">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="648" spans="1:1">
       <c r="A648">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="649" spans="1:1">
       <c r="A649">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="654" spans="1:1">
       <c r="A654">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="659" spans="1:1">
       <c r="A659">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="664" spans="1:1">
       <c r="A664">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="665" spans="1:1">
       <c r="A665">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="670" spans="1:1">
       <c r="A670">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="672" spans="1:1">
       <c r="A672">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="673" spans="1:1">
       <c r="A673">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="675" spans="1:1">
       <c r="A675">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="676" spans="1:1">
       <c r="A676">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="677" spans="1:1">
       <c r="A677">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="678" spans="1:1">
       <c r="A678">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="679" spans="1:1">
       <c r="A679">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="680" spans="1:1">
       <c r="A680">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="681" spans="1:1">
       <c r="A681">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="682" spans="1:1">
       <c r="A682">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="683" spans="1:1">
       <c r="A683">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="684" spans="1:1">
       <c r="A684">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="685" spans="1:1">
       <c r="A685">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="686" spans="1:1">
       <c r="A686">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="687" spans="1:1">
       <c r="A687">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="688" spans="1:1">
       <c r="A688">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="689" spans="1:1">
       <c r="A689">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="690" spans="1:1">
       <c r="A690">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="691" spans="1:1">
       <c r="A691">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="692" spans="1:1">
       <c r="A692">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="693" spans="1:1">
       <c r="A693">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="694" spans="1:1">
       <c r="A694">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="695" spans="1:1">
       <c r="A695">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="696" spans="1:1">
       <c r="A696">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="697" spans="1:1">
       <c r="A697">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="698" spans="1:1">
       <c r="A698">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="699" spans="1:1">
       <c r="A699">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="700" spans="1:1">
       <c r="A700">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="701" spans="1:1">
       <c r="A701">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="702" spans="1:1">
       <c r="A702">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="703" spans="1:1">
       <c r="A703">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="704" spans="1:1">
       <c r="A704">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="705" spans="1:1">
       <c r="A705">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="706" spans="1:1">
       <c r="A706">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="707" spans="1:1">
       <c r="A707">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="708" spans="1:1">
       <c r="A708">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="709" spans="1:1">
       <c r="A709">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="710" spans="1:1">
       <c r="A710">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="711" spans="1:1">
       <c r="A711">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="712" spans="1:1">
       <c r="A712">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="713" spans="1:1">
       <c r="A713">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="714" spans="1:1">
       <c r="A714">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="715" spans="1:1">
       <c r="A715">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="716" spans="1:1">
+      <c r="A716">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="717" spans="1:1">
+      <c r="A717">
         <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" email-profile Sample_Email_Profile", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="717" spans="1:1">
-      <c r="A717" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="718" spans="1:1">
-      <c r="A718" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="719" spans="1:1">
       <c r="A719" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
     </row>
     <row r="720" spans="1:1">
       <c r="A720" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
     </row>
     <row r="721" spans="1:1">
       <c r="A721" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="766" spans="1:1">
       <c r="A766" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="767" spans="1:1">
       <c r="A767" t="s">
-        <v>706</v>
+        <v>703</v>
+      </c>
+    </row>
+    <row r="768" spans="1:1">
+      <c r="A768" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="769" spans="1:1">
+      <c r="A769" t="s">
+        <v>705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update all full configs
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -1313,7 +1313,7 @@
     <t>set shared profiles url-filtering Outbound-URL credential-enforcement log-severity high</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Outbound-URL credential-enforcement block [ Black-List White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set shared profiles url-filtering Outbound-URL credential-enforcement block [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Outbound-URL log-http-hdr-user-agent yes</t>
@@ -1325,7 +1325,7 @@
     <t>set shared profiles url-filtering Outbound-URL log-http-hdr-xff yes</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Outbound-URL alert [ White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set shared profiles url-filtering Outbound-URL alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting White-List  ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Outbound-URL block [ command-and-control hacking malware phishing Black-List ]</t>
@@ -1337,10 +1337,10 @@
     <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement log-severity medium</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement alert [ Black-List White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
-  </si>
-  <si>
-    <t>set shared profiles url-filtering Alert-Only-URL alert [ Black-List White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
+  </si>
+  <si>
+    <t>set shared profiles url-filtering Alert-Only-URL alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Exception-URL credential-enforcement mode ip-user</t>
@@ -1349,7 +1349,7 @@
     <t>set shared profiles url-filtering Exception-URL credential-enforcement log-severity high</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Exception-URL credential-enforcement block [ Black-List White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set shared profiles url-filtering Exception-URL credential-enforcement block [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Exception-URL log-http-hdr-user-agent yes</t>
@@ -1361,7 +1361,7 @@
     <t>set shared profiles url-filtering Exception-URL log-http-hdr-xff yes</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Exception-URL alert [ White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set shared profiles url-filtering Exception-URL alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting White-List ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Exception-URL block [ command-and-control hacking malware phishing Black-List ]</t>

</xml_diff>

<commit_message>
panos set commands edits
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="706">
   <si>
     <t>Variable Name</t>
   </si>
@@ -38,7 +38,7 @@
     <t>PANORAMA_TYPE</t>
   </si>
   <si>
-    <t>cloud</t>
+    <t>static</t>
   </si>
   <si>
     <t>Panorama management IP type - static or cloud (for dhcp)</t>
@@ -47,7 +47,7 @@
     <t>PANORAMA_IP</t>
   </si>
   <si>
-    <t>192.168.55.8</t>
+    <t>192.168.55.161</t>
   </si>
   <si>
     <t>Panorama IP</t>
@@ -119,9 +119,6 @@
     <t>MGMT_TYPE</t>
   </si>
   <si>
-    <t>dhcp-client</t>
-  </si>
-  <si>
     <t>firewall management IP type (static or dhcp-client)</t>
   </si>
   <si>
@@ -272,7 +269,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t>include the predefined Palo Alto Networks external lists</t>
+    <t>include the predefined Palo Alto Networks external lists security rules</t>
   </si>
   <si>
     <t># set command configuration for Panorama version 8.0</t>
@@ -2612,197 +2609,197 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>46</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
         <v>54</v>
-      </c>
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
         <v>56</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>57</v>
-      </c>
-      <c r="C20" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
         <v>59</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>60</v>
-      </c>
-      <c r="C21" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
         <v>62</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>63</v>
-      </c>
-      <c r="C22" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
         <v>65</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>66</v>
-      </c>
-      <c r="C23" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
         <v>68</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>69</v>
-      </c>
-      <c r="C24" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" t="s">
         <v>71</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>72</v>
-      </c>
-      <c r="C25" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
         <v>74</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>75</v>
-      </c>
-      <c r="C26" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
         <v>77</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>78</v>
-      </c>
-      <c r="C27" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
         <v>80</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>81</v>
-      </c>
-      <c r="C28" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
         <v>83</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>84</v>
-      </c>
-      <c r="C29" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2820,27 +2817,27 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -2893,7 +2890,7 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -2910,77 +2907,77 @@
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:1">
@@ -2991,57 +2988,57 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:1">
@@ -3064,27 +3061,27 @@
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:1">
@@ -3095,177 +3092,177 @@
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="96" spans="1:1">
@@ -3282,542 +3279,542 @@
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="209" spans="1:1">
@@ -3834,62 +3831,62 @@
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="223" spans="1:1">
@@ -3906,62 +3903,62 @@
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="237" spans="1:1">
@@ -3978,62 +3975,62 @@
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="251" spans="1:1">
@@ -4050,42 +4047,42 @@
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="261" spans="1:1">
@@ -4102,1412 +4099,1412 @@
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="548" spans="1:1">
@@ -5536,227 +5533,227 @@
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="597" spans="1:1">
@@ -5779,17 +5776,17 @@
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="603" spans="1:1">
@@ -5800,67 +5797,67 @@
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="617" spans="1:1">
       <c r="A617" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="618" spans="1:1">
@@ -5889,7 +5886,7 @@
     </row>
     <row r="623" spans="1:1">
       <c r="A623" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="624" spans="1:1">
@@ -5900,7 +5897,7 @@
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="627" spans="1:1">
@@ -5929,7 +5926,7 @@
     </row>
     <row r="632" spans="1:1">
       <c r="A632" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="633" spans="1:1">
@@ -6450,257 +6447,257 @@
     </row>
     <row r="721" spans="1:1">
       <c r="A721" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="766" spans="1:1">
       <c r="A766" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="767" spans="1:1">
       <c r="A767" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="768" spans="1:1">
       <c r="A768" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="769" spans="1:1">
       <c r="A769" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="770" spans="1:1">
       <c r="A770" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="771" spans="1:1">
       <c r="A771" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rebuild for panorama snippets
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="703">
   <si>
     <t>Variable Name</t>
   </si>
@@ -47,7 +47,7 @@
     <t>PANORAMA_IP</t>
   </si>
   <si>
-    <t>192.168.55.161</t>
+    <t>192.168.55.8</t>
   </si>
   <si>
     <t>Panorama IP</t>
@@ -216,15 +216,6 @@
   </si>
   <si>
     <t>sinkhole address IPv6</t>
-  </si>
-  <si>
-    <t>INTERNET_ZONE</t>
-  </si>
-  <si>
-    <t>internet</t>
-  </si>
-  <si>
-    <t>untrust zone to filter out in reports</t>
   </si>
   <si>
     <t>EMAIL_PROFILE_GATEWAY</t>
@@ -2473,7 +2464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2789,17 +2780,6 @@
       </c>
       <c r="C28" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" t="s">
-        <v>83</v>
-      </c>
-      <c r="C29" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2817,27 +2797,27 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -2890,7 +2870,7 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -2907,77 +2887,77 @@
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:1">
@@ -2988,281 +2968,281 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57">
-        <f>SUBSTITUTE("set panorama log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
+        <f>SUBSTITUTE("set panorama log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="96" spans="1:1">
@@ -3279,542 +3259,542 @@
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="209" spans="1:1">
@@ -3831,62 +3811,62 @@
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="223" spans="1:1">
@@ -3903,62 +3883,62 @@
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="237" spans="1:1">
@@ -3975,62 +3955,62 @@
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="251" spans="1:1">
@@ -4047,42 +4027,42 @@
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="261" spans="1:1">
@@ -4099,1412 +4079,1412 @@
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="548" spans="1:1">
@@ -5533,331 +5513,331 @@
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="598" spans="1:1">
       <c r="A598">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
     </row>
     <row r="617" spans="1:1">
       <c r="A617" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
     </row>
     <row r="618" spans="1:1">
@@ -5886,7 +5866,7 @@
     </row>
     <row r="623" spans="1:1">
       <c r="A623" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="624" spans="1:1">
@@ -5897,7 +5877,7 @@
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
     </row>
     <row r="627" spans="1:1">
@@ -5926,7 +5906,7 @@
     </row>
     <row r="632" spans="1:1">
       <c r="A632" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
     </row>
     <row r="633" spans="1:1">
@@ -6447,257 +6427,257 @@
     </row>
     <row r="721" spans="1:1">
       <c r="A721" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="766" spans="1:1">
       <c r="A766" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="767" spans="1:1">
       <c r="A767" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="768" spans="1:1">
       <c r="A768" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
     </row>
     <row r="769" spans="1:1">
       <c r="A769" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="770" spans="1:1">
       <c r="A770" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="771" spans="1:1">
       <c r="A771" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating IronSkillet with smaller snippets
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="722">
   <si>
     <t>Variable Name</t>
   </si>
@@ -332,9 +332,6 @@
     <t>set mgt-config password-complexity new-password-differs-by-characters 3</t>
   </si>
   <si>
-    <t>set mgt-config password-complexity password-change expiration-period 90</t>
-  </si>
-  <si>
     <t># additional base Panorama system configuration</t>
   </si>
   <si>
@@ -1313,7 +1310,7 @@
     <t>set shared profiles url-filtering Outbound-URL credential-enforcement log-severity high</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Outbound-URL credential-enforcement block [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
+    <t>set shared profiles url-filtering Outbound-URL credential-enforcement block [ Black-List White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Outbound-URL log-http-hdr-user-agent yes</t>
@@ -1325,10 +1322,10 @@
     <t>set shared profiles url-filtering Outbound-URL log-http-hdr-xff yes</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Outbound-URL alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting White-List  ]</t>
-  </si>
-  <si>
-    <t>set shared profiles url-filtering Outbound-URL block [ command-and-control hacking malware phishing Black-List ]</t>
+    <t>set shared profiles url-filtering Outbound-URL alert [ White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+  </si>
+  <si>
+    <t>set shared profiles url-filtering Outbound-URL block [ Black-List command-and-control grayware hacking malware phishing ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement mode ip-user</t>
@@ -1337,10 +1334,10 @@
     <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement log-severity medium</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
-  </si>
-  <si>
-    <t>set shared profiles url-filtering Alert-Only-URL alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
+    <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement alert [ Black-List White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+  </si>
+  <si>
+    <t>set shared profiles url-filtering Alert-Only-URL alert [ Black-List White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Exception-URL credential-enforcement mode ip-user</t>
@@ -1349,7 +1346,7 @@
     <t>set shared profiles url-filtering Exception-URL credential-enforcement log-severity high</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Exception-URL credential-enforcement block [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
+    <t>set shared profiles url-filtering Exception-URL credential-enforcement block [ Black-List White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Exception-URL log-http-hdr-user-agent yes</t>
@@ -1361,10 +1358,10 @@
     <t>set shared profiles url-filtering Exception-URL log-http-hdr-xff yes</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Exception-URL alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting White-List ]</t>
-  </si>
-  <si>
-    <t>set shared profiles url-filtering Exception-URL block [ command-and-control hacking malware phishing Black-List ]</t>
+    <t>set shared profiles url-filtering Exception-URL alert [ White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+  </si>
+  <si>
+    <t>set shared profiles url-filtering Exception-URL block [ Black-List command-and-control grayware hacking malware phishing ]</t>
   </si>
   <si>
     <t>set shared profiles wildfire-analysis Outbound-WF rules Forward-All application any</t>
@@ -1767,9 +1764,6 @@
   </si>
   <si>
     <t>set template iron-skillet config mgt-config password-complexity new-password-differs-by-characters 3</t>
-  </si>
-  <si>
-    <t>set template iron-skillet config mgt-config password-complexity password-change expiration-period 90</t>
   </si>
   <si>
     <t>set template iron-skillet config deviceconfig system update-schedule statistics-service application-reports yes</t>
@@ -2874,7 +2868,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A788"/>
+  <dimension ref="A2:A786"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3030,8 +3024,8 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3101,14 +3095,14 @@
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" t="s">
+      <c r="A48">
+        <f>SUBSTITUTE("set deviceconfig system config-bundle-export-schedule Recommended_Config_Export protocol scp hostname {{ CONFIG_EXPORT_IP }}", "{{ CONFIG_EXPORT_IP }}", 'values'!B7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49">
-        <f>SUBSTITUTE("set deviceconfig system config-bundle-export-schedule Recommended_Config_Export protocol scp hostname {{ CONFIG_EXPORT_IP }}", "{{ CONFIG_EXPORT_IP }}", 'values'!B7)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:1">
@@ -3147,14 +3141,14 @@
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" t="s">
+      <c r="A57">
+        <f>SUBSTITUTE("set deviceconfig setting management api key lifetime {{ API_KEY_LIFETIME }}", "{{ API_KEY_LIFETIME }}", 'values'!B29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58">
-        <f>SUBSTITUTE("set deviceconfig setting management api key lifetime {{ API_KEY_LIFETIME }}", "{{ API_KEY_LIFETIME }}", 'values'!B29)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:1">
@@ -3177,8 +3171,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
-      <c r="A63" t="s">
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3188,26 +3182,26 @@
       </c>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" t="s">
-        <v>134</v>
+      <c r="A66">
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
+        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69">
-        <f>SUBSTITUTE("set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
-        <v>0</v>
+      <c r="A69" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="70" spans="1:1">
@@ -3231,14 +3225,14 @@
       </c>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" t="s">
+      <c r="A74">
+        <f>SUBSTITUTE("set panorama log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75">
-        <f>SUBSTITUTE("set panorama log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:1">
@@ -3381,13 +3375,13 @@
         <v>167</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
-      <c r="A104" t="s">
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
-      <c r="A107" t="s">
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3412,20 +3406,20 @@
       </c>
     </row>
     <row r="113" spans="1:1">
-      <c r="A113" t="s">
-        <v>174</v>
+      <c r="A113">
+        <f>SUBSTITUTE("set shared address Sinkhole-IPv4 fqdn {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114">
-        <f>SUBSTITUTE("set shared address Sinkhole-IPv4 fqdn {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1">
-      <c r="A115">
         <f>SUBSTITUTE("set shared address Sinkhole-IPv6 ip-netmask {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="117" spans="1:1">
@@ -3533,8 +3527,8 @@
         <v>195</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
-      <c r="A138" t="s">
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
         <v>196</v>
       </c>
     </row>
@@ -3623,8 +3617,8 @@
         <v>213</v>
       </c>
     </row>
-    <row r="157" spans="1:1">
-      <c r="A157" t="s">
+    <row r="158" spans="1:1">
+      <c r="A158" t="s">
         <v>214</v>
       </c>
     </row>
@@ -3984,20 +3978,20 @@
       </c>
     </row>
     <row r="230" spans="1:1">
-      <c r="A230" t="s">
-        <v>286</v>
+      <c r="A230">
+        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231">
-        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="232" spans="1:1">
-      <c r="A232">
-        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A232" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="233" spans="1:1">
@@ -4066,20 +4060,20 @@
       </c>
     </row>
     <row r="246" spans="1:1">
-      <c r="A246" t="s">
-        <v>300</v>
+      <c r="A246">
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="248" spans="1:1">
-      <c r="A248">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A248" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="249" spans="1:1">
@@ -4148,20 +4142,20 @@
       </c>
     </row>
     <row r="262" spans="1:1">
-      <c r="A262" t="s">
-        <v>314</v>
+      <c r="A262">
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="264" spans="1:1">
-      <c r="A264">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A264" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="265" spans="1:1">
@@ -4230,20 +4224,20 @@
       </c>
     </row>
     <row r="278" spans="1:1">
-      <c r="A278" t="s">
-        <v>328</v>
+      <c r="A278">
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="280" spans="1:1">
-      <c r="A280">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A280" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="281" spans="1:1">
@@ -4287,20 +4281,20 @@
       </c>
     </row>
     <row r="289" spans="1:1">
-      <c r="A289" t="s">
-        <v>337</v>
+      <c r="A289">
+        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290">
-        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="291" spans="1:1">
-      <c r="A291">
-        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A291" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="292" spans="1:1">
@@ -4938,8 +4932,8 @@
         <v>464</v>
       </c>
     </row>
-    <row r="419" spans="1:1">
-      <c r="A419" t="s">
+    <row r="420" spans="1:1">
+      <c r="A420" t="s">
         <v>465</v>
       </c>
     </row>
@@ -5083,8 +5077,8 @@
         <v>493</v>
       </c>
     </row>
-    <row r="449" spans="1:1">
-      <c r="A449" t="s">
+    <row r="450" spans="1:1">
+      <c r="A450" t="s">
         <v>494</v>
       </c>
     </row>
@@ -5468,8 +5462,8 @@
         <v>570</v>
       </c>
     </row>
-    <row r="527" spans="1:1">
-      <c r="A527" t="s">
+    <row r="528" spans="1:1">
+      <c r="A528" t="s">
         <v>571</v>
       </c>
     </row>
@@ -5484,20 +5478,20 @@
       </c>
     </row>
     <row r="531" spans="1:1">
-      <c r="A531" t="s">
-        <v>574</v>
+      <c r="A531">
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532">
-        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="533" spans="1:1">
-      <c r="A533">
-        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
-        <v>0</v>
+      <c r="A533" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="534" spans="1:1">
@@ -5636,37 +5630,37 @@
       </c>
     </row>
     <row r="561" spans="1:1">
-      <c r="A561" t="s">
-        <v>602</v>
+      <c r="A561">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="562" spans="1:1">
-      <c r="A562" t="s">
-        <v>603</v>
+      <c r="A562">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B20)</f>
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="565" spans="1:1">
-      <c r="A565">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B16)</f>
-        <v>0</v>
+      <c r="A565" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="566" spans="1:1">
-      <c r="A566">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B17)</f>
-        <v>0</v>
+      <c r="A566" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="567" spans="1:1">
@@ -5915,31 +5909,31 @@
       </c>
     </row>
     <row r="616" spans="1:1">
-      <c r="A616" t="s">
-        <v>653</v>
+      <c r="A616">
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="617" spans="1:1">
-      <c r="A617" t="s">
-        <v>654</v>
+      <c r="A617">
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="618" spans="1:1">
       <c r="A618">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="619" spans="1:1">
-      <c r="A619">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
-        <v>0</v>
+      <c r="A619" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="620" spans="1:1">
-      <c r="A620">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
-        <v>0</v>
+      <c r="A620" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="621" spans="1:1">
@@ -5948,19 +5942,19 @@
       </c>
     </row>
     <row r="622" spans="1:1">
-      <c r="A622" t="s">
-        <v>656</v>
+      <c r="A622">
+        <f>SUBSTITUTE("set template iron-skillet config shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="623" spans="1:1">
       <c r="A623" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="624" spans="1:1">
+      <c r="A624" t="s">
         <v>657</v>
-      </c>
-    </row>
-    <row r="624" spans="1:1">
-      <c r="A624">
-        <f>SUBSTITUTE("set template iron-skillet config shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="625" spans="1:1">
@@ -6008,592 +6002,592 @@
         <v>666</v>
       </c>
     </row>
-    <row r="634" spans="1:1">
-      <c r="A634" t="s">
-        <v>667</v>
-      </c>
-    </row>
     <row r="635" spans="1:1">
       <c r="A635" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="636" spans="1:1">
+      <c r="A636" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="637" spans="1:1">
-      <c r="A637" t="s">
-        <v>669</v>
+      <c r="A637">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="638" spans="1:1">
-      <c r="A638" t="s">
-        <v>670</v>
+      <c r="A638">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="640" spans="1:1">
-      <c r="A640">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B11), "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="641" spans="1:1">
-      <c r="A641">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B11), "{{ STACK }}", 'values'!B9)</f>
+      <c r="A641" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="642" spans="1:1">
+      <c r="A642">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="643" spans="1:1">
-      <c r="A643" t="s">
-        <v>671</v>
+      <c r="A643">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="646" spans="1:1">
-      <c r="A646">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="647" spans="1:1">
-      <c r="A647">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B9)</f>
+      <c r="A647" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="648" spans="1:1">
+      <c r="A648">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="649" spans="1:1">
-      <c r="A649" t="s">
-        <v>672</v>
+      <c r="A649">
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B13), "{{ STACK }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B14), "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B13), "{{ STACK }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="652" spans="1:1">
-      <c r="A652">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B14), "{{ STACK }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B15), "{{ STACK }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B15), "{{ STACK }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="654" spans="1:1">
+      <c r="A654">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="659" spans="1:1">
       <c r="A659">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="664" spans="1:1">
       <c r="A664">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="665" spans="1:1">
       <c r="A665">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="670" spans="1:1">
       <c r="A670">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="672" spans="1:1">
       <c r="A672">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="673" spans="1:1">
       <c r="A673">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="675" spans="1:1">
       <c r="A675">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="676" spans="1:1">
       <c r="A676">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="677" spans="1:1">
       <c r="A677">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="678" spans="1:1">
       <c r="A678">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="679" spans="1:1">
       <c r="A679">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="680" spans="1:1">
       <c r="A680">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="681" spans="1:1">
       <c r="A681">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="682" spans="1:1">
       <c r="A682">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="683" spans="1:1">
       <c r="A683">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="684" spans="1:1">
       <c r="A684">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="685" spans="1:1">
       <c r="A685">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="686" spans="1:1">
       <c r="A686">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="687" spans="1:1">
       <c r="A687">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="688" spans="1:1">
       <c r="A688">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="689" spans="1:1">
       <c r="A689">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="690" spans="1:1">
       <c r="A690">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="691" spans="1:1">
       <c r="A691">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="692" spans="1:1">
       <c r="A692">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="693" spans="1:1">
       <c r="A693">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="694" spans="1:1">
       <c r="A694">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="695" spans="1:1">
       <c r="A695">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="696" spans="1:1">
       <c r="A696">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="697" spans="1:1">
       <c r="A697">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="698" spans="1:1">
       <c r="A698">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="699" spans="1:1">
       <c r="A699">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="700" spans="1:1">
       <c r="A700">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="701" spans="1:1">
       <c r="A701">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="702" spans="1:1">
       <c r="A702">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="703" spans="1:1">
       <c r="A703">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="704" spans="1:1">
       <c r="A704">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="705" spans="1:1">
       <c r="A705">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="706" spans="1:1">
       <c r="A706">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="707" spans="1:1">
       <c r="A707">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="708" spans="1:1">
       <c r="A708">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="709" spans="1:1">
       <c r="A709">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="710" spans="1:1">
       <c r="A710">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="711" spans="1:1">
       <c r="A711">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="712" spans="1:1">
       <c r="A712">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="713" spans="1:1">
       <c r="A713">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="714" spans="1:1">
       <c r="A714">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="715" spans="1:1">
       <c r="A715">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="716" spans="1:1">
       <c r="A716">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="717" spans="1:1">
       <c r="A717">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="718" spans="1:1">
       <c r="A718">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="719" spans="1:1">
       <c r="A719">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="720" spans="1:1">
       <c r="A720">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="721" spans="1:1">
       <c r="A721">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="735" spans="1:1">
-      <c r="A735">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" email-profile Sample_Email_Profile", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="736" spans="1:1">
-      <c r="A736">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" email-profile Sample_Email_Profile", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
-        <v>0</v>
+      <c r="A736" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="737" spans="1:1">
+      <c r="A737" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="738" spans="1:1">
@@ -6839,16 +6833,6 @@
     <row r="786" spans="1:1">
       <c r="A786" t="s">
         <v>721</v>
-      </c>
-    </row>
-    <row r="787" spans="1:1">
-      <c r="A787" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="788" spans="1:1">
-      <c r="A788" t="s">
-        <v>723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with new url categories
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -1253,7 +1253,7 @@
     <t>set shared profiles url-filtering Outbound-URL credential-enforcement log-severity high</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Outbound-URL credential-enforcement block [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
+    <t>set shared profiles url-filtering Outbound-URL credential-enforcement block [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Outbound-URL log-http-hdr-user-agent yes</t>
@@ -1271,7 +1271,7 @@
     <t>set shared profiles url-filtering Outbound-URL alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting White-List ]</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Outbound-URL block [ command-and-control hacking malware phishing Black-List ]</t>
+    <t>set shared profiles url-filtering Outbound-URL block [ command-and-control grayware hacking malware phishing Black-List ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement mode ip-user</t>
@@ -1280,13 +1280,13 @@
     <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement log-severity medium</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
+    <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Alert-Only-URL action block</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Alert-Only-URL alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
+    <t>set shared profiles url-filtering Alert-Only-URL alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Exception-URL credential-enforcement mode ip-user</t>
@@ -1295,7 +1295,7 @@
     <t>set shared profiles url-filtering Exception-URL credential-enforcement log-severity high</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Exception-URL credential-enforcement block [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
+    <t>set shared profiles url-filtering Exception-URL credential-enforcement block [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Exception-URL log-http-hdr-user-agent yes</t>
@@ -1313,7 +1313,7 @@
     <t>set shared profiles url-filtering Exception-URL alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting White-List ]</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Exception-URL block [ command-and-control hacking malware phishing Black-List ]</t>
+    <t>set shared profiles url-filtering Exception-URL block [ command-and-control grayware hacking malware phishing Black-List ]</t>
   </si>
   <si>
     <t>set shared profiles wildfire-analysis Outbound-WF rules Forward-All application any</t>
@@ -5986,7 +5986,7 @@
     </row>
     <row r="641" spans="1:1">
       <c r="A641">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
@@ -6046,7 +6046,7 @@
     </row>
     <row r="651" spans="1:1">
       <c r="A651">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update url categories in reports
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -6120,7 +6120,7 @@
     </row>
     <row r="658" spans="1:1">
       <c r="A658">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
@@ -6180,7 +6180,7 @@
     </row>
     <row r="668" spans="1:1">
       <c r="A668">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add grayware to reports
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -6120,7 +6120,7 @@
     </row>
     <row r="658" spans="1:1">
       <c r="A658">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
@@ -6180,7 +6180,7 @@
     </row>
     <row r="668" spans="1:1">
       <c r="A668">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update full configs and spreadsheet
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -1865,16 +1865,16 @@
     <t>set template iron-skillet config deviceconfig setting management auto-acquire-commit-lock yes</t>
   </si>
   <si>
-    <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit pe size-limit 10</t>
+    <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit pe size-limit 16</t>
   </si>
   <si>
     <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit apk size-limit 30</t>
   </si>
   <si>
-    <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit pdf size-limit 1000</t>
-  </si>
-  <si>
-    <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit ms-office size-limit 2000</t>
+    <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit pdf size-limit 3072</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit ms-office size-limit 16384</t>
   </si>
   <si>
     <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit jar size-limit 5</t>
@@ -1883,13 +1883,13 @@
     <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit flash size-limit 5</t>
   </si>
   <si>
-    <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit MacOSX size-limit 1</t>
-  </si>
-  <si>
-    <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit archive size-limit 10</t>
-  </si>
-  <si>
-    <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit linux size-limit 2</t>
+    <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit MacOSX size-limit 10</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit archive size-limit 50</t>
+  </si>
+  <si>
+    <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit linux size-limit 50</t>
   </si>
   <si>
     <t>set template iron-skillet config deviceconfig setting wildfire file-size-limit script size-limit 2000</t>

</xml_diff>

<commit_message>
build spreadsheet and full xml
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="769">
   <si>
     <t>Variable Name</t>
   </si>
@@ -380,7 +380,7 @@
     <t>set deviceconfig setting management auto-acquire-commit-lock yes</t>
   </si>
   <si>
-    <t># Panorama log settings</t>
+    <t># Panorama platform log settings</t>
   </si>
   <si>
     <t>set panorama log-settings email Sample_Email_Profile server Sample_Email_Profile display-name Panorama</t>
@@ -425,72 +425,6 @@
     <t>set panorama log-settings userid match-list User-ID_Log_Forwarding filter ""All Logs""</t>
   </si>
   <si>
-    <t>set panorama log-settings threat match-list Threat_Log_Forwarding send-syslog Sample_Syslog_Profile</t>
-  </si>
-  <si>
-    <t>set panorama log-settings threat match-list Threat_Log_Forwarding filter ""All Logs""</t>
-  </si>
-  <si>
-    <t>set panorama log-settings data match-list Data_Log_Forwarding send-syslog Sample_Syslog_Profile</t>
-  </si>
-  <si>
-    <t>set panorama log-settings data match-list Data_Log_Forwarding filter ""All Logs""</t>
-  </si>
-  <si>
-    <t>set panorama log-settings wildfire match-list WildFire_Malicious send-email Sample_Email_Profile</t>
-  </si>
-  <si>
-    <t>set panorama log-settings wildfire match-list WildFire_Malicious filter ""(verdict eq malicious) or (verdict eq phishing)""</t>
-  </si>
-  <si>
-    <t>set panorama log-settings wildfire match-list WildFire_Log_Forwarding send-syslog Sample_Syslog_Profile</t>
-  </si>
-  <si>
-    <t>set panorama log-settings wildfire match-list WildFire_Log_Forwarding filter ""All Logs""</t>
-  </si>
-  <si>
-    <t>set panorama log-settings tunnel match-list Tunnel_Log_Forwarding send-syslog Sample_Syslog_Profile</t>
-  </si>
-  <si>
-    <t>set panorama log-settings tunnel match-list Tunnel_Log_Forwarding filter ""All Logs""</t>
-  </si>
-  <si>
-    <t>set panorama log-settings auth match-list Auth_Log_Forwarding send-syslog Sample_Syslog_Profile</t>
-  </si>
-  <si>
-    <t>set panorama log-settings auth match-list Auth_Log_Forwarding filter ""All Logs""</t>
-  </si>
-  <si>
-    <t>set panorama log-settings correlation match-list Correlation_Critical_Email send-email Sample_Email_Profile</t>
-  </si>
-  <si>
-    <t>set panorama log-settings correlation match-list Correlation_Critical_Email filter ""(severity geq medium)""</t>
-  </si>
-  <si>
-    <t>set panorama log-settings correlation match-list Correlation_Log_Forwarding send-syslog Sample_Syslog_Profile</t>
-  </si>
-  <si>
-    <t>set panorama log-settings correlation match-list Correlation_Log_Forwarding filter ""All Logs""</t>
-  </si>
-  <si>
-    <t>set panorama log-settings traffic match-list Traffic_Log_Forwarding send-syslog Sample_Syslog_Profile</t>
-  </si>
-  <si>
-    <t>set panorama log-settings traffic match-list Traffic_Log_Forwarding filter ""All Logs""</t>
-  </si>
-  <si>
-    <t>set panorama log-settings hipmatch match-list HIP_Log_Forwarding send-syslog Sample_Syslog_Profile</t>
-  </si>
-  <si>
-    <t>set panorama log-settings hipmatch match-list HIP_Log_Forwarding filter ""All Logs""</t>
-  </si>
-  <si>
-    <t>set panorama log-settings url match-list URL_Log_Forwarding send-syslog Sample_Syslog_Profile</t>
-  </si>
-  <si>
-    <t>set panorama log-settings url match-list URL_Log_Forwarding filter ""All Logs""</t>
-  </si>
-  <si>
     <t># shared values used by device-groups and template-stacks</t>
   </si>
   <si>
@@ -509,7 +443,7 @@
     <t>set shared tag iron-skillet-version comments ""version 0.0.1 for 10.0: version of this IronSkillet template file""</t>
   </si>
   <si>
-    <t># shared log settings</t>
+    <t># shared log settings for the NGFW</t>
   </si>
   <si>
     <t>set shared log-settings profiles default match-list Traffic_Log_Forwarding log-type traffic</t>
@@ -1313,12 +1247,6 @@
     <t>set shared profiles spyware Exception-AS botnet-domains lists default-paloalto-dns action sinkhole</t>
   </si>
   <si>
-    <t>set shared profiles spyware Exception-AS botnet-domains lists default-paloalto-cloud packet-capture single-packet</t>
-  </si>
-  <si>
-    <t>set shared profiles spyware Exception-AS botnet-domains lists default-paloalto-cloud action sinkhole</t>
-  </si>
-  <si>
     <t>set shared profiles vulnerability Outbound-VP rules Block-Critical-High-Medium action reset-both</t>
   </si>
   <si>
@@ -2000,7 +1928,7 @@
     <t>set template iron-skillet config deviceconfig system update-schedule anti-virus recurring hourly action download-and-install</t>
   </si>
   <si>
-    <t>set template iron-skillet config deviceconfig system update-schedule wildfire recurring every-min action download-and-install</t>
+    <t>set template iron-skillet config deviceconfig system update-schedule wildfire recurring real-time</t>
   </si>
   <si>
     <t>set template iron-skillet config deviceconfig system update-schedule global-protect-datafile recurring hourly at 40</t>
@@ -2351,7 +2279,7 @@
     <t>set log-collector-group Default_Collector_Group log-settings correlation match-list Email_Critical_Correlations filter ""(severity geq medium)""</t>
   </si>
   <si>
-    <t>set log-collector-group Default_Collector_Group log-settings correlation match-list Email_Critical_Correlations description ""Emal all Critical Correlation Events""</t>
+    <t>set log-collector-group Default_Collector_Group log-settings correlation match-list Email_Critical_Correlations description ""Email all Critical Correlation Events""</t>
   </si>
   <si>
     <t>set log-collector-group Default_Collector_Group log-settings correlation match-list Syslog_Correlation_Logs send-syslog Sample_Syslog_Profile</t>
@@ -3037,7 +2965,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A864"/>
+  <dimension ref="A2:A842"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3439,118 +3367,118 @@
         <v>135</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
-      <c r="A83" t="s">
-        <v>136</v>
-      </c>
-    </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>157</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3674,18 +3602,18 @@
         <v>182</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
-      <c r="A134" t="s">
-        <v>183</v>
-      </c>
-    </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
         <v>185</v>
       </c>
     </row>
@@ -3784,3598 +3712,3478 @@
         <v>204</v>
       </c>
     </row>
+    <row r="157" spans="1:1">
+      <c r="A157" t="s">
+        <v>205</v>
+      </c>
+    </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="252" spans="1:1">
       <c r="A252" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="257" spans="1:1">
-      <c r="A257" t="s">
-        <v>304</v>
+      <c r="A257">
+        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="258" spans="1:1">
-      <c r="A258" t="s">
-        <v>305</v>
+      <c r="A258">
+        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1">
+      <c r="A280" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="280" spans="1:1">
-      <c r="A280">
-        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="281" spans="1:1">
-      <c r="A281">
-        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A281" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="286" spans="1:1">
-      <c r="A286" t="s">
-        <v>331</v>
+      <c r="A286">
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="287" spans="1:1">
-      <c r="A287" t="s">
-        <v>332</v>
+      <c r="A287">
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1">
+      <c r="A309" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="309" spans="1:1">
-      <c r="A309">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="310" spans="1:1">
-      <c r="A310">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A310" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="315" spans="1:1">
-      <c r="A315" t="s">
-        <v>358</v>
+      <c r="A315">
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="316" spans="1:1">
-      <c r="A316" t="s">
-        <v>359</v>
+      <c r="A316">
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1">
+      <c r="A338" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="338" spans="1:1">
-      <c r="A338">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="339" spans="1:1">
-      <c r="A339">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A339" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="344" spans="1:1">
-      <c r="A344" t="s">
-        <v>385</v>
+      <c r="A344">
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="345" spans="1:1">
-      <c r="A345" t="s">
-        <v>386</v>
+      <c r="A345">
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1">
+      <c r="A367" t="s">
         <v>407</v>
-      </c>
-    </row>
-    <row r="367" spans="1:1">
-      <c r="A367">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="369" spans="1:1">
-      <c r="A369" t="s">
-        <v>408</v>
+      <c r="A369">
+        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="372" spans="1:1">
-      <c r="A372" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="373" spans="1:1">
-      <c r="A373" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="374" spans="1:1">
-      <c r="A374" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="391" spans="1:1">
-      <c r="A391">
-        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A391" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="392" spans="1:1">
-      <c r="A392">
-        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A392" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="421" spans="1:1">
       <c r="A421" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="463" spans="1:1">
-      <c r="A463" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>521</v>
+        <v>518</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1">
+      <c r="A485" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="506" spans="1:1">
-      <c r="A506" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>563</v>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="528" spans="1:1">
+      <c r="A528" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="529" spans="1:1">
       <c r="A529" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="536" spans="1:1">
-      <c r="A536" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="548" spans="1:1">
       <c r="A548" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="549" spans="1:1">
       <c r="A549" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="550" spans="1:1">
       <c r="A550" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="551" spans="1:1">
       <c r="A551" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>592</v>
+        <v>589</v>
+      </c>
+    </row>
+    <row r="558" spans="1:1">
+      <c r="A558" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="588" spans="1:1">
-      <c r="A588" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="592" spans="1:1">
-      <c r="A592" t="s">
-        <v>626</v>
+      <c r="A592">
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="593" spans="1:1">
-      <c r="A593" t="s">
-        <v>627</v>
+      <c r="A593">
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>643</v>
+        <v>638</v>
+      </c>
+    </row>
+    <row r="610" spans="1:1">
+      <c r="A610" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614">
-        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="615" spans="1:1">
       <c r="A615">
-        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="616" spans="1:1">
-      <c r="A616" t="s">
-        <v>647</v>
+      <c r="A616">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="617" spans="1:1">
-      <c r="A617" t="s">
-        <v>648</v>
+      <c r="A617">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="618" spans="1:1">
       <c r="A618" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
     </row>
     <row r="619" spans="1:1">
       <c r="A619" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
     </row>
     <row r="620" spans="1:1">
       <c r="A620" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
     </row>
     <row r="621" spans="1:1">
       <c r="A621" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
     </row>
     <row r="622" spans="1:1">
       <c r="A622" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
     </row>
     <row r="623" spans="1:1">
       <c r="A623" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
     </row>
     <row r="624" spans="1:1">
       <c r="A624" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
     </row>
     <row r="625" spans="1:1">
       <c r="A625" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
     </row>
     <row r="627" spans="1:1">
       <c r="A627" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
     </row>
     <row r="628" spans="1:1">
       <c r="A628" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
     </row>
     <row r="629" spans="1:1">
       <c r="A629" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
     </row>
     <row r="630" spans="1:1">
       <c r="A630" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
     </row>
     <row r="631" spans="1:1">
       <c r="A631" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
     </row>
     <row r="632" spans="1:1">
       <c r="A632" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
     </row>
     <row r="633" spans="1:1">
       <c r="A633" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
     </row>
     <row r="634" spans="1:1">
       <c r="A634" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="635" spans="1:1">
       <c r="A635" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
     </row>
     <row r="636" spans="1:1">
-      <c r="A636">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B18)</f>
-        <v>0</v>
+      <c r="A636" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="637" spans="1:1">
-      <c r="A637">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B19)</f>
-        <v>0</v>
+      <c r="A637" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="638" spans="1:1">
-      <c r="A638">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
-        <v>0</v>
+      <c r="A638" t="s">
+        <v>663</v>
       </c>
     </row>
     <row r="639" spans="1:1">
-      <c r="A639">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
-        <v>0</v>
+      <c r="A639" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="641" spans="1:1">
       <c r="A641" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="642" spans="1:1">
       <c r="A642" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="643" spans="1:1">
       <c r="A643" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="647" spans="1:1">
       <c r="A647" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="648" spans="1:1">
       <c r="A648" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="649" spans="1:1">
       <c r="A649" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="654" spans="1:1">
       <c r="A654" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="659" spans="1:1">
       <c r="A659" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="664" spans="1:1">
       <c r="A664" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="665" spans="1:1">
-      <c r="A665" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="670" spans="1:1">
       <c r="A670" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="672" spans="1:1">
       <c r="A672" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="673" spans="1:1">
       <c r="A673" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="675" spans="1:1">
       <c r="A675" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
     </row>
     <row r="676" spans="1:1">
       <c r="A676" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="677" spans="1:1">
       <c r="A677" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="678" spans="1:1">
       <c r="A678" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="679" spans="1:1">
       <c r="A679" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="680" spans="1:1">
       <c r="A680" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="681" spans="1:1">
       <c r="A681" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="682" spans="1:1">
       <c r="A682" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
     </row>
     <row r="683" spans="1:1">
       <c r="A683" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
     </row>
     <row r="684" spans="1:1">
       <c r="A684" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
     </row>
     <row r="685" spans="1:1">
       <c r="A685" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
     <row r="686" spans="1:1">
       <c r="A686" t="s">
-        <v>713</v>
+        <v>710</v>
+      </c>
+    </row>
+    <row r="687" spans="1:1">
+      <c r="A687" t="s">
+        <v>711</v>
       </c>
     </row>
     <row r="688" spans="1:1">
       <c r="A688" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="689" spans="1:1">
       <c r="A689" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="690" spans="1:1">
-      <c r="A690" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
     </row>
     <row r="691" spans="1:1">
       <c r="A691" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
     </row>
     <row r="692" spans="1:1">
       <c r="A692" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
     </row>
     <row r="693" spans="1:1">
-      <c r="A693" t="s">
-        <v>719</v>
+      <c r="A693">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="694" spans="1:1">
-      <c r="A694" t="s">
-        <v>720</v>
+      <c r="A694">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="695" spans="1:1">
-      <c r="A695" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="696" spans="1:1">
-      <c r="A696" t="s">
-        <v>722</v>
+      <c r="A695">
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B10), "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="697" spans="1:1">
       <c r="A697" t="s">
-        <v>723</v>
+        <v>716</v>
       </c>
     </row>
     <row r="698" spans="1:1">
-      <c r="A698" t="s">
-        <v>724</v>
+      <c r="A698">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="699" spans="1:1">
-      <c r="A699" t="s">
-        <v>725</v>
+      <c r="A699">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="700" spans="1:1">
-      <c r="A700" t="s">
-        <v>726</v>
+      <c r="A700">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="701" spans="1:1">
-      <c r="A701" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="702" spans="1:1">
-      <c r="A702" t="s">
-        <v>728</v>
+      <c r="A701">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="703" spans="1:1">
       <c r="A703" t="s">
-        <v>729</v>
+        <v>717</v>
       </c>
     </row>
     <row r="704" spans="1:1">
-      <c r="A704" t="s">
-        <v>730</v>
+      <c r="A704">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="705" spans="1:1">
-      <c r="A705" t="s">
-        <v>731</v>
+      <c r="A705">
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B12), "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="706" spans="1:1">
-      <c r="A706" t="s">
-        <v>732</v>
+      <c r="A706">
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B13), "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="707" spans="1:1">
-      <c r="A707" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="708" spans="1:1">
-      <c r="A708" t="s">
-        <v>734</v>
+      <c r="A707">
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B14), "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="709" spans="1:1">
-      <c r="A709" t="s">
-        <v>735</v>
+      <c r="A709">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="710" spans="1:1">
-      <c r="A710" t="s">
-        <v>736</v>
+      <c r="A710">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="711" spans="1:1">
-      <c r="A711" t="s">
-        <v>737</v>
+      <c r="A711">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="712" spans="1:1">
+      <c r="A712">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="713" spans="1:1">
-      <c r="A713" t="s">
-        <v>738</v>
+      <c r="A713">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="714" spans="1:1">
-      <c r="A714" t="s">
-        <v>739</v>
+      <c r="A714">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="715" spans="1:1">
       <c r="A715">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="716" spans="1:1">
       <c r="A716">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="717" spans="1:1">
       <c r="A717">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B10), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="718" spans="1:1">
+      <c r="A718">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="719" spans="1:1">
-      <c r="A719" t="s">
-        <v>740</v>
+      <c r="A719">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="720" spans="1:1">
       <c r="A720">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="721" spans="1:1">
       <c r="A721">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="724" spans="1:1">
+      <c r="A724">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="725" spans="1:1">
-      <c r="A725" t="s">
-        <v>741</v>
+      <c r="A725">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B12), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B13), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B14), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="730" spans="1:1">
+      <c r="A730">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="766" spans="1:1">
       <c r="A766">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="767" spans="1:1">
       <c r="A767">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="768" spans="1:1">
       <c r="A768">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="769" spans="1:1">
       <c r="A769">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="770" spans="1:1">
       <c r="A770">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="771" spans="1:1">
       <c r="A771">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="772" spans="1:1">
       <c r="A772">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="773" spans="1:1">
       <c r="A773">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="774" spans="1:1">
       <c r="A774">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="775" spans="1:1">
       <c r="A775">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="776" spans="1:1">
       <c r="A776">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="777" spans="1:1">
       <c r="A777">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="778" spans="1:1">
       <c r="A778">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="779" spans="1:1">
       <c r="A779">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="780" spans="1:1">
       <c r="A780">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="781" spans="1:1">
       <c r="A781">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="782" spans="1:1">
       <c r="A782">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="783" spans="1:1">
       <c r="A783">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="784" spans="1:1">
       <c r="A784">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="785" spans="1:1">
       <c r="A785">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="786" spans="1:1">
       <c r="A786">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="787" spans="1:1">
       <c r="A787">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="788" spans="1:1">
       <c r="A788">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="789" spans="1:1">
       <c r="A789">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="790" spans="1:1">
       <c r="A790">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="791" spans="1:1">
-      <c r="A791">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" email-profile Sample_Email_Profile", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="792" spans="1:1">
-      <c r="A792">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A792" t="s">
+        <v>718</v>
       </c>
     </row>
     <row r="793" spans="1:1">
-      <c r="A793">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A793" t="s">
+        <v>719</v>
       </c>
     </row>
     <row r="794" spans="1:1">
-      <c r="A794">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A794" t="s">
+        <v>720</v>
       </c>
     </row>
     <row r="795" spans="1:1">
-      <c r="A795">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A795" t="s">
+        <v>721</v>
       </c>
     </row>
     <row r="796" spans="1:1">
-      <c r="A796">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A796" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="797" spans="1:1">
-      <c r="A797">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A797" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="798" spans="1:1">
-      <c r="A798">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A798" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="799" spans="1:1">
-      <c r="A799">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A799" t="s">
+        <v>725</v>
       </c>
     </row>
     <row r="800" spans="1:1">
-      <c r="A800">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A800" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="801" spans="1:1">
-      <c r="A801">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A801" t="s">
+        <v>727</v>
       </c>
     </row>
     <row r="802" spans="1:1">
-      <c r="A802">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A802" t="s">
+        <v>728</v>
       </c>
     </row>
     <row r="803" spans="1:1">
-      <c r="A803">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A803" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="804" spans="1:1">
-      <c r="A804">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A804" t="s">
+        <v>730</v>
       </c>
     </row>
     <row r="805" spans="1:1">
-      <c r="A805">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A805" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="806" spans="1:1">
-      <c r="A806">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A806" t="s">
+        <v>732</v>
       </c>
     </row>
     <row r="807" spans="1:1">
-      <c r="A807">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A807" t="s">
+        <v>733</v>
       </c>
     </row>
     <row r="808" spans="1:1">
-      <c r="A808">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A808" t="s">
+        <v>734</v>
       </c>
     </row>
     <row r="809" spans="1:1">
-      <c r="A809">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A809" t="s">
+        <v>735</v>
       </c>
     </row>
     <row r="810" spans="1:1">
-      <c r="A810">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A810" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="811" spans="1:1">
-      <c r="A811">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A811" t="s">
+        <v>737</v>
       </c>
     </row>
     <row r="812" spans="1:1">
-      <c r="A812">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" email-profile Sample_Email_Profile", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A812" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="813" spans="1:1">
+      <c r="A813" t="s">
+        <v>739</v>
       </c>
     </row>
     <row r="814" spans="1:1">
       <c r="A814" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="815" spans="1:1">
       <c r="A815" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="816" spans="1:1">
       <c r="A816" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="817" spans="1:1">
       <c r="A817" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="818" spans="1:1">
       <c r="A818" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="819" spans="1:1">
       <c r="A819" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="820" spans="1:1">
       <c r="A820" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="821" spans="1:1">
       <c r="A821" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="822" spans="1:1">
       <c r="A822" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="823" spans="1:1">
       <c r="A823" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
     </row>
     <row r="824" spans="1:1">
       <c r="A824" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="825" spans="1:1">
       <c r="A825" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
     </row>
     <row r="826" spans="1:1">
       <c r="A826" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="827" spans="1:1">
       <c r="A827" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="828" spans="1:1">
       <c r="A828" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="829" spans="1:1">
       <c r="A829" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="830" spans="1:1">
       <c r="A830" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="831" spans="1:1">
       <c r="A831" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="832" spans="1:1">
       <c r="A832" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="833" spans="1:1">
       <c r="A833" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="834" spans="1:1">
       <c r="A834" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="835" spans="1:1">
       <c r="A835" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="836" spans="1:1">
       <c r="A836" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="837" spans="1:1">
       <c r="A837" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="838" spans="1:1">
       <c r="A838" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="839" spans="1:1">
       <c r="A839" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="840" spans="1:1">
       <c r="A840" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="841" spans="1:1">
       <c r="A841" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="842" spans="1:1">
       <c r="A842" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="843" spans="1:1">
-      <c r="A843" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="844" spans="1:1">
-      <c r="A844" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="845" spans="1:1">
-      <c r="A845" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="846" spans="1:1">
-      <c r="A846" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="847" spans="1:1">
-      <c r="A847" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="848" spans="1:1">
-      <c r="A848" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="849" spans="1:1">
-      <c r="A849" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="850" spans="1:1">
-      <c r="A850" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="851" spans="1:1">
-      <c r="A851" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="852" spans="1:1">
-      <c r="A852" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="853" spans="1:1">
-      <c r="A853" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="854" spans="1:1">
-      <c r="A854" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="855" spans="1:1">
-      <c r="A855" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="856" spans="1:1">
-      <c r="A856" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="857" spans="1:1">
-      <c r="A857" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="858" spans="1:1">
-      <c r="A858" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="859" spans="1:1">
-      <c r="A859" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="860" spans="1:1">
-      <c r="A860" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="861" spans="1:1">
-      <c r="A861" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="862" spans="1:1">
-      <c r="A862" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="863" spans="1:1">
-      <c r="A863" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="864" spans="1:1">
-      <c r="A864" t="s">
-        <v>792</v>
+        <v>768</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update loadables and xls
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -1514,13 +1514,13 @@
     <t>set shared profiles file-blocking Alert-Only-FB rules Alert-Only action alert</t>
   </si>
   <si>
-    <t>set shared profiles custom-url-category Black-List</t>
-  </si>
-  <si>
-    <t>set shared profiles custom-url-category White-List</t>
-  </si>
-  <si>
-    <t>set shared profiles custom-url-category Custom-No-Decrypt</t>
+    <t>set shared profiles custom-url-category Block type ""URL List""</t>
+  </si>
+  <si>
+    <t>set shared profiles custom-url-category Allow type ""URL List""</t>
+  </si>
+  <si>
+    <t>set shared profiles custom-url-category Custom-No-Decrypt type ""URL List""</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Outbound-URL credential-enforcement mode ip-user</t>
@@ -1529,7 +1529,7 @@
     <t>set shared profiles url-filtering Outbound-URL credential-enforcement log-severity high</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Outbound-URL credential-enforcement block [ Black-List White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set shared profiles url-filtering Outbound-URL credential-enforcement block [ Block Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Outbound-URL log-http-hdr-user-agent yes</t>
@@ -1541,10 +1541,10 @@
     <t>set shared profiles url-filtering Outbound-URL log-http-hdr-xff yes</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Outbound-URL alert [ White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
-  </si>
-  <si>
-    <t>set shared profiles url-filtering Outbound-URL block [ Black-List command-and-control grayware malware phishing ]</t>
+    <t>set shared profiles url-filtering Outbound-URL alert [ Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+  </si>
+  <si>
+    <t>set shared profiles url-filtering Outbound-URL block [ Block command-and-control grayware malware phishing ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Outbound-URL mlav-engine-urlbased-enabled ""Phishing Detection"" mlav-policy-action block</t>
@@ -1559,10 +1559,10 @@
     <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement log-severity medium</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement alert [ Black-List White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
-  </si>
-  <si>
-    <t>set shared profiles url-filtering Alert-Only-URL alert [ Black-List White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement alert [ Block Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+  </si>
+  <si>
+    <t>set shared profiles url-filtering Alert-Only-URL alert [ Block Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Alert-Only-URL mlav-engine-urlbased-enabled ""Phishing Detection"" mlav-policy-action alert</t>
@@ -1577,7 +1577,7 @@
     <t>set shared profiles url-filtering Exception-URL credential-enforcement log-severity high</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Exception-URL credential-enforcement block [ Black-List White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set shared profiles url-filtering Exception-URL credential-enforcement block [ Block Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Exception-URL log-http-hdr-user-agent yes</t>
@@ -1589,10 +1589,10 @@
     <t>set shared profiles url-filtering Exception-URL log-http-hdr-xff yes</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Exception-URL alert [ White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
-  </si>
-  <si>
-    <t>set shared profiles url-filtering Exception-URL block [ Black-List command-and-control grayware malware phishing ]</t>
+    <t>set shared profiles url-filtering Exception-URL alert [ Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+  </si>
+  <si>
+    <t>set shared profiles url-filtering Exception-URL block [ Block command-and-control grayware malware phishing ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Exception-URL mlav-engine-urlbased-enabled ""Phishing Detection"" mlav-policy-action block</t>

</xml_diff>

<commit_message>
fix panorama template set command issue
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="774">
   <si>
     <t>Variable Name</t>
   </si>
@@ -1892,7 +1892,10 @@
     <t># shared template configuration referenced in template stacks</t>
   </si>
   <si>
-    <t>set template iron-skillet settings default-vsys vsys1</t>
+    <t># the commented out line below may not be required in 10.0. Users can enter if needed</t>
+  </si>
+  <si>
+    <t># set template iron-skillet settings default-vsys vsys1</t>
   </si>
   <si>
     <t>set template iron-skillet config vsys vsys1</t>
@@ -2977,7 +2980,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A848"/>
+  <dimension ref="A2:A849"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5895,20 +5898,20 @@
       </c>
     </row>
     <row r="598" spans="1:1">
-      <c r="A598">
-        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
-        <v>0</v>
+      <c r="A598" t="s">
+        <v>627</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599">
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="600" spans="1:1">
+      <c r="A600">
         <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="600" spans="1:1">
-      <c r="A600" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="601" spans="1:1">
@@ -6007,32 +6010,32 @@
       </c>
     </row>
     <row r="620" spans="1:1">
-      <c r="A620">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B18)</f>
-        <v>0</v>
+      <c r="A620" t="s">
+        <v>647</v>
       </c>
     </row>
     <row r="621" spans="1:1">
       <c r="A621">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B19)</f>
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="622" spans="1:1">
       <c r="A622">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="623" spans="1:1">
       <c r="A623">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="624" spans="1:1">
+      <c r="A624">
         <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="624" spans="1:1">
-      <c r="A624" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="625" spans="1:1">
@@ -6265,8 +6268,8 @@
         <v>693</v>
       </c>
     </row>
-    <row r="672" spans="1:1">
-      <c r="A672" t="s">
+    <row r="671" spans="1:1">
+      <c r="A671" t="s">
         <v>694</v>
       </c>
     </row>
@@ -6385,8 +6388,8 @@
         <v>717</v>
       </c>
     </row>
-    <row r="697" spans="1:1">
-      <c r="A697" t="s">
+    <row r="696" spans="1:1">
+      <c r="A696" t="s">
         <v>718</v>
       </c>
     </row>
@@ -6396,576 +6399,576 @@
       </c>
     </row>
     <row r="699" spans="1:1">
-      <c r="A699">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A699" t="s">
+        <v>720</v>
       </c>
     </row>
     <row r="700" spans="1:1">
       <c r="A700">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="701" spans="1:1">
       <c r="A701">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="702" spans="1:1">
+      <c r="A702">
         <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B10), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="703" spans="1:1">
-      <c r="A703" t="s">
-        <v>720</v>
-      </c>
-    </row>
     <row r="704" spans="1:1">
-      <c r="A704">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A704" t="s">
+        <v>721</v>
       </c>
     </row>
     <row r="705" spans="1:1">
       <c r="A705">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="706" spans="1:1">
       <c r="A706">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="707" spans="1:1">
       <c r="A707">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="708" spans="1:1">
+      <c r="A708">
         <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="709" spans="1:1">
-      <c r="A709" t="s">
-        <v>721</v>
-      </c>
-    </row>
     <row r="710" spans="1:1">
-      <c r="A710">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A710" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="711" spans="1:1">
       <c r="A711">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B12), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="712" spans="1:1">
       <c r="A712">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B13), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B12), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="713" spans="1:1">
       <c r="A713">
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B13), "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="714" spans="1:1">
+      <c r="A714">
         <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B14), "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="715" spans="1:1">
-      <c r="A715">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="716" spans="1:1">
       <c r="A716">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="717" spans="1:1">
       <c r="A717">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="718" spans="1:1">
       <c r="A718">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="719" spans="1:1">
       <c r="A719">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="720" spans="1:1">
       <c r="A720">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="721" spans="1:1">
       <c r="A721">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="766" spans="1:1">
       <c r="A766">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="767" spans="1:1">
       <c r="A767">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="768" spans="1:1">
       <c r="A768">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="769" spans="1:1">
       <c r="A769">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="770" spans="1:1">
       <c r="A770">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="771" spans="1:1">
       <c r="A771">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="772" spans="1:1">
       <c r="A772">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="773" spans="1:1">
       <c r="A773">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="774" spans="1:1">
       <c r="A774">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="775" spans="1:1">
       <c r="A775">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="776" spans="1:1">
       <c r="A776">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="777" spans="1:1">
       <c r="A777">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="778" spans="1:1">
       <c r="A778">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="779" spans="1:1">
       <c r="A779">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="780" spans="1:1">
       <c r="A780">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="781" spans="1:1">
       <c r="A781">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="782" spans="1:1">
       <c r="A782">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="783" spans="1:1">
       <c r="A783">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="784" spans="1:1">
       <c r="A784">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="785" spans="1:1">
       <c r="A785">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="786" spans="1:1">
       <c r="A786">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="787" spans="1:1">
       <c r="A787">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="788" spans="1:1">
       <c r="A788">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="789" spans="1:1">
       <c r="A789">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="790" spans="1:1">
       <c r="A790">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="791" spans="1:1">
       <c r="A791">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="792" spans="1:1">
       <c r="A792">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="793" spans="1:1">
       <c r="A793">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="794" spans="1:1">
       <c r="A794">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="795" spans="1:1">
       <c r="A795">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="796" spans="1:1">
       <c r="A796">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="797" spans="1:1">
+      <c r="A797">
         <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" email-profile Sample_Email_Profile", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="798" spans="1:1">
-      <c r="A798" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="799" spans="1:1">
@@ -7216,6 +7219,11 @@
     <row r="848" spans="1:1">
       <c r="A848" t="s">
         <v>772</v>
+      </c>
+    </row>
+    <row r="849" spans="1:1">
+      <c r="A849" t="s">
+        <v>773</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made Ironskillet 10.0 backdrop changes
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="774">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="780">
   <si>
     <t>Variable Name</t>
   </si>
@@ -452,7 +452,7 @@
     <t>set shared tag Internal comments ""Internal to Internal""</t>
   </si>
   <si>
-    <t>set shared tag iron-skillet-version comments ""version 0.0.1 for 10.0: version of this IronSkillet template file""</t>
+    <t>set shared tag iron-skillet-version comments ""version 0.0.2 for 10.0: version of this IronSkillet template file""</t>
   </si>
   <si>
     <t># shared log settings for the NGFW</t>
@@ -1553,6 +1553,12 @@
     <t>set shared profiles url-filtering Outbound-URL mlav-engine-urlbased-enabled ""Javascript Exploit Detection"" mlav-policy-action block</t>
   </si>
   <si>
+    <t>set shared profiles url-filtering Outbound-URL credential-enforcement alert real-time-detection</t>
+  </si>
+  <si>
+    <t>set shared profiles url-filtering Outbound-URL alert real-time-detection</t>
+  </si>
+  <si>
     <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement mode ip-user</t>
   </si>
   <si>
@@ -1571,6 +1577,12 @@
     <t>set shared profiles url-filtering Alert-Only-URL mlav-engine-urlbased-enabled ""Javascript Exploit Detection"" mlav-policy-action alert</t>
   </si>
   <si>
+    <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement alert real-time-detection</t>
+  </si>
+  <si>
+    <t>set shared profiles url-filtering Alert-Only-URL alert real-time-detection</t>
+  </si>
+  <si>
     <t>set shared profiles url-filtering Exception-URL credential-enforcement mode ip-user</t>
   </si>
   <si>
@@ -1599,6 +1611,12 @@
   </si>
   <si>
     <t>set shared profiles url-filtering Exception-URL mlav-engine-urlbased-enabled ""Javascript Exploit Detection"" mlav-policy-action block</t>
+  </si>
+  <si>
+    <t>set shared profiles url-filtering Exception-URL credential-enforcement alert real-time-detection</t>
+  </si>
+  <si>
+    <t>set shared profiles url-filtering Exception-URL alert real-time-detection</t>
   </si>
   <si>
     <t>set shared profiles wildfire-analysis Outbound-WF rules Forward-All application any</t>
@@ -2980,7 +2998,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A849"/>
+  <dimension ref="A2:A855"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5482,33 +5500,33 @@
         <v>543</v>
       </c>
     </row>
+    <row r="512" spans="1:1">
+      <c r="A512" t="s">
+        <v>544</v>
+      </c>
+    </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="518" spans="1:1">
-      <c r="A518" t="s">
         <v>549</v>
       </c>
     </row>
@@ -5627,33 +5645,33 @@
         <v>572</v>
       </c>
     </row>
+    <row r="542" spans="1:1">
+      <c r="A542" t="s">
+        <v>573</v>
+      </c>
+    </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="548" spans="1:1">
-      <c r="A548" t="s">
         <v>578</v>
       </c>
     </row>
@@ -5882,66 +5900,66 @@
         <v>623</v>
       </c>
     </row>
+    <row r="594" spans="1:1">
+      <c r="A594" t="s">
+        <v>624</v>
+      </c>
+    </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="599" spans="1:1">
-      <c r="A599">
-        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="600" spans="1:1">
-      <c r="A600">
-        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
-        <v>0</v>
+      <c r="A599" t="s">
+        <v>629</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
     </row>
     <row r="605" spans="1:1">
-      <c r="A605" t="s">
-        <v>632</v>
+      <c r="A605">
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="606" spans="1:1">
-      <c r="A606" t="s">
-        <v>633</v>
+      <c r="A606">
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="607" spans="1:1">
@@ -6015,57 +6033,57 @@
       </c>
     </row>
     <row r="621" spans="1:1">
-      <c r="A621">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B18)</f>
-        <v>0</v>
+      <c r="A621" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="622" spans="1:1">
-      <c r="A622">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B19)</f>
-        <v>0</v>
+      <c r="A622" t="s">
+        <v>649</v>
       </c>
     </row>
     <row r="623" spans="1:1">
-      <c r="A623">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
-        <v>0</v>
+      <c r="A623" t="s">
+        <v>650</v>
       </c>
     </row>
     <row r="624" spans="1:1">
-      <c r="A624">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
-        <v>0</v>
+      <c r="A624" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="625" spans="1:1">
       <c r="A625" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>649</v>
+        <v>653</v>
       </c>
     </row>
     <row r="627" spans="1:1">
-      <c r="A627" t="s">
-        <v>650</v>
+      <c r="A627">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B18)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="628" spans="1:1">
-      <c r="A628" t="s">
-        <v>651</v>
+      <c r="A628">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B19)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="629" spans="1:1">
-      <c r="A629" t="s">
-        <v>652</v>
+      <c r="A629">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="630" spans="1:1">
-      <c r="A630" t="s">
-        <v>653</v>
+      <c r="A630">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="631" spans="1:1">
@@ -6273,33 +6291,33 @@
         <v>694</v>
       </c>
     </row>
+    <row r="672" spans="1:1">
+      <c r="A672" t="s">
+        <v>695</v>
+      </c>
+    </row>
     <row r="673" spans="1:1">
       <c r="A673" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="675" spans="1:1">
       <c r="A675" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="676" spans="1:1">
       <c r="A676" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="677" spans="1:1">
       <c r="A677" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="678" spans="1:1">
-      <c r="A678" t="s">
         <v>700</v>
       </c>
     </row>
@@ -6393,612 +6411,612 @@
         <v>718</v>
       </c>
     </row>
+    <row r="697" spans="1:1">
+      <c r="A697" t="s">
+        <v>719</v>
+      </c>
+    </row>
     <row r="698" spans="1:1">
       <c r="A698" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="699" spans="1:1">
       <c r="A699" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="700" spans="1:1">
-      <c r="A700">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A700" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="701" spans="1:1">
-      <c r="A701">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A701" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="702" spans="1:1">
-      <c r="A702">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B10), "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A702" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="704" spans="1:1">
       <c r="A704" t="s">
-        <v>721</v>
+        <v>725</v>
       </c>
     </row>
     <row r="705" spans="1:1">
-      <c r="A705">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A705" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="706" spans="1:1">
       <c r="A706">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="707" spans="1:1">
       <c r="A707">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="708" spans="1:1">
       <c r="A708">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B10), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="710" spans="1:1">
       <c r="A710" t="s">
-        <v>722</v>
+        <v>727</v>
       </c>
     </row>
     <row r="711" spans="1:1">
       <c r="A711">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="712" spans="1:1">
       <c r="A712">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B12), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="713" spans="1:1">
       <c r="A713">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B13), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="714" spans="1:1">
       <c r="A714">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B14), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="716" spans="1:1">
-      <c r="A716">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A716" t="s">
+        <v>728</v>
       </c>
     </row>
     <row r="717" spans="1:1">
       <c r="A717">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="718" spans="1:1">
       <c r="A718">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B12), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="719" spans="1:1">
       <c r="A719">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B13), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="720" spans="1:1">
       <c r="A720">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="721" spans="1:1">
-      <c r="A721">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B14), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="766" spans="1:1">
       <c r="A766">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="767" spans="1:1">
       <c r="A767">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="768" spans="1:1">
       <c r="A768">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="769" spans="1:1">
       <c r="A769">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="770" spans="1:1">
       <c r="A770">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="771" spans="1:1">
       <c r="A771">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="772" spans="1:1">
       <c r="A772">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="773" spans="1:1">
       <c r="A773">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="774" spans="1:1">
       <c r="A774">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="775" spans="1:1">
       <c r="A775">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="776" spans="1:1">
       <c r="A776">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="777" spans="1:1">
       <c r="A777">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="778" spans="1:1">
       <c r="A778">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="779" spans="1:1">
       <c r="A779">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="780" spans="1:1">
       <c r="A780">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="781" spans="1:1">
       <c r="A781">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="782" spans="1:1">
       <c r="A782">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="783" spans="1:1">
       <c r="A783">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="784" spans="1:1">
       <c r="A784">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="785" spans="1:1">
       <c r="A785">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="786" spans="1:1">
       <c r="A786">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="787" spans="1:1">
       <c r="A787">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="788" spans="1:1">
       <c r="A788">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="789" spans="1:1">
       <c r="A789">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="790" spans="1:1">
       <c r="A790">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="791" spans="1:1">
       <c r="A791">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="792" spans="1:1">
       <c r="A792">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="793" spans="1:1">
       <c r="A793">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="794" spans="1:1">
       <c r="A794">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="795" spans="1:1">
       <c r="A795">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="796" spans="1:1">
       <c r="A796">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="797" spans="1:1">
       <c r="A797">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="798" spans="1:1">
+      <c r="A798">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="799" spans="1:1">
+      <c r="A799">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="800" spans="1:1">
+      <c r="A800">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="801" spans="1:1">
+      <c r="A801">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="802" spans="1:1">
+      <c r="A802">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="803" spans="1:1">
+      <c r="A803">
         <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" email-profile Sample_Email_Profile", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="799" spans="1:1">
-      <c r="A799" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="800" spans="1:1">
-      <c r="A800" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="801" spans="1:1">
-      <c r="A801" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="802" spans="1:1">
-      <c r="A802" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="803" spans="1:1">
-      <c r="A803" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="804" spans="1:1">
-      <c r="A804" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="805" spans="1:1">
@@ -7224,6 +7242,36 @@
     <row r="849" spans="1:1">
       <c r="A849" t="s">
         <v>773</v>
+      </c>
+    </row>
+    <row r="850" spans="1:1">
+      <c r="A850" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="851" spans="1:1">
+      <c r="A851" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="852" spans="1:1">
+      <c r="A852" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="853" spans="1:1">
+      <c r="A853" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="854" spans="1:1">
+      <c r="A854" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="855" spans="1:1">
+      <c r="A855" t="s">
+        <v>779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added changes for static and dhcp loadable configs .conf files
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -1697,6 +1697,12 @@
     <t>set shared profiles url-filtering Outbound-URL mlav-engine-urlbased-enabled ""Javascript Exploit Detection"" mlav-policy-action block</t>
   </si>
   <si>
+    <t>set shared profiles url-filtering Outbound-URL credential-enforcement alert real-time-detection</t>
+  </si>
+  <si>
+    <t>set shared profiles url-filtering Outbound-URL alert real-time-detection</t>
+  </si>
+  <si>
     <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement mode ip-user</t>
   </si>
   <si>
@@ -1715,6 +1721,12 @@
     <t>set shared profiles url-filtering Alert-Only-URL mlav-engine-urlbased-enabled ""Javascript Exploit Detection"" mlav-policy-action alert</t>
   </si>
   <si>
+    <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement alert real-time-detection</t>
+  </si>
+  <si>
+    <t>set shared profiles url-filtering Alert-Only-URL alert real-time-detection</t>
+  </si>
+  <si>
     <t>set shared profiles url-filtering Exception-URL credential-enforcement mode ip-user</t>
   </si>
   <si>
@@ -1743,18 +1755,6 @@
   </si>
   <si>
     <t>set shared profiles url-filtering Exception-URL mlav-engine-urlbased-enabled ""Javascript Exploit Detection"" mlav-policy-action block</t>
-  </si>
-  <si>
-    <t>set shared profiles url-filtering Outbound-URL credential-enforcement alert real-time-detection</t>
-  </si>
-  <si>
-    <t>set shared profiles url-filtering Outbound-URL alert real-time-detection</t>
-  </si>
-  <si>
-    <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement alert real-time-detection</t>
-  </si>
-  <si>
-    <t>set shared profiles url-filtering Alert-Only-URL alert real-time-detection</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Exception-URL credential-enforcement alert real-time-detection</t>

</xml_diff>

<commit_message>
ran build all script
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="835">
   <si>
     <t>Variable Name</t>
   </si>
@@ -452,7 +452,7 @@
     <t>set shared tag Internal comments ""Internal to Internal""</t>
   </si>
   <si>
-    <t>set shared tag iron-skillet-version comments ""version 0.0.1 for 10.1: version of this IronSkillet template file""</t>
+    <t>set shared tag iron-skillet-version comments ""version 0.0.2 for 10.1: version of this IronSkillet template file""</t>
   </si>
   <si>
     <t># shared log settings for the NGFW</t>
@@ -653,6 +653,9 @@
     <t>set shared profiles virus Alert-Only-AV mlav-engine-filebased-enabled ""PowerShell Script 2"" mlav-policy-action enable(alert-only)</t>
   </si>
   <si>
+    <t>set shared profiles virus Alert-Only-AV mlav-engine-filebased-enabled ""Executable Linked Format"" mlav-policy-action enable(alert-only)</t>
+  </si>
+  <si>
     <t>set shared profiles virus Outbound-AV decoder ftp action reset-both</t>
   </si>
   <si>
@@ -725,6 +728,9 @@
     <t>set shared profiles virus Outbound-AV mlav-engine-filebased-enabled ""PowerShell Script 2"" mlav-policy-action enable</t>
   </si>
   <si>
+    <t>set shared profiles virus Outbound-AV mlav-engine-filebased-enabled ""Executable Linked Format"" mlav-policy-action enable</t>
+  </si>
+  <si>
     <t>set shared profiles virus Inbound-AV decoder ftp action reset-both</t>
   </si>
   <si>
@@ -797,6 +803,9 @@
     <t>set shared profiles virus Inbound-AV mlav-engine-filebased-enabled ""PowerShell Script 2"" mlav-policy-action enable</t>
   </si>
   <si>
+    <t>set shared profiles virus Inbound-AV mlav-engine-filebased-enabled ""Executable Linked Format"" mlav-policy-action enable</t>
+  </si>
+  <si>
     <t>set shared profiles virus Internal-AV decoder ftp action reset-both</t>
   </si>
   <si>
@@ -869,6 +878,9 @@
     <t>set shared profiles virus Internal-AV mlav-engine-filebased-enabled ""PowerShell Script 2"" mlav-policy-action enable</t>
   </si>
   <si>
+    <t>set shared profiles virus Internal-AV mlav-engine-filebased-enabled ""Executable Linked Format"" mlav-policy-action enable</t>
+  </si>
+  <si>
     <t>set shared profiles virus Exception-AV decoder ftp action reset-both</t>
   </si>
   <si>
@@ -942,6 +954,9 @@
   </si>
   <si>
     <t>set shared profiles virus Exception-AV mlav-engine-filebased-enabled ""PowerShell Script 2"" mlav-policy-action enable</t>
+  </si>
+  <si>
+    <t>set shared profiles virus Exception-AV mlav-engine-filebased-enabled ""Executable Linked Format"" mlav-policy-action enable</t>
   </si>
   <si>
     <t>set shared profiles spyware Outbound-AS botnet-domains lists default-paloalto-dns packet-capture single-packet</t>
@@ -3145,7 +3160,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A907"/>
+  <dimension ref="A2:A912"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4418,40 +4433,40 @@
       </c>
     </row>
     <row r="264" spans="1:1">
-      <c r="A264">
-        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A264" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="265" spans="1:1">
-      <c r="A265">
-        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A265" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="269" spans="1:1">
-      <c r="A269" t="s">
-        <v>312</v>
+      <c r="A269">
+        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="270" spans="1:1">
-      <c r="A270" t="s">
-        <v>313</v>
+      <c r="A270">
+        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="271" spans="1:1">
@@ -4625,40 +4640,40 @@
       </c>
     </row>
     <row r="305" spans="1:1">
-      <c r="A305">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A305" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="306" spans="1:1">
-      <c r="A306">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A306" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="310" spans="1:1">
-      <c r="A310" t="s">
-        <v>351</v>
+      <c r="A310">
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="311" spans="1:1">
-      <c r="A311" t="s">
-        <v>352</v>
+      <c r="A311">
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="312" spans="1:1">
@@ -4832,40 +4847,40 @@
       </c>
     </row>
     <row r="346" spans="1:1">
-      <c r="A346">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A346" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="347" spans="1:1">
-      <c r="A347">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A347" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="351" spans="1:1">
-      <c r="A351" t="s">
-        <v>390</v>
+      <c r="A351">
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="352" spans="1:1">
-      <c r="A352" t="s">
-        <v>391</v>
+      <c r="A352">
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="353" spans="1:1">
@@ -5039,40 +5054,40 @@
       </c>
     </row>
     <row r="387" spans="1:1">
-      <c r="A387">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A387" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="388" spans="1:1">
-      <c r="A388">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A388" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="391" spans="1:1">
       <c r="A391" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="392" spans="1:1">
-      <c r="A392" t="s">
-        <v>429</v>
+      <c r="A392">
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="393" spans="1:1">
-      <c r="A393" t="s">
-        <v>430</v>
+      <c r="A393">
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="394" spans="1:1">
@@ -5221,49 +5236,49 @@
       </c>
     </row>
     <row r="423" spans="1:1">
-      <c r="A423">
-        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A423" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="424" spans="1:1">
-      <c r="A424">
-        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A424" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>461</v>
+        <v>463</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1">
+      <c r="A427" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1">
+      <c r="A428">
+        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1">
+      <c r="A429">
+        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="432" spans="1:1">
-      <c r="A432" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="433" spans="1:1">
-      <c r="A433" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="434" spans="1:1">
-      <c r="A434" t="s">
         <v>466</v>
       </c>
     </row>
@@ -5682,28 +5697,28 @@
         <v>549</v>
       </c>
     </row>
+    <row r="518" spans="1:1">
+      <c r="A518" t="s">
+        <v>550</v>
+      </c>
+    </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="523" spans="1:1">
-      <c r="A523" t="s">
         <v>554</v>
       </c>
     </row>
@@ -5922,28 +5937,28 @@
         <v>597</v>
       </c>
     </row>
+    <row r="567" spans="1:1">
+      <c r="A567" t="s">
+        <v>598</v>
+      </c>
+    </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="572" spans="1:1">
-      <c r="A572" t="s">
         <v>602</v>
       </c>
     </row>
@@ -6067,28 +6082,28 @@
         <v>626</v>
       </c>
     </row>
+    <row r="597" spans="1:1">
+      <c r="A597" t="s">
+        <v>627</v>
+      </c>
+    </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="602" spans="1:1">
-      <c r="A602" t="s">
         <v>631</v>
       </c>
     </row>
@@ -6322,61 +6337,61 @@
         <v>677</v>
       </c>
     </row>
+    <row r="649" spans="1:1">
+      <c r="A649" t="s">
+        <v>678</v>
+      </c>
+    </row>
     <row r="650" spans="1:1">
       <c r="A650" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="654" spans="1:1">
-      <c r="A654">
-        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
-        <v>0</v>
+        <v>682</v>
       </c>
     </row>
     <row r="655" spans="1:1">
-      <c r="A655">
-        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
-        <v>0</v>
+      <c r="A655" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="659" spans="1:1">
-      <c r="A659" t="s">
-        <v>685</v>
+      <c r="A659">
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="660" spans="1:1">
-      <c r="A660" t="s">
-        <v>686</v>
+      <c r="A660">
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="661" spans="1:1">
@@ -6455,52 +6470,52 @@
       </c>
     </row>
     <row r="676" spans="1:1">
-      <c r="A676">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B18)</f>
-        <v>0</v>
+      <c r="A676" t="s">
+        <v>702</v>
       </c>
     </row>
     <row r="677" spans="1:1">
-      <c r="A677">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B19)</f>
-        <v>0</v>
+      <c r="A677" t="s">
+        <v>703</v>
       </c>
     </row>
     <row r="678" spans="1:1">
-      <c r="A678">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
-        <v>0</v>
+      <c r="A678" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="679" spans="1:1">
-      <c r="A679">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
-        <v>0</v>
+      <c r="A679" t="s">
+        <v>705</v>
       </c>
     </row>
     <row r="680" spans="1:1">
       <c r="A680" t="s">
-        <v>702</v>
+        <v>706</v>
       </c>
     </row>
     <row r="681" spans="1:1">
-      <c r="A681" t="s">
-        <v>703</v>
+      <c r="A681">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B18)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="682" spans="1:1">
-      <c r="A682" t="s">
-        <v>704</v>
+      <c r="A682">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B19)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="683" spans="1:1">
-      <c r="A683" t="s">
-        <v>705</v>
+      <c r="A683">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="684" spans="1:1">
-      <c r="A684" t="s">
-        <v>706</v>
+      <c r="A684">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="685" spans="1:1">
@@ -6713,28 +6728,28 @@
         <v>748</v>
       </c>
     </row>
+    <row r="727" spans="1:1">
+      <c r="A727" t="s">
+        <v>749</v>
+      </c>
+    </row>
     <row r="728" spans="1:1">
       <c r="A728" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="732" spans="1:1">
-      <c r="A732" t="s">
         <v>753</v>
       </c>
     </row>
@@ -6833,617 +6848,617 @@
         <v>772</v>
       </c>
     </row>
+    <row r="752" spans="1:1">
+      <c r="A752" t="s">
+        <v>773</v>
+      </c>
+    </row>
     <row r="753" spans="1:1">
       <c r="A753" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754" t="s">
-        <v>774</v>
+        <v>775</v>
+      </c>
+    </row>
+    <row r="755" spans="1:1">
+      <c r="A755" t="s">
+        <v>776</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="757" spans="1:1">
-      <c r="A757" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="758" spans="1:1">
-      <c r="A758">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A758" t="s">
+        <v>778</v>
       </c>
     </row>
     <row r="759" spans="1:1">
-      <c r="A759">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="760" spans="1:1">
-      <c r="A760">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B10), "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A759" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="761" spans="1:1">
+      <c r="A761" t="s">
+        <v>780</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762" t="s">
-        <v>777</v>
+        <v>781</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="766" spans="1:1">
-      <c r="A766">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B10), "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="767" spans="1:1">
+      <c r="A767" t="s">
+        <v>782</v>
       </c>
     </row>
     <row r="768" spans="1:1">
-      <c r="A768" t="s">
-        <v>778</v>
+      <c r="A768">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="769" spans="1:1">
       <c r="A769">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="770" spans="1:1">
       <c r="A770">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B12), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="771" spans="1:1">
       <c r="A771">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B13), "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="772" spans="1:1">
-      <c r="A772">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B14), "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="773" spans="1:1">
+      <c r="A773" t="s">
+        <v>783</v>
       </c>
     </row>
     <row r="774" spans="1:1">
       <c r="A774">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="775" spans="1:1">
       <c r="A775">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B12), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="776" spans="1:1">
       <c r="A776">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B13), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="777" spans="1:1">
       <c r="A777">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="778" spans="1:1">
-      <c r="A778">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B14), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="779" spans="1:1">
       <c r="A779">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="780" spans="1:1">
       <c r="A780">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="781" spans="1:1">
       <c r="A781">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="782" spans="1:1">
       <c r="A782">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="783" spans="1:1">
       <c r="A783">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="784" spans="1:1">
       <c r="A784">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="785" spans="1:1">
       <c r="A785">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="786" spans="1:1">
       <c r="A786">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="787" spans="1:1">
       <c r="A787">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="788" spans="1:1">
       <c r="A788">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="789" spans="1:1">
       <c r="A789">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="790" spans="1:1">
       <c r="A790">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="791" spans="1:1">
       <c r="A791">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="792" spans="1:1">
       <c r="A792">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="793" spans="1:1">
       <c r="A793">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="794" spans="1:1">
       <c r="A794">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="795" spans="1:1">
       <c r="A795">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="796" spans="1:1">
       <c r="A796">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="797" spans="1:1">
       <c r="A797">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="798" spans="1:1">
       <c r="A798">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="799" spans="1:1">
       <c r="A799">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="800" spans="1:1">
       <c r="A800">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="801" spans="1:1">
       <c r="A801">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="802" spans="1:1">
       <c r="A802">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="803" spans="1:1">
       <c r="A803">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="804" spans="1:1">
       <c r="A804">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="805" spans="1:1">
       <c r="A805">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="806" spans="1:1">
       <c r="A806">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="807" spans="1:1">
       <c r="A807">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="808" spans="1:1">
       <c r="A808">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="809" spans="1:1">
       <c r="A809">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="810" spans="1:1">
       <c r="A810">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="811" spans="1:1">
       <c r="A811">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="812" spans="1:1">
       <c r="A812">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="813" spans="1:1">
       <c r="A813">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="814" spans="1:1">
       <c r="A814">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="815" spans="1:1">
       <c r="A815">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="816" spans="1:1">
       <c r="A816">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="817" spans="1:1">
       <c r="A817">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="818" spans="1:1">
       <c r="A818">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="819" spans="1:1">
       <c r="A819">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="820" spans="1:1">
       <c r="A820">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="821" spans="1:1">
       <c r="A821">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="822" spans="1:1">
       <c r="A822">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="823" spans="1:1">
       <c r="A823">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="824" spans="1:1">
       <c r="A824">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="825" spans="1:1">
       <c r="A825">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="826" spans="1:1">
       <c r="A826">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="827" spans="1:1">
       <c r="A827">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="828" spans="1:1">
       <c r="A828">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="829" spans="1:1">
       <c r="A829">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="830" spans="1:1">
       <c r="A830">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="831" spans="1:1">
       <c r="A831">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="832" spans="1:1">
       <c r="A832">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="833" spans="1:1">
       <c r="A833">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="834" spans="1:1">
       <c r="A834">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="835" spans="1:1">
       <c r="A835">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="836" spans="1:1">
       <c r="A836">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="837" spans="1:1">
       <c r="A837">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="838" spans="1:1">
       <c r="A838">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="839" spans="1:1">
       <c r="A839">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="840" spans="1:1">
       <c r="A840">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="841" spans="1:1">
       <c r="A841">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="842" spans="1:1">
       <c r="A842">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="843" spans="1:1">
       <c r="A843">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="844" spans="1:1">
       <c r="A844">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="845" spans="1:1">
       <c r="A845">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="846" spans="1:1">
       <c r="A846">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="847" spans="1:1">
       <c r="A847">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="848" spans="1:1">
       <c r="A848">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="849" spans="1:1">
       <c r="A849">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="850" spans="1:1">
       <c r="A850">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="851" spans="1:1">
       <c r="A851">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="852" spans="1:1">
       <c r="A852">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="853" spans="1:1">
       <c r="A853">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="854" spans="1:1">
       <c r="A854">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="855" spans="1:1">
       <c r="A855">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="856" spans="1:1">
+      <c r="A856">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="857" spans="1:1">
+      <c r="A857">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="858" spans="1:1">
+      <c r="A858">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="859" spans="1:1">
+      <c r="A859">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="860" spans="1:1">
+      <c r="A860">
         <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" email-profile Sample_Email_Profile", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="857" spans="1:1">
-      <c r="A857" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="858" spans="1:1">
-      <c r="A858" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="859" spans="1:1">
-      <c r="A859" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="860" spans="1:1">
-      <c r="A860" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="861" spans="1:1">
-      <c r="A861" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="862" spans="1:1">
@@ -7674,6 +7689,31 @@
     <row r="907" spans="1:1">
       <c r="A907" t="s">
         <v>829</v>
+      </c>
+    </row>
+    <row r="908" spans="1:1">
+      <c r="A908" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="909" spans="1:1">
+      <c r="A909" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="910" spans="1:1">
+      <c r="A910" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="911" spans="1:1">
+      <c r="A911" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="912" spans="1:1">
+      <c r="A912" t="s">
+        <v>834</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the ELF profiles into the right files this time
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="786">
   <si>
     <t>Variable Name</t>
   </si>
@@ -452,7 +452,7 @@
     <t>set shared tag Internal comments ""Internal to Internal""</t>
   </si>
   <si>
-    <t>set shared tag iron-skillet-version comments ""version 0.0.2 for 10.0: version of this IronSkillet template file""</t>
+    <t>set shared tag iron-skillet-version comments ""version 0.0.3 for 10.0: version of this IronSkillet template file""</t>
   </si>
   <si>
     <t># shared log settings for the NGFW</t>
@@ -653,6 +653,9 @@
     <t>set shared profiles virus Alert-Only-AV mlav-engine-filebased-enabled ""PowerShell Script 2"" mlav-policy-action enable(alert-only)</t>
   </si>
   <si>
+    <t>set shared profiles virus Alert-Only-AV mlav-engine-filebased-enabled ""Executable Linked Format"" mlav-policy-action enable(alert-only)</t>
+  </si>
+  <si>
     <t>set shared profiles virus Outbound-AV decoder ftp action reset-both</t>
   </si>
   <si>
@@ -725,6 +728,9 @@
     <t>set shared profiles virus Outbound-AV mlav-engine-filebased-enabled ""PowerShell Script 2"" mlav-policy-action enable</t>
   </si>
   <si>
+    <t>set shared profiles virus Outbound-AV mlav-engine-filebased-enabled ""Executable Linked Format"" mlav-policy-action enable</t>
+  </si>
+  <si>
     <t>set shared profiles virus Inbound-AV decoder ftp action reset-both</t>
   </si>
   <si>
@@ -797,6 +803,9 @@
     <t>set shared profiles virus Inbound-AV mlav-engine-filebased-enabled ""PowerShell Script 2"" mlav-policy-action enable</t>
   </si>
   <si>
+    <t>set shared profiles virus Inbound-AV mlav-engine-filebased-enabled ""Executable Linked Format"" mlav-policy-action enable</t>
+  </si>
+  <si>
     <t>set shared profiles virus Internal-AV decoder ftp action reset-both</t>
   </si>
   <si>
@@ -869,6 +878,9 @@
     <t>set shared profiles virus Internal-AV mlav-engine-filebased-enabled ""PowerShell Script 2"" mlav-policy-action enable</t>
   </si>
   <si>
+    <t>set shared profiles virus Internal-AV mlav-engine-filebased-enabled ""Executable Linked Format"" mlav-policy-action enable</t>
+  </si>
+  <si>
     <t>set shared profiles virus Exception-AV decoder ftp action reset-both</t>
   </si>
   <si>
@@ -944,6 +956,9 @@
     <t>set shared profiles virus Exception-AV mlav-engine-filebased-enabled ""PowerShell Script 2"" mlav-policy-action enable</t>
   </si>
   <si>
+    <t>set shared profiles virus Exception-AV mlav-engine-filebased-enabled ""Executable Linked Format"" mlav-policy-action enable</t>
+  </si>
+  <si>
     <t>set shared profiles spyware Outbound-AS botnet-domains lists default-paloalto-dns packet-capture single-packet</t>
   </si>
   <si>
@@ -1617,6 +1632,9 @@
   </si>
   <si>
     <t>set shared profiles url-filtering Exception-URL alert real-time-detection</t>
+  </si>
+  <si>
+    <t>#Wildfire Analysis Profiles</t>
   </si>
   <si>
     <t>set shared profiles wildfire-analysis Outbound-WF rules Forward-All application any</t>
@@ -2998,7 +3016,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A855"/>
+  <dimension ref="A2:A862"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4266,40 +4284,40 @@
       </c>
     </row>
     <row r="263" spans="1:1">
-      <c r="A263">
-        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A263" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="264" spans="1:1">
-      <c r="A264">
-        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A264" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="268" spans="1:1">
-      <c r="A268" t="s">
-        <v>312</v>
+      <c r="A268">
+        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="269" spans="1:1">
-      <c r="A269" t="s">
-        <v>313</v>
+      <c r="A269">
+        <f>SUBSTITUTE("set shared profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="270" spans="1:1">
@@ -4413,40 +4431,40 @@
       </c>
     </row>
     <row r="292" spans="1:1">
-      <c r="A292">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A292" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="293" spans="1:1">
-      <c r="A293">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A293" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="297" spans="1:1">
-      <c r="A297" t="s">
-        <v>339</v>
+      <c r="A297">
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="298" spans="1:1">
-      <c r="A298" t="s">
-        <v>340</v>
+      <c r="A298">
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="299" spans="1:1">
@@ -4560,40 +4578,40 @@
       </c>
     </row>
     <row r="321" spans="1:1">
-      <c r="A321">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A321" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="322" spans="1:1">
-      <c r="A322">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A322" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="326" spans="1:1">
-      <c r="A326" t="s">
-        <v>366</v>
+      <c r="A326">
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="327" spans="1:1">
-      <c r="A327" t="s">
-        <v>367</v>
+      <c r="A327">
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="328" spans="1:1">
@@ -4707,40 +4725,40 @@
       </c>
     </row>
     <row r="350" spans="1:1">
-      <c r="A350">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A350" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="351" spans="1:1">
-      <c r="A351">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A351" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="355" spans="1:1">
-      <c r="A355" t="s">
-        <v>393</v>
+      <c r="A355">
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="356" spans="1:1">
-      <c r="A356" t="s">
-        <v>394</v>
+      <c r="A356">
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="357" spans="1:1">
@@ -4829,49 +4847,49 @@
       </c>
     </row>
     <row r="374" spans="1:1">
-      <c r="A374">
-        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A374" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="375" spans="1:1">
-      <c r="A375">
-        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A375" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>413</v>
+        <v>415</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1">
+      <c r="A378" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1">
+      <c r="A379">
+        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1">
+      <c r="A380">
+        <f>SUBSTITUTE("set shared profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="383" spans="1:1">
-      <c r="A383" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="384" spans="1:1">
-      <c r="A384" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="385" spans="1:1">
-      <c r="A385" t="s">
         <v>418</v>
       </c>
     </row>
@@ -5290,28 +5308,28 @@
         <v>501</v>
       </c>
     </row>
+    <row r="469" spans="1:1">
+      <c r="A469" t="s">
+        <v>502</v>
+      </c>
+    </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="474" spans="1:1">
-      <c r="A474" t="s">
         <v>506</v>
       </c>
     </row>
@@ -5475,58 +5493,58 @@
         <v>538</v>
       </c>
     </row>
-    <row r="507" spans="1:1">
-      <c r="A507" t="s">
-        <v>539</v>
-      </c>
-    </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1">
+      <c r="A518" t="s">
         <v>549</v>
       </c>
     </row>
@@ -5560,118 +5578,118 @@
         <v>555</v>
       </c>
     </row>
-    <row r="525" spans="1:1">
-      <c r="A525" t="s">
-        <v>556</v>
-      </c>
-    </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="529" spans="1:1">
       <c r="A529" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="548" spans="1:1">
+      <c r="A548" t="s">
         <v>578</v>
       </c>
     </row>
@@ -5705,228 +5723,228 @@
         <v>584</v>
       </c>
     </row>
-    <row r="555" spans="1:1">
-      <c r="A555" t="s">
-        <v>585</v>
-      </c>
-    </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="600" spans="1:1">
+      <c r="A600" t="s">
         <v>629</v>
       </c>
     </row>
@@ -5951,373 +5969,373 @@
       </c>
     </row>
     <row r="605" spans="1:1">
-      <c r="A605">
-        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
-        <v>0</v>
+      <c r="A605" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="606" spans="1:1">
-      <c r="A606">
-        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="607" spans="1:1">
-      <c r="A607" t="s">
-        <v>634</v>
+      <c r="A606" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="612" spans="1:1">
-      <c r="A612" t="s">
-        <v>639</v>
+      <c r="A612">
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="613" spans="1:1">
-      <c r="A613" t="s">
-        <v>640</v>
+      <c r="A613">
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="615" spans="1:1">
       <c r="A615" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="617" spans="1:1">
       <c r="A617" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="618" spans="1:1">
       <c r="A618" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="619" spans="1:1">
       <c r="A619" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="620" spans="1:1">
       <c r="A620" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="621" spans="1:1">
       <c r="A621" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="622" spans="1:1">
       <c r="A622" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="623" spans="1:1">
       <c r="A623" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="624" spans="1:1">
       <c r="A624" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="625" spans="1:1">
       <c r="A625" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="627" spans="1:1">
+      <c r="A627" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="627" spans="1:1">
-      <c r="A627">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B18)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="628" spans="1:1">
-      <c r="A628">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B19)</f>
-        <v>0</v>
+      <c r="A628" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="629" spans="1:1">
-      <c r="A629">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
-        <v>0</v>
+      <c r="A629" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="630" spans="1:1">
-      <c r="A630">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
-        <v>0</v>
+      <c r="A630" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="631" spans="1:1">
       <c r="A631" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
     </row>
     <row r="632" spans="1:1">
       <c r="A632" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
     </row>
     <row r="633" spans="1:1">
       <c r="A633" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
     </row>
     <row r="634" spans="1:1">
-      <c r="A634" t="s">
-        <v>657</v>
+      <c r="A634">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B18)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="635" spans="1:1">
-      <c r="A635" t="s">
-        <v>658</v>
+      <c r="A635">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B19)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="636" spans="1:1">
-      <c r="A636" t="s">
-        <v>659</v>
+      <c r="A636">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="637" spans="1:1">
-      <c r="A637" t="s">
-        <v>660</v>
+      <c r="A637">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="638" spans="1:1">
       <c r="A638" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="641" spans="1:1">
       <c r="A641" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="642" spans="1:1">
       <c r="A642" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="643" spans="1:1">
       <c r="A643" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="647" spans="1:1">
       <c r="A647" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="648" spans="1:1">
       <c r="A648" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="649" spans="1:1">
       <c r="A649" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="654" spans="1:1">
       <c r="A654" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="659" spans="1:1">
       <c r="A659" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="664" spans="1:1">
       <c r="A664" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="665" spans="1:1">
       <c r="A665" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="670" spans="1:1">
       <c r="A670" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="672" spans="1:1">
       <c r="A672" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="673" spans="1:1">
       <c r="A673" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="675" spans="1:1">
       <c r="A675" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="676" spans="1:1">
       <c r="A676" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="677" spans="1:1">
       <c r="A677" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="678" spans="1:1">
+      <c r="A678" t="s">
         <v>700</v>
       </c>
     </row>
@@ -6351,93 +6369,93 @@
         <v>706</v>
       </c>
     </row>
-    <row r="685" spans="1:1">
-      <c r="A685" t="s">
-        <v>707</v>
-      </c>
-    </row>
     <row r="686" spans="1:1">
       <c r="A686" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="687" spans="1:1">
       <c r="A687" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="688" spans="1:1">
       <c r="A688" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="689" spans="1:1">
       <c r="A689" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="690" spans="1:1">
       <c r="A690" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="691" spans="1:1">
       <c r="A691" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="692" spans="1:1">
       <c r="A692" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="693" spans="1:1">
       <c r="A693" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="694" spans="1:1">
       <c r="A694" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="695" spans="1:1">
       <c r="A695" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="696" spans="1:1">
       <c r="A696" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="697" spans="1:1">
       <c r="A697" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="698" spans="1:1">
       <c r="A698" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="699" spans="1:1">
       <c r="A699" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="700" spans="1:1">
       <c r="A700" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="701" spans="1:1">
       <c r="A701" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="702" spans="1:1">
       <c r="A702" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="703" spans="1:1">
+      <c r="A703" t="s">
         <v>724</v>
       </c>
     </row>
@@ -6452,826 +6470,856 @@
       </c>
     </row>
     <row r="706" spans="1:1">
-      <c r="A706">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A706" t="s">
+        <v>727</v>
       </c>
     </row>
     <row r="707" spans="1:1">
-      <c r="A707">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A707" t="s">
+        <v>728</v>
       </c>
     </row>
     <row r="708" spans="1:1">
-      <c r="A708">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B10), "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="710" spans="1:1">
-      <c r="A710" t="s">
-        <v>727</v>
+      <c r="A708" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="709" spans="1:1">
+      <c r="A709" t="s">
+        <v>730</v>
       </c>
     </row>
     <row r="711" spans="1:1">
-      <c r="A711">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A711" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="712" spans="1:1">
-      <c r="A712">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A712" t="s">
+        <v>732</v>
       </c>
     </row>
     <row r="713" spans="1:1">
       <c r="A713">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="714" spans="1:1">
       <c r="A714">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="716" spans="1:1">
-      <c r="A716" t="s">
-        <v>728</v>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="715" spans="1:1">
+      <c r="A715">
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B10), "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="717" spans="1:1">
-      <c r="A717">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A717" t="s">
+        <v>733</v>
       </c>
     </row>
     <row r="718" spans="1:1">
       <c r="A718">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B12), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="719" spans="1:1">
       <c r="A719">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B13), "{{ STACK }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="720" spans="1:1">
       <c r="A720">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B14), "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="722" spans="1:1">
-      <c r="A722">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="721" spans="1:1">
+      <c r="A721">
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="723" spans="1:1">
-      <c r="A723">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A723" t="s">
+        <v>734</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B12), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B13), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="728" spans="1:1">
-      <c r="A728">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B14), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="766" spans="1:1">
       <c r="A766">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="767" spans="1:1">
       <c r="A767">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="768" spans="1:1">
       <c r="A768">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="769" spans="1:1">
       <c r="A769">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="770" spans="1:1">
       <c r="A770">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="771" spans="1:1">
       <c r="A771">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="772" spans="1:1">
       <c r="A772">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="773" spans="1:1">
       <c r="A773">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="774" spans="1:1">
       <c r="A774">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="775" spans="1:1">
       <c r="A775">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="776" spans="1:1">
       <c r="A776">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="777" spans="1:1">
       <c r="A777">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="778" spans="1:1">
       <c r="A778">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="779" spans="1:1">
       <c r="A779">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="780" spans="1:1">
       <c r="A780">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="781" spans="1:1">
       <c r="A781">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="782" spans="1:1">
       <c r="A782">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="783" spans="1:1">
       <c r="A783">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="784" spans="1:1">
       <c r="A784">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="785" spans="1:1">
       <c r="A785">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="786" spans="1:1">
       <c r="A786">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="787" spans="1:1">
       <c r="A787">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="788" spans="1:1">
       <c r="A788">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="789" spans="1:1">
       <c r="A789">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="790" spans="1:1">
       <c r="A790">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="791" spans="1:1">
       <c r="A791">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="792" spans="1:1">
       <c r="A792">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="793" spans="1:1">
       <c r="A793">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="794" spans="1:1">
       <c r="A794">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="795" spans="1:1">
       <c r="A795">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="796" spans="1:1">
       <c r="A796">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="797" spans="1:1">
       <c r="A797">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="798" spans="1:1">
       <c r="A798">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="799" spans="1:1">
       <c r="A799">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="800" spans="1:1">
       <c r="A800">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="801" spans="1:1">
       <c r="A801">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="802" spans="1:1">
       <c r="A802">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="803" spans="1:1">
       <c r="A803">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="804" spans="1:1">
+      <c r="A804">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="805" spans="1:1">
+      <c r="A805">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="806" spans="1:1">
+      <c r="A806">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="807" spans="1:1">
+      <c r="A807">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="808" spans="1:1">
+      <c r="A808">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="809" spans="1:1">
+      <c r="A809">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="810" spans="1:1">
+      <c r="A810">
         <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" email-profile Sample_Email_Profile", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="805" spans="1:1">
-      <c r="A805" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="806" spans="1:1">
-      <c r="A806" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="807" spans="1:1">
-      <c r="A807" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="808" spans="1:1">
-      <c r="A808" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="809" spans="1:1">
-      <c r="A809" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="810" spans="1:1">
-      <c r="A810" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="811" spans="1:1">
-      <c r="A811" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="812" spans="1:1">
       <c r="A812" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="813" spans="1:1">
       <c r="A813" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="814" spans="1:1">
       <c r="A814" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="815" spans="1:1">
       <c r="A815" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="816" spans="1:1">
       <c r="A816" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="817" spans="1:1">
       <c r="A817" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="818" spans="1:1">
       <c r="A818" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="819" spans="1:1">
       <c r="A819" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="820" spans="1:1">
       <c r="A820" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="821" spans="1:1">
       <c r="A821" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="822" spans="1:1">
       <c r="A822" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="823" spans="1:1">
       <c r="A823" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="824" spans="1:1">
       <c r="A824" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="825" spans="1:1">
       <c r="A825" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="826" spans="1:1">
       <c r="A826" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="827" spans="1:1">
       <c r="A827" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="828" spans="1:1">
       <c r="A828" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="829" spans="1:1">
       <c r="A829" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="830" spans="1:1">
       <c r="A830" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="831" spans="1:1">
       <c r="A831" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="832" spans="1:1">
       <c r="A832" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="833" spans="1:1">
       <c r="A833" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="834" spans="1:1">
       <c r="A834" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="835" spans="1:1">
       <c r="A835" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="836" spans="1:1">
       <c r="A836" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="837" spans="1:1">
       <c r="A837" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="838" spans="1:1">
       <c r="A838" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="839" spans="1:1">
       <c r="A839" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="840" spans="1:1">
       <c r="A840" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="841" spans="1:1">
       <c r="A841" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="842" spans="1:1">
       <c r="A842" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="843" spans="1:1">
       <c r="A843" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="844" spans="1:1">
       <c r="A844" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="845" spans="1:1">
       <c r="A845" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="846" spans="1:1">
       <c r="A846" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="847" spans="1:1">
       <c r="A847" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="848" spans="1:1">
       <c r="A848" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="849" spans="1:1">
       <c r="A849" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="850" spans="1:1">
       <c r="A850" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="851" spans="1:1">
       <c r="A851" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="852" spans="1:1">
       <c r="A852" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="853" spans="1:1">
       <c r="A853" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="854" spans="1:1">
       <c r="A854" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="855" spans="1:1">
       <c r="A855" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="856" spans="1:1">
+      <c r="A856" t="s">
         <v>779</v>
+      </c>
+    </row>
+    <row r="857" spans="1:1">
+      <c r="A857" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="858" spans="1:1">
+      <c r="A858" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="859" spans="1:1">
+      <c r="A859" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="860" spans="1:1">
+      <c r="A860" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="861" spans="1:1">
+      <c r="A861" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="862" spans="1:1">
+      <c r="A862" t="s">
+        <v>785</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deleted tooling directory and replaced with sli bash script
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="785">
   <si>
     <t>Variable Name</t>
   </si>
@@ -23,9 +23,6 @@
     <t>Variable Value</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>PANORAMA_NAME</t>
   </si>
   <si>
@@ -260,13 +257,13 @@
     <t># in operations mode you can elect to enable scripting mode for rapid paste into the ClI</t>
   </si>
   <si>
-    <t>set cli scripting-mode on</t>
+    <t>#set cli scripting-mode on</t>
   </si>
   <si>
     <t># if not in configuration mode</t>
   </si>
   <si>
-    <t>configure</t>
+    <t>#configure</t>
   </si>
   <si>
     <t># management interface configuration - may be skipped if already online</t>
@@ -2730,283 +2727,280 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
         <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
         <v>41</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
         <v>44</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>45</v>
-      </c>
-      <c r="C16" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>48</v>
-      </c>
-      <c r="C17" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
         <v>50</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>51</v>
-      </c>
-      <c r="C18" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
         <v>53</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>54</v>
-      </c>
-      <c r="C19" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
         <v>56</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>57</v>
-      </c>
-      <c r="C20" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
         <v>59</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>60</v>
-      </c>
-      <c r="C21" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
         <v>62</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>63</v>
-      </c>
-      <c r="C22" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
         <v>65</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>66</v>
-      </c>
-      <c r="C23" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
         <v>68</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>69</v>
-      </c>
-      <c r="C24" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" t="s">
         <v>71</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>72</v>
-      </c>
-      <c r="C25" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26">
         <v>525600</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3024,47 +3018,47 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:1">
@@ -3117,7 +3111,7 @@
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:1">
@@ -3134,132 +3128,132 @@
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:1">
@@ -3270,42 +3264,42 @@
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:1">
@@ -3316,37 +3310,37 @@
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="72" spans="1:1">
@@ -3369,32 +3363,32 @@
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="81" spans="1:1">
@@ -3405,907 +3399,907 @@
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="252" spans="1:1">
       <c r="A252" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="268" spans="1:1">
@@ -4322,137 +4316,137 @@
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="297" spans="1:1">
@@ -4469,137 +4463,137 @@
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="326" spans="1:1">
@@ -4616,137 +4610,137 @@
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="355" spans="1:1">
@@ -4763,112 +4757,112 @@
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="379" spans="1:1">
@@ -4885,1117 +4879,1117 @@
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="391" spans="1:1">
       <c r="A391" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="421" spans="1:1">
       <c r="A421" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="529" spans="1:1">
       <c r="A529" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="548" spans="1:1">
       <c r="A548" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="549" spans="1:1">
       <c r="A549" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="550" spans="1:1">
       <c r="A550" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="551" spans="1:1">
       <c r="A551" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="612" spans="1:1">
@@ -6012,102 +6006,102 @@
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="615" spans="1:1">
       <c r="A615" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="617" spans="1:1">
       <c r="A617" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="618" spans="1:1">
       <c r="A618" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="619" spans="1:1">
       <c r="A619" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="620" spans="1:1">
       <c r="A620" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="621" spans="1:1">
       <c r="A621" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="622" spans="1:1">
       <c r="A622" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="623" spans="1:1">
       <c r="A623" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="624" spans="1:1">
       <c r="A624" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="625" spans="1:1">
       <c r="A625" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="627" spans="1:1">
       <c r="A627" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="628" spans="1:1">
       <c r="A628" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="629" spans="1:1">
       <c r="A629" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="630" spans="1:1">
       <c r="A630" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="631" spans="1:1">
       <c r="A631" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="632" spans="1:1">
       <c r="A632" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="633" spans="1:1">
       <c r="A633" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="634" spans="1:1">
@@ -6136,367 +6130,367 @@
     </row>
     <row r="638" spans="1:1">
       <c r="A638" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="641" spans="1:1">
       <c r="A641" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="642" spans="1:1">
       <c r="A642" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="643" spans="1:1">
       <c r="A643" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="647" spans="1:1">
       <c r="A647" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="648" spans="1:1">
       <c r="A648" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="649" spans="1:1">
       <c r="A649" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="654" spans="1:1">
       <c r="A654" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="659" spans="1:1">
       <c r="A659" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="664" spans="1:1">
       <c r="A664" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="665" spans="1:1">
       <c r="A665" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="670" spans="1:1">
       <c r="A670" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="672" spans="1:1">
       <c r="A672" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="673" spans="1:1">
       <c r="A673" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="675" spans="1:1">
       <c r="A675" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="676" spans="1:1">
       <c r="A676" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="677" spans="1:1">
       <c r="A677" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="678" spans="1:1">
       <c r="A678" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="679" spans="1:1">
       <c r="A679" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="680" spans="1:1">
       <c r="A680" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="681" spans="1:1">
       <c r="A681" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="682" spans="1:1">
       <c r="A682" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="683" spans="1:1">
       <c r="A683" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="684" spans="1:1">
       <c r="A684" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="686" spans="1:1">
       <c r="A686" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="687" spans="1:1">
       <c r="A687" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="688" spans="1:1">
       <c r="A688" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="689" spans="1:1">
       <c r="A689" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="690" spans="1:1">
       <c r="A690" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="691" spans="1:1">
       <c r="A691" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="692" spans="1:1">
       <c r="A692" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="693" spans="1:1">
       <c r="A693" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="694" spans="1:1">
       <c r="A694" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="695" spans="1:1">
       <c r="A695" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="696" spans="1:1">
       <c r="A696" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="697" spans="1:1">
       <c r="A697" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="698" spans="1:1">
       <c r="A698" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="699" spans="1:1">
       <c r="A699" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="700" spans="1:1">
       <c r="A700" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="701" spans="1:1">
       <c r="A701" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="702" spans="1:1">
       <c r="A702" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="703" spans="1:1">
       <c r="A703" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="704" spans="1:1">
       <c r="A704" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="705" spans="1:1">
       <c r="A705" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="706" spans="1:1">
       <c r="A706" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="707" spans="1:1">
       <c r="A707" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="708" spans="1:1">
       <c r="A708" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="709" spans="1:1">
       <c r="A709" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="711" spans="1:1">
       <c r="A711" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="712" spans="1:1">
       <c r="A712" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="713" spans="1:1">
@@ -6519,7 +6513,7 @@
     </row>
     <row r="717" spans="1:1">
       <c r="A717" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="718" spans="1:1">
@@ -6548,7 +6542,7 @@
     </row>
     <row r="723" spans="1:1">
       <c r="A723" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="724" spans="1:1">
@@ -7069,257 +7063,257 @@
     </row>
     <row r="812" spans="1:1">
       <c r="A812" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="813" spans="1:1">
       <c r="A813" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="814" spans="1:1">
       <c r="A814" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="815" spans="1:1">
       <c r="A815" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="816" spans="1:1">
       <c r="A816" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="817" spans="1:1">
       <c r="A817" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="818" spans="1:1">
       <c r="A818" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="819" spans="1:1">
       <c r="A819" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="820" spans="1:1">
       <c r="A820" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="821" spans="1:1">
       <c r="A821" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="822" spans="1:1">
       <c r="A822" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="823" spans="1:1">
       <c r="A823" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="824" spans="1:1">
       <c r="A824" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="825" spans="1:1">
       <c r="A825" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="826" spans="1:1">
       <c r="A826" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="827" spans="1:1">
       <c r="A827" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="828" spans="1:1">
       <c r="A828" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="829" spans="1:1">
       <c r="A829" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="830" spans="1:1">
       <c r="A830" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="831" spans="1:1">
       <c r="A831" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="832" spans="1:1">
       <c r="A832" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="833" spans="1:1">
       <c r="A833" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="834" spans="1:1">
       <c r="A834" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="835" spans="1:1">
       <c r="A835" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="836" spans="1:1">
       <c r="A836" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="837" spans="1:1">
       <c r="A837" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="838" spans="1:1">
       <c r="A838" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="839" spans="1:1">
       <c r="A839" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="840" spans="1:1">
       <c r="A840" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="841" spans="1:1">
       <c r="A841" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="842" spans="1:1">
       <c r="A842" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="843" spans="1:1">
       <c r="A843" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="844" spans="1:1">
       <c r="A844" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="845" spans="1:1">
       <c r="A845" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="846" spans="1:1">
       <c r="A846" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="847" spans="1:1">
       <c r="A847" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="848" spans="1:1">
       <c r="A848" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="849" spans="1:1">
       <c r="A849" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="850" spans="1:1">
       <c r="A850" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="851" spans="1:1">
       <c r="A851" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="852" spans="1:1">
       <c r="A852" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="853" spans="1:1">
       <c r="A853" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="854" spans="1:1">
       <c r="A854" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="855" spans="1:1">
       <c r="A855" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="856" spans="1:1">
       <c r="A856" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="857" spans="1:1">
       <c r="A857" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="858" spans="1:1">
       <c r="A858" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="859" spans="1:1">
       <c r="A859" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="860" spans="1:1">
       <c r="A860" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="861" spans="1:1">
       <c r="A861" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="862" spans="1:1">
       <c r="A862" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ransomware and encrypted dns update
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -1688,7 +1688,7 @@
     <t>set shared profiles url-filtering Outbound-URL credential-enforcement log-severity high</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Outbound-URL credential-enforcement block [ Block Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set shared profiles url-filtering Outbound-URL credential-enforcement block [ Block Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions encrypted-dns entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable ransomware real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Outbound-URL log-http-hdr-user-agent yes</t>
@@ -1700,10 +1700,10 @@
     <t>set shared profiles url-filtering Outbound-URL log-http-hdr-xff yes</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Outbound-URL alert [ Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
-  </si>
-  <si>
-    <t>set shared profiles url-filtering Outbound-URL block [ Block command-and-control grayware malware phishing ]</t>
+    <t>set shared profiles url-filtering Outbound-URL alert [ Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions encrypted-dns entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+  </si>
+  <si>
+    <t>set shared profiles url-filtering Outbound-URL block [ Block command-and-control grayware malware phishing ransomware ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Outbound-URL mlav-engine-urlbased-enabled ""Phishing Detection"" mlav-policy-action block</t>
@@ -1724,10 +1724,10 @@
     <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement log-severity medium</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement alert [ Block Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
-  </si>
-  <si>
-    <t>set shared profiles url-filtering Alert-Only-URL alert [ Block Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set shared profiles url-filtering Alert-Only-URL credential-enforcement alert [ Block Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions encrypted-dns entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable ransomware real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+  </si>
+  <si>
+    <t>set shared profiles url-filtering Alert-Only-URL alert [ Block Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions encrypted-dns entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable ransomware real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Alert-Only-URL mlav-engine-urlbased-enabled ""Phishing Detection"" mlav-policy-action alert</t>
@@ -1748,7 +1748,7 @@
     <t>set shared profiles url-filtering Exception-URL credential-enforcement log-severity high</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Exception-URL credential-enforcement block [ Block Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set shared profiles url-filtering Exception-URL credential-enforcement block [ Block Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions encrypted-dns entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable ransomware real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Exception-URL log-http-hdr-user-agent yes</t>
@@ -1760,10 +1760,10 @@
     <t>set shared profiles url-filtering Exception-URL log-http-hdr-xff yes</t>
   </si>
   <si>
-    <t>set shared profiles url-filtering Exception-URL alert [ Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
-  </si>
-  <si>
-    <t>set shared profiles url-filtering Exception-URL block [ Block command-and-control grayware malware phishing ]</t>
+    <t>set shared profiles url-filtering Exception-URL alert [ Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions encrypted-dns entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+  </si>
+  <si>
+    <t>set shared profiles url-filtering Exception-URL block [ Block command-and-control grayware malware phishing ransomware ]</t>
   </si>
   <si>
     <t>set shared profiles url-filtering Exception-URL mlav-engine-urlbased-enabled ""Phishing Detection"" mlav-policy-action block</t>

</xml_diff>

<commit_message>
updated anti spyware profiles with inline ML
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="855">
   <si>
     <t>Variable Name</t>
   </si>
@@ -1022,6 +1022,24 @@
     <t>set shared profiles spyware Outbound-AS rules Default-Low-Info packet-capture disable</t>
   </si>
   <si>
+    <t>set shared profiles spyware Outbound-AS cloud-inline-analysis yes</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Outbound-AS mica-engine-spyware-enabled ""HTTP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Outbound-AS mica-engine-spyware-enabled ""HTTP2 Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Outbound-AS mica-engine-spyware-enabled ""SSL Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Outbound-AS mica-engine-spyware-enabled ""Unknown-TCP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Outbound-AS mica-engine-spyware-enabled ""Unknown-UDP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
     <t>set shared profiles spyware Inbound-AS botnet-domains lists default-paloalto-dns packet-capture single-packet</t>
   </si>
   <si>
@@ -1139,6 +1157,24 @@
     <t>set shared profiles spyware Inbound-AS rules Default-Low-Info packet-capture disable</t>
   </si>
   <si>
+    <t>set shared profiles spyware Inbound-AS cloud-inline-analysis yes</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Inbound-AS mica-engine-spyware-enabled ""HTTP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Inbound-AS mica-engine-spyware-enabled ""HTTP2 Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Inbound-AS mica-engine-spyware-enabled ""SSL Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Inbound-AS mica-engine-spyware-enabled ""Unknown-TCP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Inbound-AS mica-engine-spyware-enabled ""Unknown-UDP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
     <t>set shared profiles spyware Internal-AS botnet-domains lists default-paloalto-dns packet-capture single-packet</t>
   </si>
   <si>
@@ -1256,6 +1292,24 @@
     <t>set shared profiles spyware Internal-AS rules Default-Medium-Low-Info packet-capture disable</t>
   </si>
   <si>
+    <t>set shared profiles spyware Internal-AS cloud-inline-analysis yes</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Internal-AS mica-engine-spyware-enabled ""HTTP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Internal-AS mica-engine-spyware-enabled ""HTTP2 Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Internal-AS mica-engine-spyware-enabled ""SSL Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Internal-AS mica-engine-spyware-enabled ""Unknown-TCP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Internal-AS mica-engine-spyware-enabled ""Unknown-UDP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
     <t>set shared profiles spyware Alert-Only-AS botnet-domains lists default-paloalto-dns packet-capture disable</t>
   </si>
   <si>
@@ -1356,6 +1410,24 @@
   </si>
   <si>
     <t>set shared profiles spyware Alert-Only-AS rules Alert-All packet-capture disable</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Alert-Only-AS cloud-inline-analysis yes</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Alert-Only-AS mica-engine-spyware-enabled ""HTTP Command and Control detector"" inline-policy-action alert</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Alert-Only-AS mica-engine-spyware-enabled ""HTTP2 Command and Control detector"" inline-policy-action alert</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Alert-Only-AS mica-engine-spyware-enabled ""SSL Command and Control detector"" inline-policy-action alert</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Alert-Only-AS mica-engine-spyware-enabled ""Unknown-TCP Command and Control detector"" inline-policy-action alert</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Alert-Only-AS mica-engine-spyware-enabled ""Unknown-UDP Command and Control detector"" inline-policy-action alert</t>
   </si>
   <si>
     <t>set shared profiles vulnerability Outbound-VP rules Block-Critical-High-Medium action reset-both</t>
@@ -2854,8 +2926,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="1" max="2" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3148,7 +3219,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A911"/>
+  <dimension ref="A2:A937"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4587,45 +4658,45 @@
       </c>
     </row>
     <row r="298" spans="1:1">
-      <c r="A298">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A298" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="299" spans="1:1">
-      <c r="A299">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A299" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="304" spans="1:1">
-      <c r="A304" t="s">
-        <v>339</v>
+      <c r="A304">
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="305" spans="1:1">
-      <c r="A305" t="s">
-        <v>340</v>
+      <c r="A305">
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="306" spans="1:1">
@@ -4794,75 +4865,75 @@
       </c>
     </row>
     <row r="339" spans="1:1">
-      <c r="A339">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A339" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="340" spans="1:1">
-      <c r="A340">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A340" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="351" spans="1:1">
-      <c r="A351" t="s">
-        <v>384</v>
+      <c r="A351">
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="352" spans="1:1">
-      <c r="A352" t="s">
-        <v>385</v>
+      <c r="A352">
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="353" spans="1:1">
@@ -5001,105 +5072,105 @@
       </c>
     </row>
     <row r="380" spans="1:1">
-      <c r="A380">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A380" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="381" spans="1:1">
-      <c r="A381">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A381" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="391" spans="1:1">
       <c r="A391" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="398" spans="1:1">
-      <c r="A398" t="s">
-        <v>429</v>
+      <c r="A398">
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="399" spans="1:1">
-      <c r="A399" t="s">
-        <v>430</v>
+      <c r="A399">
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="400" spans="1:1">
@@ -5182,2524 +5253,2644 @@
         <v>446</v>
       </c>
     </row>
+    <row r="416" spans="1:1">
+      <c r="A416" t="s">
+        <v>447</v>
+      </c>
+    </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="421" spans="1:1">
       <c r="A421" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="440" spans="1:1">
-      <c r="A440" t="s">
         <v>470</v>
-      </c>
-    </row>
-    <row r="441" spans="1:1">
-      <c r="A441" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="442" spans="1:1">
-      <c r="A442" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>533</v>
+        <v>531</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1">
+      <c r="A504" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="529" spans="1:1">
       <c r="A529" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="530" spans="1:1">
-      <c r="A530" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>572</v>
+        <v>570</v>
+      </c>
+    </row>
+    <row r="544" spans="1:1">
+      <c r="A544" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="548" spans="1:1">
       <c r="A548" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="549" spans="1:1">
       <c r="A549" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="550" spans="1:1">
       <c r="A550" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="551" spans="1:1">
       <c r="A551" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="570" spans="1:1">
-      <c r="A570" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>601</v>
+        <v>599</v>
+      </c>
+    </row>
+    <row r="574" spans="1:1">
+      <c r="A574" t="s">
+        <v>600</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="600" spans="1:1">
-      <c r="A600" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="615" spans="1:1">
       <c r="A615" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="617" spans="1:1">
       <c r="A617" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="618" spans="1:1">
       <c r="A618" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="619" spans="1:1">
       <c r="A619" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="620" spans="1:1">
       <c r="A620" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="621" spans="1:1">
       <c r="A621" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="622" spans="1:1">
       <c r="A622" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="623" spans="1:1">
       <c r="A623" t="s">
-        <v>650</v>
+        <v>648</v>
+      </c>
+    </row>
+    <row r="624" spans="1:1">
+      <c r="A624" t="s">
+        <v>649</v>
       </c>
     </row>
     <row r="625" spans="1:1">
       <c r="A625" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="627" spans="1:1">
       <c r="A627" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="628" spans="1:1">
       <c r="A628" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="629" spans="1:1">
+      <c r="A629" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="629" spans="1:1">
-      <c r="A629">
-        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="630" spans="1:1">
-      <c r="A630">
-        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
-        <v>0</v>
+      <c r="A630" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="631" spans="1:1">
       <c r="A631" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="632" spans="1:1">
       <c r="A632" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="633" spans="1:1">
       <c r="A633" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="634" spans="1:1">
       <c r="A634" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="635" spans="1:1">
       <c r="A635" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="636" spans="1:1">
       <c r="A636" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="637" spans="1:1">
       <c r="A637" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="638" spans="1:1">
       <c r="A638" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="641" spans="1:1">
       <c r="A641" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="642" spans="1:1">
       <c r="A642" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="643" spans="1:1">
       <c r="A643" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="647" spans="1:1">
       <c r="A647" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="648" spans="1:1">
       <c r="A648" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="649" spans="1:1">
       <c r="A649" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="650" spans="1:1">
-      <c r="A650" t="s">
         <v>674</v>
       </c>
     </row>
     <row r="651" spans="1:1">
-      <c r="A651">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B18)</f>
-        <v>0</v>
+      <c r="A651" t="s">
+        <v>675</v>
       </c>
     </row>
     <row r="652" spans="1:1">
-      <c r="A652">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B19)</f>
-        <v>0</v>
+      <c r="A652" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="653" spans="1:1">
-      <c r="A653">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
-        <v>0</v>
+      <c r="A653" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="654" spans="1:1">
-      <c r="A654">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
-        <v>0</v>
+      <c r="A654" t="s">
+        <v>678</v>
       </c>
     </row>
     <row r="655" spans="1:1">
-      <c r="A655" t="s">
-        <v>675</v>
+      <c r="A655">
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="656" spans="1:1">
-      <c r="A656" t="s">
-        <v>676</v>
+      <c r="A656">
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
     </row>
     <row r="659" spans="1:1">
       <c r="A659" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
     <row r="664" spans="1:1">
       <c r="A664" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="665" spans="1:1">
       <c r="A665" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
     </row>
     <row r="670" spans="1:1">
       <c r="A670" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
     </row>
     <row r="672" spans="1:1">
       <c r="A672" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
     <row r="673" spans="1:1">
       <c r="A673" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="675" spans="1:1">
       <c r="A675" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
     </row>
     <row r="676" spans="1:1">
       <c r="A676" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="677" spans="1:1">
-      <c r="A677" t="s">
-        <v>697</v>
+      <c r="A677">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B18)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="678" spans="1:1">
-      <c r="A678" t="s">
-        <v>698</v>
+      <c r="A678">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B19)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="679" spans="1:1">
-      <c r="A679" t="s">
-        <v>699</v>
+      <c r="A679">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="680" spans="1:1">
-      <c r="A680" t="s">
-        <v>700</v>
+      <c r="A680">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="681" spans="1:1">
       <c r="A681" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="682" spans="1:1">
       <c r="A682" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="683" spans="1:1">
       <c r="A683" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="684" spans="1:1">
       <c r="A684" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="685" spans="1:1">
       <c r="A685" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="686" spans="1:1">
       <c r="A686" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="687" spans="1:1">
       <c r="A687" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="688" spans="1:1">
       <c r="A688" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="689" spans="1:1">
       <c r="A689" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="690" spans="1:1">
       <c r="A690" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="691" spans="1:1">
       <c r="A691" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="692" spans="1:1">
       <c r="A692" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="693" spans="1:1">
       <c r="A693" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
     </row>
     <row r="694" spans="1:1">
       <c r="A694" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="695" spans="1:1">
       <c r="A695" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="696" spans="1:1">
       <c r="A696" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="697" spans="1:1">
       <c r="A697" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
     </row>
     <row r="698" spans="1:1">
       <c r="A698" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="699" spans="1:1">
       <c r="A699" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="700" spans="1:1">
       <c r="A700" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="701" spans="1:1">
       <c r="A701" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="702" spans="1:1">
       <c r="A702" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="703" spans="1:1">
       <c r="A703" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="704" spans="1:1">
       <c r="A704" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="705" spans="1:1">
       <c r="A705" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="706" spans="1:1">
       <c r="A706" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="707" spans="1:1">
       <c r="A707" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="708" spans="1:1">
       <c r="A708" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="709" spans="1:1">
       <c r="A709" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
     <row r="710" spans="1:1">
       <c r="A710" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="711" spans="1:1">
       <c r="A711" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="712" spans="1:1">
       <c r="A712" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="713" spans="1:1">
       <c r="A713" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="714" spans="1:1">
       <c r="A714" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="715" spans="1:1">
       <c r="A715" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="716" spans="1:1">
       <c r="A716" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
     </row>
     <row r="717" spans="1:1">
       <c r="A717" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
     </row>
     <row r="718" spans="1:1">
       <c r="A718" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="719" spans="1:1">
       <c r="A719" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="720" spans="1:1">
       <c r="A720" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="721" spans="1:1">
       <c r="A721" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730" t="s">
-        <v>750</v>
+        <v>748</v>
+      </c>
+    </row>
+    <row r="731" spans="1:1">
+      <c r="A731" t="s">
+        <v>749</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="756" spans="1:1">
+      <c r="A756" t="s">
         <v>774</v>
       </c>
     </row>
-    <row r="757" spans="1:1">
-      <c r="A757" t="s">
+    <row r="758" spans="1:1">
+      <c r="A758" t="s">
         <v>775</v>
       </c>
     </row>
-    <row r="758" spans="1:1">
-      <c r="A758">
-        <f>SUBSTITUTE("set template {{ STACK }} config deviceconfig setting session packet-buffer-protection-enable yes", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+    <row r="759" spans="1:1">
+      <c r="A759" t="s">
+        <v>776</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="762" spans="1:1">
-      <c r="A762">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A762" t="s">
+        <v>779</v>
       </c>
     </row>
     <row r="763" spans="1:1">
-      <c r="A763">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A763" t="s">
+        <v>780</v>
       </c>
     </row>
     <row r="764" spans="1:1">
-      <c r="A764">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B10), "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A764" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="765" spans="1:1">
+      <c r="A765" t="s">
+        <v>782</v>
       </c>
     </row>
     <row r="766" spans="1:1">
       <c r="A766" t="s">
-        <v>778</v>
+        <v>783</v>
       </c>
     </row>
     <row r="767" spans="1:1">
-      <c r="A767">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A767" t="s">
+        <v>784</v>
       </c>
     </row>
     <row r="768" spans="1:1">
-      <c r="A768">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A768" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="769" spans="1:1">
-      <c r="A769">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A769" t="s">
+        <v>786</v>
       </c>
     </row>
     <row r="770" spans="1:1">
-      <c r="A770">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A770" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="771" spans="1:1">
+      <c r="A771" t="s">
+        <v>788</v>
       </c>
     </row>
     <row r="772" spans="1:1">
       <c r="A772" t="s">
-        <v>779</v>
+        <v>789</v>
       </c>
     </row>
     <row r="773" spans="1:1">
-      <c r="A773">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A773" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="774" spans="1:1">
-      <c r="A774">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B12), "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A774" t="s">
+        <v>791</v>
       </c>
     </row>
     <row r="775" spans="1:1">
-      <c r="A775">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B13), "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A775" t="s">
+        <v>792</v>
       </c>
     </row>
     <row r="776" spans="1:1">
-      <c r="A776">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B14), "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A776" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="777" spans="1:1">
+      <c r="A777" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="778" spans="1:1">
-      <c r="A778">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A778" t="s">
+        <v>795</v>
       </c>
     </row>
     <row r="779" spans="1:1">
-      <c r="A779">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A779" t="s">
+        <v>796</v>
       </c>
     </row>
     <row r="780" spans="1:1">
-      <c r="A780">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A780" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="781" spans="1:1">
-      <c r="A781">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="782" spans="1:1">
-      <c r="A782">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A781" t="s">
+        <v>798</v>
       </c>
     </row>
     <row r="783" spans="1:1">
-      <c r="A783">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A783" t="s">
+        <v>799</v>
       </c>
     </row>
     <row r="784" spans="1:1">
       <c r="A784">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="785" spans="1:1">
-      <c r="A785">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template {{ STACK }} config deviceconfig setting session packet-buffer-protection-enable yes", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="786" spans="1:1">
-      <c r="A786">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A786" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="787" spans="1:1">
-      <c r="A787">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A787" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="788" spans="1:1">
       <c r="A788">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="789" spans="1:1">
       <c r="A789">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="790" spans="1:1">
       <c r="A790">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="791" spans="1:1">
-      <c r="A791">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B10), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="792" spans="1:1">
-      <c r="A792">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A792" t="s">
+        <v>802</v>
       </c>
     </row>
     <row r="793" spans="1:1">
       <c r="A793">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="794" spans="1:1">
       <c r="A794">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="795" spans="1:1">
       <c r="A795">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="796" spans="1:1">
       <c r="A796">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="797" spans="1:1">
-      <c r="A797">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="798" spans="1:1">
-      <c r="A798">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A798" t="s">
+        <v>803</v>
       </c>
     </row>
     <row r="799" spans="1:1">
       <c r="A799">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="800" spans="1:1">
       <c r="A800">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B12), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="801" spans="1:1">
       <c r="A801">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B13), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="802" spans="1:1">
       <c r="A802">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="803" spans="1:1">
-      <c r="A803">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B14), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="804" spans="1:1">
       <c r="A804">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="805" spans="1:1">
       <c r="A805">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="806" spans="1:1">
       <c r="A806">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="807" spans="1:1">
       <c r="A807">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="808" spans="1:1">
       <c r="A808">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="809" spans="1:1">
       <c r="A809">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="810" spans="1:1">
       <c r="A810">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="811" spans="1:1">
       <c r="A811">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="812" spans="1:1">
       <c r="A812">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="813" spans="1:1">
       <c r="A813">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="814" spans="1:1">
       <c r="A814">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="815" spans="1:1">
       <c r="A815">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="816" spans="1:1">
       <c r="A816">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="817" spans="1:1">
       <c r="A817">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="818" spans="1:1">
       <c r="A818">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="819" spans="1:1">
       <c r="A819">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="820" spans="1:1">
       <c r="A820">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="821" spans="1:1">
       <c r="A821">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="822" spans="1:1">
       <c r="A822">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="823" spans="1:1">
       <c r="A823">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="824" spans="1:1">
       <c r="A824">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="825" spans="1:1">
       <c r="A825">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="826" spans="1:1">
       <c r="A826">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="827" spans="1:1">
       <c r="A827">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="828" spans="1:1">
       <c r="A828">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="829" spans="1:1">
       <c r="A829">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="830" spans="1:1">
       <c r="A830">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="831" spans="1:1">
       <c r="A831">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="832" spans="1:1">
       <c r="A832">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="833" spans="1:1">
       <c r="A833">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="834" spans="1:1">
       <c r="A834">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="835" spans="1:1">
       <c r="A835">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="836" spans="1:1">
       <c r="A836">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="837" spans="1:1">
       <c r="A837">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="838" spans="1:1">
       <c r="A838">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="839" spans="1:1">
       <c r="A839">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="840" spans="1:1">
       <c r="A840">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="841" spans="1:1">
       <c r="A841">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="842" spans="1:1">
       <c r="A842">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="843" spans="1:1">
       <c r="A843">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="844" spans="1:1">
       <c r="A844">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="845" spans="1:1">
       <c r="A845">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="846" spans="1:1">
       <c r="A846">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="847" spans="1:1">
       <c r="A847">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="848" spans="1:1">
       <c r="A848">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="849" spans="1:1">
       <c r="A849">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="850" spans="1:1">
       <c r="A850">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="851" spans="1:1">
       <c r="A851">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="852" spans="1:1">
       <c r="A852">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="853" spans="1:1">
       <c r="A853">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="854" spans="1:1">
       <c r="A854">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="855" spans="1:1">
       <c r="A855">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="856" spans="1:1">
       <c r="A856">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="857" spans="1:1">
       <c r="A857">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="858" spans="1:1">
       <c r="A858">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="859" spans="1:1">
       <c r="A859">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="860" spans="1:1">
+      <c r="A860">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="861" spans="1:1">
+      <c r="A861">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="862" spans="1:1">
+      <c r="A862">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="863" spans="1:1">
+      <c r="A863">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="864" spans="1:1">
+      <c r="A864">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="865" spans="1:1">
+      <c r="A865">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="866" spans="1:1">
+      <c r="A866">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="867" spans="1:1">
+      <c r="A867">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="868" spans="1:1">
+      <c r="A868">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="869" spans="1:1">
+      <c r="A869">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="870" spans="1:1">
+      <c r="A870">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="871" spans="1:1">
+      <c r="A871">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic group-by from", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="872" spans="1:1">
+      <c r="A872">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic aggregate-by [ src srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="873" spans="1:1">
+      <c r="A873">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="874" spans="1:1">
+      <c r="A874">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 1 custom-report ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="875" spans="1:1">
+      <c r="A875">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 2 custom-report ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="876" spans="1:1">
+      <c r="A876">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 3 custom-report ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="877" spans="1:1">
+      <c r="A877">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 4 custom-report ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="878" spans="1:1">
+      <c r="A878">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 5 custom-report ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="879" spans="1:1">
+      <c r="A879">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 6 custom-report ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="880" spans="1:1">
+      <c r="A880">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" custom-widget 7 custom-report ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="881" spans="1:1">
+      <c r="A881">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" title-page yes", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="882" spans="1:1">
+      <c r="A882">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} report-group ""Possible Compromise"" variable title value ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="883" spans="1:1">
+      <c r="A883">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" report-group ""Possible Compromise""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="884" spans="1:1">
+      <c r="A884">
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" recurring disabled", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="885" spans="1:1">
+      <c r="A885">
         <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} email-scheduler ""Possible Compromise"" email-profile Sample_Email_Profile", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="861" spans="1:1">
-      <c r="A861" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="862" spans="1:1">
-      <c r="A862" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="863" spans="1:1">
-      <c r="A863" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="864" spans="1:1">
-      <c r="A864" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="865" spans="1:1">
-      <c r="A865" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="866" spans="1:1">
-      <c r="A866" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="867" spans="1:1">
-      <c r="A867" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="868" spans="1:1">
-      <c r="A868" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="869" spans="1:1">
-      <c r="A869" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="870" spans="1:1">
-      <c r="A870" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="871" spans="1:1">
-      <c r="A871" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="872" spans="1:1">
-      <c r="A872" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="873" spans="1:1">
-      <c r="A873" t="s">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="874" spans="1:1">
-      <c r="A874" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="875" spans="1:1">
-      <c r="A875" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="876" spans="1:1">
-      <c r="A876" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="877" spans="1:1">
-      <c r="A877" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="878" spans="1:1">
-      <c r="A878" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="879" spans="1:1">
-      <c r="A879" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="880" spans="1:1">
-      <c r="A880" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="881" spans="1:1">
-      <c r="A881" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="882" spans="1:1">
-      <c r="A882" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="883" spans="1:1">
-      <c r="A883" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="884" spans="1:1">
-      <c r="A884" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="885" spans="1:1">
-      <c r="A885" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="886" spans="1:1">
-      <c r="A886" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="887" spans="1:1">
       <c r="A887" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="888" spans="1:1">
       <c r="A888" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="889" spans="1:1">
       <c r="A889" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
     </row>
     <row r="890" spans="1:1">
       <c r="A890" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="891" spans="1:1">
       <c r="A891" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="892" spans="1:1">
       <c r="A892" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
     <row r="893" spans="1:1">
       <c r="A893" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
     </row>
     <row r="894" spans="1:1">
       <c r="A894" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
     <row r="895" spans="1:1">
       <c r="A895" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="896" spans="1:1">
       <c r="A896" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
     </row>
     <row r="897" spans="1:1">
       <c r="A897" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
     </row>
     <row r="898" spans="1:1">
       <c r="A898" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
     </row>
     <row r="899" spans="1:1">
       <c r="A899" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
     </row>
     <row r="900" spans="1:1">
       <c r="A900" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
     </row>
     <row r="901" spans="1:1">
       <c r="A901" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="902" spans="1:1">
       <c r="A902" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
     </row>
     <row r="903" spans="1:1">
       <c r="A903" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
     </row>
     <row r="904" spans="1:1">
       <c r="A904" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
     </row>
     <row r="905" spans="1:1">
       <c r="A905" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
     </row>
     <row r="906" spans="1:1">
       <c r="A906" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
     </row>
     <row r="907" spans="1:1">
       <c r="A907" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="908" spans="1:1">
       <c r="A908" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="909" spans="1:1">
       <c r="A909" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
     </row>
     <row r="910" spans="1:1">
       <c r="A910" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
     </row>
     <row r="911" spans="1:1">
       <c r="A911" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="912" spans="1:1">
+      <c r="A912" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="913" spans="1:1">
+      <c r="A913" t="s">
         <v>830</v>
+      </c>
+    </row>
+    <row r="914" spans="1:1">
+      <c r="A914" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="915" spans="1:1">
+      <c r="A915" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="916" spans="1:1">
+      <c r="A916" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="917" spans="1:1">
+      <c r="A917" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="918" spans="1:1">
+      <c r="A918" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="919" spans="1:1">
+      <c r="A919" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="920" spans="1:1">
+      <c r="A920" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="921" spans="1:1">
+      <c r="A921" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="922" spans="1:1">
+      <c r="A922" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="923" spans="1:1">
+      <c r="A923" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="924" spans="1:1">
+      <c r="A924" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="925" spans="1:1">
+      <c r="A925" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="926" spans="1:1">
+      <c r="A926" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="927" spans="1:1">
+      <c r="A927" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="928" spans="1:1">
+      <c r="A928" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="929" spans="1:1">
+      <c r="A929" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="930" spans="1:1">
+      <c r="A930" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="931" spans="1:1">
+      <c r="A931" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="932" spans="1:1">
+      <c r="A932" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="933" spans="1:1">
+      <c r="A933" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="934" spans="1:1">
+      <c r="A934" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="935" spans="1:1">
+      <c r="A935" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="936" spans="1:1">
+      <c r="A936" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="937" spans="1:1">
+      <c r="A937" t="s">
+        <v>854</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated AS profiles for 11.0
</commit_message>
<xml_diff>
--- a/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
+++ b/templates/panorama/set_commands/iron_skillet_panorama_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="868">
   <si>
     <t>Variable Name</t>
   </si>
@@ -1025,6 +1025,24 @@
     <t>set shared profiles spyware Outbound-AS rules Default-Low-Info packet-capture disable</t>
   </si>
   <si>
+    <t>set shared profiles spyware Outbound-AS cloud-inline-analysis yes</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Outbound-AS mica-engine-spyware-enabled ""HTTP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Outbound-AS mica-engine-spyware-enabled ""HTTP2 Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Outbound-AS mica-engine-spyware-enabled ""SSL Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Outbound-AS mica-engine-spyware-enabled ""Unknown-TCP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Outbound-AS mica-engine-spyware-enabled ""Unknown-UDP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
     <t>set shared profiles spyware Inbound-AS botnet-domains lists default-paloalto-dns packet-capture single-packet</t>
   </si>
   <si>
@@ -1142,6 +1160,24 @@
     <t>set shared profiles spyware Inbound-AS rules Default-Low-Info packet-capture disable</t>
   </si>
   <si>
+    <t>set shared profiles spyware Inbound-AS cloud-inline-analysis yes</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Inbound-AS mica-engine-spyware-enabled ""HTTP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Inbound-AS mica-engine-spyware-enabled ""HTTP2 Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Inbound-AS mica-engine-spyware-enabled ""SSL Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Inbound-AS mica-engine-spyware-enabled ""Unknown-TCP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Inbound-AS mica-engine-spyware-enabled ""Unknown-UDP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
     <t>set shared profiles spyware Internal-AS botnet-domains lists default-paloalto-dns packet-capture single-packet</t>
   </si>
   <si>
@@ -1259,6 +1295,24 @@
     <t>set shared profiles spyware Internal-AS rules Default-Medium-Low-Info packet-capture disable</t>
   </si>
   <si>
+    <t>set shared profiles spyware Internal-AS cloud-inline-analysis yes</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Internal-AS mica-engine-spyware-enabled ""HTTP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Internal-AS mica-engine-spyware-enabled ""HTTP2 Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Internal-AS mica-engine-spyware-enabled ""SSL Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Internal-AS mica-engine-spyware-enabled ""Unknown-TCP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Internal-AS mica-engine-spyware-enabled ""Unknown-UDP Command and Control detector"" inline-policy-action reset-both</t>
+  </si>
+  <si>
     <t>set shared profiles spyware Alert-Only-AS botnet-domains lists default-paloalto-dns packet-capture disable</t>
   </si>
   <si>
@@ -1359,6 +1413,24 @@
   </si>
   <si>
     <t>set shared profiles spyware Alert-Only-AS rules Alert-All packet-capture disable</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Alert-Only-AS cloud-inline-analysis yes</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Alert-Only-AS mica-engine-spyware-enabled ""HTTP Command and Control detector"" inline-policy-action alert</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Alert-Only-AS mica-engine-spyware-enabled ""HTTP2 Command and Control detector"" inline-policy-action alert</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Alert-Only-AS mica-engine-spyware-enabled ""SSL Command and Control detector"" inline-policy-action alert</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Alert-Only-AS mica-engine-spyware-enabled ""Unknown-TCP Command and Control detector"" inline-policy-action alert</t>
+  </si>
+  <si>
+    <t>set shared profiles spyware Alert-Only-AS mica-engine-spyware-enabled ""Unknown-UDP Command and Control detector"" inline-policy-action alert</t>
   </si>
   <si>
     <t>set shared profiles vulnerability Outbound-VP rules Block-Critical-High-Medium action reset-both</t>
@@ -2893,8 +2965,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="1" max="2" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3187,7 +3258,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A924"/>
+  <dimension ref="A2:A948"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4631,45 +4702,45 @@
       </c>
     </row>
     <row r="299" spans="1:1">
-      <c r="A299">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A299" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="300" spans="1:1">
-      <c r="A300">
-        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A300" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="305" spans="1:1">
-      <c r="A305" t="s">
-        <v>340</v>
+      <c r="A305">
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="306" spans="1:1">
-      <c r="A306" t="s">
-        <v>341</v>
+      <c r="A306">
+        <f>SUBSTITUTE("set shared profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="307" spans="1:1">
@@ -4838,75 +4909,75 @@
       </c>
     </row>
     <row r="340" spans="1:1">
-      <c r="A340">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A340" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="341" spans="1:1">
-      <c r="A341">
-        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A341" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="352" spans="1:1">
-      <c r="A352" t="s">
-        <v>385</v>
+      <c r="A352">
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="353" spans="1:1">
-      <c r="A353" t="s">
-        <v>386</v>
+      <c r="A353">
+        <f>SUBSTITUTE("set shared profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="354" spans="1:1">
@@ -5045,105 +5116,105 @@
       </c>
     </row>
     <row r="381" spans="1:1">
-      <c r="A381">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
-        <v>0</v>
+      <c r="A381" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="382" spans="1:1">
-      <c r="A382">
-        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
-        <v>0</v>
+      <c r="A382" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="391" spans="1:1">
       <c r="A391" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="399" spans="1:1">
-      <c r="A399" t="s">
-        <v>430</v>
+      <c r="A399">
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="400" spans="1:1">
-      <c r="A400" t="s">
-        <v>431</v>
+      <c r="A400">
+        <f>SUBSTITUTE("set shared profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="401" spans="1:1">
@@ -5226,123 +5297,123 @@
         <v>447</v>
       </c>
     </row>
+    <row r="417" spans="1:1">
+      <c r="A417" t="s">
+        <v>448</v>
+      </c>
+    </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="421" spans="1:1">
       <c r="A421" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="441" spans="1:1">
-      <c r="A441" t="s">
         <v>471</v>
       </c>
     </row>
@@ -5721,123 +5792,123 @@
         <v>546</v>
       </c>
     </row>
+    <row r="517" spans="1:1">
+      <c r="A517" t="s">
+        <v>547</v>
+      </c>
+    </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="529" spans="1:1">
       <c r="A529" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="541" spans="1:1">
-      <c r="A541" t="s">
         <v>570</v>
       </c>
     </row>
@@ -5916,123 +5987,123 @@
         <v>585</v>
       </c>
     </row>
+    <row r="557" spans="1:1">
+      <c r="A557" t="s">
+        <v>586</v>
+      </c>
+    </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="581" spans="1:1">
-      <c r="A581" t="s">
         <v>609</v>
       </c>
     </row>
@@ -6061,123 +6132,123 @@
         <v>614</v>
       </c>
     </row>
+    <row r="587" spans="1:1">
+      <c r="A587" t="s">
+        <v>615</v>
+      </c>
+    </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="611" spans="1:1">
-      <c r="A611" t="s">
         <v>638</v>
       </c>
     </row>
@@ -6306,280 +6377,280 @@
         <v>663</v>
       </c>
     </row>
+    <row r="637" spans="1:1">
+      <c r="A637" t="s">
+        <v>664</v>
+      </c>
+    </row>
     <row r="638" spans="1:1">
       <c r="A638" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="641" spans="1:1">
       <c r="A641" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="642" spans="1:1">
-      <c r="A642">
-        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
-        <v>0</v>
+      <c r="A642" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="643" spans="1:1">
-      <c r="A643">
-        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
-        <v>0</v>
+      <c r="A643" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
     </row>
     <row r="647" spans="1:1">
       <c r="A647" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
     </row>
     <row r="648" spans="1:1">
       <c r="A648" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
     </row>
     <row r="649" spans="1:1">
       <c r="A649" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
     </row>
     <row r="654" spans="1:1">
       <c r="A654" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
     </row>
     <row r="659" spans="1:1">
       <c r="A659" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="661" spans="1:1">
-      <c r="A661" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
     </row>
     <row r="664" spans="1:1">
-      <c r="A664">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B18)</f>
-        <v>0</v>
+      <c r="A664" t="s">
+        <v>690</v>
       </c>
     </row>
     <row r="665" spans="1:1">
-      <c r="A665">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B19)</f>
-        <v>0</v>
+      <c r="A665" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} phash $1$GmGy8oJJ$V75cNdSRDx0V78yJqXZ111", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667">
-        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
+        <f>SUBSTITUTE("set template iron-skillet config mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
     </row>
     <row r="670" spans="1:1">
       <c r="A670" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671" t="s">
-        <v>691</v>
+        <v>695</v>
       </c>
     </row>
     <row r="672" spans="1:1">
       <c r="A672" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
     </row>
     <row r="673" spans="1:1">
       <c r="A673" t="s">
-        <v>693</v>
+        <v>697</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674" t="s">
-        <v>694</v>
+        <v>698</v>
       </c>
     </row>
     <row r="675" spans="1:1">
       <c r="A675" t="s">
-        <v>695</v>
+        <v>699</v>
       </c>
     </row>
     <row r="676" spans="1:1">
       <c r="A676" t="s">
-        <v>696</v>
+        <v>700</v>
       </c>
     </row>
     <row r="677" spans="1:1">
       <c r="A677" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
     </row>
     <row r="678" spans="1:1">
       <c r="A678" t="s">
-        <v>698</v>
+        <v>702</v>
       </c>
     </row>
     <row r="679" spans="1:1">
       <c r="A679" t="s">
-        <v>699</v>
+        <v>703</v>
       </c>
     </row>
     <row r="680" spans="1:1">
       <c r="A680" t="s">
-        <v>700</v>
+        <v>704</v>
       </c>
     </row>
     <row r="681" spans="1:1">
       <c r="A681" t="s">
-        <v>701</v>
+        <v>705</v>
       </c>
     </row>
     <row r="682" spans="1:1">
       <c r="A682" t="s">
-        <v>702</v>
+        <v>706</v>
       </c>
     </row>
     <row r="683" spans="1:1">
       <c r="A683" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
     </row>
     <row r="684" spans="1:1">
       <c r="A684" t="s">
-        <v>704</v>
+        <v>708</v>
       </c>
     </row>
     <row r="685" spans="1:1">
       <c r="A685" t="s">
-        <v>705</v>
+        <v>709</v>
       </c>
     </row>
     <row r="686" spans="1:1">
       <c r="A686" t="s">
-        <v>706</v>
+        <v>710</v>
       </c>
     </row>
     <row r="687" spans="1:1">
       <c r="A687" t="s">
-        <v>707</v>
+        <v>711</v>
       </c>
     </row>
     <row r="688" spans="1:1">
-      <c r="A688" t="s">
-        <v>708</v>
+      <c r="A688">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B18)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="689" spans="1:1">
-      <c r="A689" t="s">
-        <v>709</v>
+      <c r="A689">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B19)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="690" spans="1:1">
-      <c r="A690" t="s">
-        <v>710</v>
+      <c r="A690">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="691" spans="1:1">
-      <c r="A691" t="s">
-        <v>711</v>
+      <c r="A691">
+        <f>SUBSTITUTE("set template iron-skillet config deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="692" spans="1:1">
@@ -6842,833 +6913,833 @@
         <v>763</v>
       </c>
     </row>
+    <row r="744" spans="1:1">
+      <c r="A744" t="s">
+        <v>764</v>
+      </c>
+    </row>
     <row r="745" spans="1:1">
       <c r="A745" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
     </row>
     <row r="766" spans="1:1">
       <c r="A766" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="767" spans="1:1">
       <c r="A767" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="768" spans="1:1">
-      <c r="A768" t="s">
         <v>787</v>
+      </c>
+    </row>
+    <row r="769" spans="1:1">
+      <c r="A769" t="s">
+        <v>788</v>
       </c>
     </row>
     <row r="770" spans="1:1">
       <c r="A770" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
     </row>
     <row r="771" spans="1:1">
-      <c r="A771">
-        <f>SUBSTITUTE("set template {{ STACK }} config deviceconfig setting session packet-buffer-protection-enable yes", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A771" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="772" spans="1:1">
+      <c r="A772" t="s">
+        <v>791</v>
       </c>
     </row>
     <row r="773" spans="1:1">
       <c r="A773" t="s">
-        <v>789</v>
+        <v>792</v>
       </c>
     </row>
     <row r="774" spans="1:1">
       <c r="A774" t="s">
-        <v>790</v>
+        <v>793</v>
       </c>
     </row>
     <row r="775" spans="1:1">
-      <c r="A775">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A775" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="776" spans="1:1">
-      <c r="A776">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A776" t="s">
+        <v>795</v>
       </c>
     </row>
     <row r="777" spans="1:1">
-      <c r="A777">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B10), "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A777" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="778" spans="1:1">
+      <c r="A778" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="779" spans="1:1">
       <c r="A779" t="s">
-        <v>791</v>
+        <v>798</v>
       </c>
     </row>
     <row r="780" spans="1:1">
-      <c r="A780">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A780" t="s">
+        <v>799</v>
       </c>
     </row>
     <row r="781" spans="1:1">
-      <c r="A781">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A781" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="782" spans="1:1">
-      <c r="A782">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A782" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="783" spans="1:1">
-      <c r="A783">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A783" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="784" spans="1:1">
+      <c r="A784" t="s">
+        <v>803</v>
       </c>
     </row>
     <row r="785" spans="1:1">
       <c r="A785" t="s">
-        <v>792</v>
+        <v>804</v>
       </c>
     </row>
     <row r="786" spans="1:1">
-      <c r="A786">
-        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A786" t="s">
+        <v>805</v>
       </c>
     </row>
     <row r="787" spans="1:1">
-      <c r="A787">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B12), "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A787" t="s">
+        <v>806</v>
       </c>
     </row>
     <row r="788" spans="1:1">
-      <c r="A788">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B13), "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A788" t="s">
+        <v>807</v>
       </c>
     </row>
     <row r="789" spans="1:1">
-      <c r="A789">
-        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B14), "{{ STACK }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A789" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="790" spans="1:1">
+      <c r="A790" t="s">
+        <v>809</v>
       </c>
     </row>
     <row r="791" spans="1:1">
-      <c r="A791">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A791" t="s">
+        <v>810</v>
       </c>
     </row>
     <row r="792" spans="1:1">
-      <c r="A792">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="793" spans="1:1">
-      <c r="A793">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A792" t="s">
+        <v>811</v>
       </c>
     </row>
     <row r="794" spans="1:1">
-      <c r="A794">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A794" t="s">
+        <v>812</v>
       </c>
     </row>
     <row r="795" spans="1:1">
       <c r="A795">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="796" spans="1:1">
-      <c r="A796">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template {{ STACK }} config deviceconfig setting session packet-buffer-protection-enable yes", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="797" spans="1:1">
-      <c r="A797">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A797" t="s">
+        <v>813</v>
       </c>
     </row>
     <row r="798" spans="1:1">
-      <c r="A798">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A798" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="799" spans="1:1">
       <c r="A799">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} templates iron-skillet", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="800" spans="1:1">
       <c r="A800">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} settings default-vsys vsys1", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="801" spans="1:1">
       <c r="A801">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="802" spans="1:1">
-      <c r="A802">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B10), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="803" spans="1:1">
-      <c r="A803">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A803" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="804" spans="1:1">
       <c r="A804">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-hostname yes", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="805" spans="1:1">
       <c r="A805">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client send-client-id no", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="806" spans="1:1">
       <c r="A806">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-hostname no", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="807" spans="1:1">
       <c r="A807">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="808" spans="1:1">
-      <c r="A808">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type dhcp-client accept-dhcp-domain no", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="809" spans="1:1">
-      <c r="A809">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A809" t="s">
+        <v>816</v>
       </c>
     </row>
     <row r="810" spans="1:1">
       <c r="A810">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system type static", "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="811" spans="1:1">
       <c r="A811">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B12), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="812" spans="1:1">
       <c r="A812">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B13), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="813" spans="1:1">
       <c r="A813">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="814" spans="1:1">
-      <c r="A814">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE(SUBSTITUTE("set template-stack {{ STACK }} config devices localhost.localdomain deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B14), "{{ STACK }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="815" spans="1:1">
       <c r="A815">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="816" spans="1:1">
       <c r="A816">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="817" spans="1:1">
       <c r="A817">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="818" spans="1:1">
       <c r="A818">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" caption ""Host-visit malicious sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="819" spans="1:1">
       <c r="A819">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="820" spans="1:1">
       <c r="A820">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="821" spans="1:1">
       <c r="A821">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="822" spans="1:1">
       <c r="A822">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="823" spans="1:1">
       <c r="A823">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="824" spans="1:1">
       <c r="A824">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit malicious sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="825" spans="1:1">
       <c r="A825">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="826" spans="1:1">
       <c r="A826">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="827" spans="1:1">
       <c r="A827">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="828" spans="1:1">
       <c r="A828">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" caption ""Hosts visit malicious sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="829" spans="1:1">
       <c r="A829">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="830" spans="1:1">
       <c r="A830">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" query ""(category eq command-and-control) or (category eq hacking) or (category eq malware) or (category eq phishing) or (category eq grayware)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="831" spans="1:1">
       <c r="A831">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="832" spans="1:1">
       <c r="A832">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="833" spans="1:1">
       <c r="A833">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="834" spans="1:1">
       <c r="A834">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit malicious sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="835" spans="1:1">
       <c r="A835">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" caption ""Wildfire malicious verdicts""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="836" spans="1:1">
       <c r="A836">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="837" spans="1:1">
       <c r="A837">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" query ""(app neq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="838" spans="1:1">
       <c r="A838">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" description ""Files uploaded or downloaded that were later found to be malicious. This is a summary. Act on real-time email.""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" caption ""Hosts visit questionable sites""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="839" spans="1:1">
       <c r="A839">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="840" spans="1:1">
       <c r="A840">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="841" spans="1:1">
       <c r="A841">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" type panorama-wildfire values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="842" spans="1:1">
       <c r="A842">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="843" spans="1:1">
       <c r="A843">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url aggregate-by [ from srcuser ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="844" spans="1:1">
       <c r="A844">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" topm 10", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Hosts visit questionable sites"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="845" spans="1:1">
       <c r="A845">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" caption ""Wildfire verdicts SMTP""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" period last-7-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="846" spans="1:1">
       <c r="A846">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="847" spans="1:1">
       <c r="A847">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" query ""(app eq smtp) and (category neq benign)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="848" spans="1:1">
       <c r="A848">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" description ""Links sent from emails found to be malicious. """, "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" caption ""Host-visit quest sites plus""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="849" spans="1:1">
       <c r="A849">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="850" spans="1:1">
       <c r="A850">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire verdicts SMTP"" type panorama-wildfire aggregate-by [ filedigest container-of-app app category filetype rule subject sender recipient misc ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" query ""(category eq dynamic-dns) and (category eq parked) and (category eq questionable) and (category eq unknown)""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="851" spans="1:1">
       <c r="A851">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" description ""Detail of hosts visiting questionable URLs""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="852" spans="1:1">
       <c r="A852">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topn 500", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="853" spans="1:1">
       <c r="A853">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" topm 50", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url group-by src", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="854" spans="1:1">
       <c r="A854">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" caption ""Clients sinkholed""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url aggregate-by [ from srcuser category action ]", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="855" spans="1:1">
       <c r="A855">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" query ""(rule eq 'DNS Sinkhole Block')""", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Host-visit quest sites plus"" type panorama-url values repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="856" spans="1:1">
       <c r="A856">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" frequency daily", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfire malicious verdicts"" period last-30-calendar-days", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="857" spans="1:1">
       <c r="A857">
-        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Clients sinkholed"" type panorama-traffic sortby repeatcnt", "{{ DEVICE_GROUP }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set device-group {{ DEVICE_GROUP }} reports ""Wildfi